<commit_message>
Allergy Intolerance latest + resource map
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="560" windowWidth="28800" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="32660" yWindow="-2680" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
+    <sheet name="AllergyIntolerance" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="94">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -234,6 +235,78 @@
   </si>
   <si>
     <t>primarycare-condition-associated-extension</t>
+  </si>
+  <si>
+    <t>PrimaryCare-AllergyIntolerance</t>
+  </si>
+  <si>
+    <t>AllergyIntolerance</t>
+  </si>
+  <si>
+    <t>problem.parentProblem</t>
+  </si>
+  <si>
+    <t>onset</t>
+  </si>
+  <si>
+    <t>recordedDate</t>
+  </si>
+  <si>
+    <t>recorder</t>
+  </si>
+  <si>
+    <t>reporter</t>
+  </si>
+  <si>
+    <t>substance</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>criticality</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>lastOccurence</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>author[x]</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>reaction</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/StructureDefinition/encounter-associatedEncounter</t>
+  </si>
+  <si>
+    <t>AllergyType</t>
+  </si>
+  <si>
+    <t>CausativeAgent</t>
+  </si>
+  <si>
+    <t>OnsetDate</t>
+  </si>
+  <si>
+    <t>LastOccurence</t>
+  </si>
+  <si>
+    <t>RecordedDate</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>A common way of representing allergies in GP care management systems is to record the allergy or adverse reaction as a coded statement e.g. ‘Adverse reaction to penicillins’ (SCTID: 292954005). The actual substance responsible for the adverse reaction is not recorded and a mapping may or may not exist in the source system. Even if a substance mapping does exist, it feels right that the original statement should also be preserved. The AllergyIntolerance resource drives you down the route of recording a substance, which I think is actually a much more solid approach. However, this does result in a disparity when trying to model the GP data.</t>
   </si>
 </sst>
 </file>
@@ -285,7 +358,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -310,6 +383,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -323,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -346,13 +425,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7192"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -624,10 +726,507 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="3"/>
+      <c r="C4" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="3"/>
+      <c r="C6" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="3"/>
+      <c r="C7" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C41" s="1"/>
+      <c r="D41" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D44" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,7 +1236,7 @@
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="37.33203125" customWidth="1"/>
     <col min="5" max="5" width="33.83203125" customWidth="1"/>
-    <col min="6" max="6" width="41.5" customWidth="1"/>
+    <col min="6" max="6" width="52.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.2">
@@ -645,18 +1244,20 @@
         <v>2</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
@@ -666,67 +1267,83 @@
         <v>64</v>
       </c>
       <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
-      <c r="C4" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="3"/>
-      <c r="C6" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="14"/>
+      <c r="C4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="3"/>
-      <c r="C7" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="14"/>
+      <c r="B7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="3"/>
-      <c r="C8" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="14"/>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>28</v>
+      <c r="B10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>8</v>
+      <c r="B11" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
@@ -739,365 +1356,241 @@
       <c r="D12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E12" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>10</v>
+      <c r="B13" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" t="s">
-        <v>42</v>
+      <c r="D14" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="4" t="s">
-        <v>12</v>
+      <c r="B15" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>48</v>
+        <v>37</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="12" t="s">
-        <v>13</v>
+      <c r="B16" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" t="s">
-        <v>44</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="7" t="s">
-        <v>29</v>
+      <c r="B17" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" s="8" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="B21" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="8" t="s">
-        <v>33</v>
+      <c r="B22" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>34</v>
+      <c r="B23" s="14" t="s">
+        <v>78</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="5" t="s">
-        <v>21</v>
+      <c r="B32" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="5" t="s">
-        <v>22</v>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D43" s="1"/>
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
+  <mergeCells count="4">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Procedure latest + resource map
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="32660" yWindow="-2680" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="540" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
     <sheet name="AllergyIntolerance" sheetId="3" r:id="rId2"/>
+    <sheet name="Procedure" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="120">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -307,6 +308,84 @@
   </si>
   <si>
     <t>A common way of representing allergies in GP care management systems is to record the allergy or adverse reaction as a coded statement e.g. ‘Adverse reaction to penicillins’ (SCTID: 292954005). The actual substance responsible for the adverse reaction is not recorded and a mapping may or may not exist in the source system. Even if a substance mapping does exist, it feels right that the original statement should also be preserved. The AllergyIntolerance resource drives you down the route of recording a substance, which I think is actually a much more solid approach. However, this does result in a disparity when trying to model the GP data.</t>
+  </si>
+  <si>
+    <t>PrimaryCare-Procedure</t>
+  </si>
+  <si>
+    <t>Procedure</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>notPerformed</t>
+  </si>
+  <si>
+    <t>reasonNotPerformed</t>
+  </si>
+  <si>
+    <t>reason[x]</t>
+  </si>
+  <si>
+    <t>performer</t>
+  </si>
+  <si>
+    <t>actor</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>performed[x]</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>complication</t>
+  </si>
+  <si>
+    <t>followUp</t>
+  </si>
+  <si>
+    <t>request</t>
+  </si>
+  <si>
+    <t>focalDevice</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>ProcedureCode</t>
+  </si>
+  <si>
+    <t>BodySite</t>
+  </si>
+  <si>
+    <t>Performer</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>event.authorisingUserInRole -&gt; adminDomain.UserInRole</t>
+  </si>
+  <si>
+    <t>event.organisation -&gt; adminDomain.organisation.location</t>
+  </si>
+  <si>
+    <t>primarycare-daterecorded-extension</t>
   </si>
 </sst>
 </file>
@@ -438,12 +517,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -728,7 +807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -1225,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1374,13 +1453,13 @@
       <c r="C14" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="21" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1595,4 +1674,457 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="48.33203125" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" customWidth="1"/>
+    <col min="6" max="6" width="52.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="3"/>
+      <c r="C4" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FamilyMemberHistory latest + resource map
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="540" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
     <sheet name="AllergyIntolerance" sheetId="3" r:id="rId2"/>
     <sheet name="Procedure" sheetId="4" r:id="rId3"/>
+    <sheet name="FamilyMemberHistory" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="137">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -386,13 +387,64 @@
   </si>
   <si>
     <t>primarycare-daterecorded-extension</t>
+  </si>
+  <si>
+    <t>PrimaryCare-FamilyMemberHistory</t>
+  </si>
+  <si>
+    <t>FamilyMemberHistory</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>relationship</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>born[x]</t>
+  </si>
+  <si>
+    <t>age[x]</t>
+  </si>
+  <si>
+    <t>deceased[x]</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>1 .. *</t>
+  </si>
+  <si>
+    <t>event.code.qualifier.value.codeSystem</t>
+  </si>
+  <si>
+    <t>event.code.qualifier.value.code</t>
+  </si>
+  <si>
+    <t>event.code.qualifier.value.displayName</t>
+  </si>
+  <si>
+    <t>event.code.qualifier (name = FH code)</t>
+  </si>
+  <si>
+    <t>primarycare-family-member-history-recorder-extension</t>
+  </si>
+  <si>
+    <t>primarycare-family-member-history-reporter-extension</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -434,6 +486,22 @@
       <sz val="10"/>
       <color theme="9"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -478,10 +546,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -523,8 +593,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -807,7 +892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -1305,7 +1390,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A28" sqref="A28:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1680,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2127,4 +2212,518 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="35.33203125" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="3"/>
+      <c r="C4" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="3"/>
+      <c r="C6" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ReferralRequest latest + resource map
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="31080" yWindow="-2740" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
     <sheet name="AllergyIntolerance" sheetId="3" r:id="rId2"/>
     <sheet name="Procedure" sheetId="4" r:id="rId3"/>
     <sheet name="FamilyMemberHistory" sheetId="5" r:id="rId4"/>
+    <sheet name="ReferralRequest" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="160">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -438,6 +439,75 @@
   </si>
   <si>
     <t>primarycare-family-member-history-reporter-extension</t>
+  </si>
+  <si>
+    <t>PrimaryCare-ReferralRequest</t>
+  </si>
+  <si>
+    <t>ReferralRequest</t>
+  </si>
+  <si>
+    <t>UBRN ✄</t>
+  </si>
+  <si>
+    <t>speciality</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>requester</t>
+  </si>
+  <si>
+    <t>recipient</t>
+  </si>
+  <si>
+    <t>dateSent</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>serviceRequested</t>
+  </si>
+  <si>
+    <t>supportingInformation</t>
+  </si>
+  <si>
+    <t>fulfillmentTime</t>
+  </si>
+  <si>
+    <t>Not Specified</t>
+  </si>
+  <si>
+    <t>event.referral.speciality</t>
+  </si>
+  <si>
+    <t>event.referral.targetUserInRole / event.referral.targetOrganisation</t>
+  </si>
+  <si>
+    <t>event.referral.urgency</t>
+  </si>
+  <si>
+    <t>event.referral.requestType</t>
+  </si>
+  <si>
+    <t>event.referral.reason</t>
+  </si>
+  <si>
+    <t>event.referral.UBRN</t>
+  </si>
+  <si>
+    <t>event.authorisingUserInRole /  event.referral.sourceOrganisation</t>
+  </si>
+  <si>
+    <t>event.referral.datedReferral</t>
+  </si>
+  <si>
+    <t>event.referral.referralActivity</t>
   </si>
 </sst>
 </file>
@@ -551,8 +621,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -605,6 +676,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -893,7 +977,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -907,87 +991,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="3"/>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="3"/>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="3"/>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -995,22 +1079,22 @@
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="2"/>
       <c r="E12" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E13" t="s">
@@ -1021,20 +1105,20 @@
       <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="C14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E15" t="s">
@@ -1042,25 +1126,25 @@
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="C16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E17" t="s">
@@ -1068,120 +1152,120 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="C20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="C21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="1"/>
+      <c r="C26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="2"/>
       <c r="E26" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="5" t="s">
         <v>57</v>
       </c>
       <c r="E27" t="s">
@@ -1189,87 +1273,87 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="C29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="C30" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="1"/>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="1" t="s">
+      <c r="C31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="1"/>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="1" t="s">
+      <c r="C35" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>56</v>
       </c>
       <c r="E35" t="s">
@@ -1277,97 +1361,97 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="C37" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E37" s="1"/>
+      <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="C38" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="1"/>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E40" s="1"/>
+      <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C41" s="1"/>
-      <c r="D41" s="5" t="s">
+      <c r="C41" s="2"/>
+      <c r="D41" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E41" s="1"/>
+      <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D44" s="1"/>
+      <c r="D44" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1390,7 +1474,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD31"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1404,55 +1488,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1460,22 +1544,22 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="2"/>
       <c r="E8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E9" t="s">
@@ -1483,13 +1567,13 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
       <c r="E10" t="s">
@@ -1497,13 +1581,13 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E11" t="s">
@@ -1511,143 +1595,143 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="22" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="C17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="C20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="10" t="s">
         <v>38</v>
       </c>
       <c r="E23" t="s">
@@ -1655,18 +1739,18 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="10" t="s">
         <v>38</v>
       </c>
       <c r="E25" t="s">
@@ -1674,18 +1758,18 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="10" t="s">
         <v>38</v>
       </c>
       <c r="E27" t="s">
@@ -1693,10 +1777,10 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>38</v>
       </c>
       <c r="E28" t="s">
@@ -1704,48 +1788,48 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1766,7 +1850,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1780,55 +1864,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1836,22 +1920,22 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="2"/>
       <c r="E8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>46</v>
       </c>
       <c r="E9" t="s">
@@ -1859,10 +1943,10 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E10" t="s">
@@ -1870,10 +1954,10 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>38</v>
       </c>
       <c r="E11" t="s">
@@ -1881,136 +1965,136 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E12" t="s">
         <v>113</v>
       </c>
-      <c r="F12" s="21"/>
+      <c r="F12" s="22"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="C15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="1"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="C18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="10" t="s">
         <v>37</v>
       </c>
       <c r="E23" t="s">
@@ -2018,21 +2102,21 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="2" t="s">
         <v>49</v>
       </c>
       <c r="E25" t="s">
@@ -2040,51 +2124,51 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="1" t="s">
+      <c r="C26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="1" t="s">
+      <c r="C27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="C28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D30" t="s">
@@ -2095,50 +2179,50 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C36" s="9" t="s">
+      <c r="C36" s="10" t="s">
         <v>37</v>
       </c>
       <c r="E36" t="s">
@@ -2146,59 +2230,59 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C37" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C38" s="9" t="s">
+      <c r="C38" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="9" t="s">
+      <c r="C40" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="C41" s="10" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="C42" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2216,10 +2300,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2228,76 +2312,76 @@
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="35.33203125" customWidth="1"/>
-    <col min="5" max="5" width="33.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28.5" customWidth="1"/>
     <col min="6" max="6" width="41.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="3"/>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2305,417 +2389,429 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="33" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="33"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="C14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>134</v>
       </c>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="1"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="33"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="4" t="s">
+      <c r="C17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="33"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="C18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="33"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="4" t="s">
+      <c r="C19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E19" s="1"/>
+      <c r="E19" s="33"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E20" s="1"/>
+      <c r="E20" s="33"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="C21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="33"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="1"/>
+      <c r="C22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="33"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="1"/>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="33"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="4"/>
+      <c r="C24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="33"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="C25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="33"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="C26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="33"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="C27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="33"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="10" t="s">
         <v>39</v>
       </c>
+      <c r="E28" s="33"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="10" t="s">
         <v>39</v>
       </c>
+      <c r="E29" s="33"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="33"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="E31" s="33"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="33"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="33"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="4" t="s">
+      <c r="C34" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E34" s="33"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
+      <c r="C35" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="33"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="4" t="s">
+      <c r="C36" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="33"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="C37" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E37" s="1"/>
+      <c r="E37" s="33"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="C38" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="33"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C39" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E39" s="1"/>
+      <c r="E39" s="33"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="C40" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="1"/>
+      <c r="E40" s="33"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="C41" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="1"/>
+      <c r="C41" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="5"/>
+      <c r="E41" s="33"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="1"/>
+      <c r="C42" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="5"/>
+      <c r="E42" s="33"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="C43" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" s="33"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="10" t="s">
         <v>39</v>
       </c>
+      <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="10" t="s">
         <v>39</v>
       </c>
+      <c r="E45" s="33"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B46" s="27" t="s">
+      <c r="B46" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="E46" s="33"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="10" t="s">
         <v>36</v>
       </c>
+      <c r="D47" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" s="33"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="C48" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E48" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="E10:E48"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
@@ -2726,4 +2822,372 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="F7" s="29"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="31" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="32"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="32"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="32"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="32"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="32"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="32"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" s="32"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="32"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="32"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="32"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28" s="32"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="32"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" t="s">
+        <v>159</v>
+      </c>
+      <c r="E30" s="32"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E31" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E7:E31"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Observation latest + resource map
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="31080" yWindow="-2740" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-420" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,8 @@
     <sheet name="Procedure" sheetId="4" r:id="rId3"/>
     <sheet name="FamilyMemberHistory" sheetId="5" r:id="rId4"/>
     <sheet name="ReferralRequest" sheetId="6" r:id="rId5"/>
+    <sheet name="Observation" sheetId="8" r:id="rId6"/>
+    <sheet name="MedicationRegime" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="222">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -501,6 +503,9 @@
     <t>event.referral.UBRN</t>
   </si>
   <si>
+    <t>authorisingUserInRole</t>
+  </si>
+  <si>
     <t>event.authorisingUserInRole /  event.referral.sourceOrganisation</t>
   </si>
   <si>
@@ -508,6 +513,189 @@
   </si>
   <si>
     <t>event.referral.referralActivity</t>
+  </si>
+  <si>
+    <t>PrimaryCare-MedicationRegime</t>
+  </si>
+  <si>
+    <t>MedicationStatement</t>
+  </si>
+  <si>
+    <t>informationSource</t>
+  </si>
+  <si>
+    <t>dateAsserted</t>
+  </si>
+  <si>
+    <t>wasNotTaken</t>
+  </si>
+  <si>
+    <t>reasonNotTaken</t>
+  </si>
+  <si>
+    <t>reasonForUse[x]</t>
+  </si>
+  <si>
+    <t>effective[x]</t>
+  </si>
+  <si>
+    <t>medication[x]</t>
+  </si>
+  <si>
+    <t>dosage</t>
+  </si>
+  <si>
+    <t>event.medication.reviewDate</t>
+  </si>
+  <si>
+    <t>event.medication.expiryDate</t>
+  </si>
+  <si>
+    <t>event.medication.dosage</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>event.medication.quantity &amp; event.medication.quantityUnit</t>
+  </si>
+  <si>
+    <t>event.medication.quantityRepresentation</t>
+  </si>
+  <si>
+    <t>event.medication.durationOfIssue</t>
+  </si>
+  <si>
+    <t>event.medication.prescriptionType</t>
+  </si>
+  <si>
+    <t>event.medication.pharmacyText</t>
+  </si>
+  <si>
+    <t>event.medication.patientText</t>
+  </si>
+  <si>
+    <t>event.medication.drugStatus</t>
+  </si>
+  <si>
+    <t>event.medication.private</t>
+  </si>
+  <si>
+    <t>event.medication.minNextIssueDays</t>
+  </si>
+  <si>
+    <t>event.medication.maxNextIssueDays</t>
+  </si>
+  <si>
+    <t>event.medication.firstIssueDate</t>
+  </si>
+  <si>
+    <t>event.medication.mostRecentIssueDate</t>
+  </si>
+  <si>
+    <t>event.medication.numberOfIssues</t>
+  </si>
+  <si>
+    <t>event.medication.authorisedIssues</t>
+  </si>
+  <si>
+    <t>authorisedDate</t>
+  </si>
+  <si>
+    <t>authorisedIssues</t>
+  </si>
+  <si>
+    <t>event.medication.mostRecentIssueMethod</t>
+  </si>
+  <si>
+    <t>event.medication.prescribedAsContraception</t>
+  </si>
+  <si>
+    <t>event.medication.cancellation</t>
+  </si>
+  <si>
+    <t>cancelledByUserInRole</t>
+  </si>
+  <si>
+    <t>cancellationDateTime</t>
+  </si>
+  <si>
+    <t>cancellationText</t>
+  </si>
+  <si>
+    <t>linkedEvent</t>
+  </si>
+  <si>
+    <t>PrimaryCare-Observation</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t>issued</t>
+  </si>
+  <si>
+    <t>value[x]</t>
+  </si>
+  <si>
+    <t>dataAbsentReason</t>
+  </si>
+  <si>
+    <t>interpretation</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>specimen</t>
+  </si>
+  <si>
+    <t>device</t>
+  </si>
+  <si>
+    <t>referenceRange</t>
+  </si>
+  <si>
+    <t>related</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>ObservationCode</t>
+  </si>
+  <si>
+    <t>ObservationDateTime / ObservationPeriod</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>ObservationBodySite</t>
+  </si>
+  <si>
+    <t>ComponentObsCode / Value</t>
+  </si>
+  <si>
+    <t>event.observation.value</t>
+  </si>
+  <si>
+    <t>event.observation.abnormal</t>
+  </si>
+  <si>
+    <t>report.component.specimen</t>
+  </si>
+  <si>
+    <t>event.observation.value.numeric.range</t>
+  </si>
+  <si>
+    <t>event.observation.complexObservation.childLink</t>
+  </si>
+  <si>
+    <t>report.component.battery etc.</t>
   </si>
 </sst>
 </file>
@@ -621,7 +809,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -689,6 +877,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1850,7 +2041,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2110,11 +2301,11 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="34" t="s">
         <v>100</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>49</v>
@@ -2124,11 +2315,11 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="16" t="s">
         <v>101</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>49</v>
@@ -2828,8 +3019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2983,23 +3174,23 @@
       <c r="E14" s="32"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="12" t="s">
         <v>142</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E15" s="32"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="12" t="s">
         <v>143</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>152</v>
@@ -3164,7 +3355,7 @@
         <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E30" s="32"/>
     </row>
@@ -3176,7 +3367,7 @@
         <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E31" s="32"/>
     </row>
@@ -3190,4 +3381,751 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="41.6640625" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>200</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>201</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E24" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>202</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>203</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>206</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>207</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>210</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E34" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F46"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C21" s="10"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="30" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D38" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D39" s="30" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D41" s="31" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="30" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D44" s="30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D45" s="30" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D46" s="30" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="E7:E13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Diagnostic Report + resource map
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-420" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="FamilyMemberHistory" sheetId="5" r:id="rId4"/>
     <sheet name="ReferralRequest" sheetId="6" r:id="rId5"/>
     <sheet name="Observation" sheetId="8" r:id="rId6"/>
-    <sheet name="MedicationRegime" sheetId="7" r:id="rId7"/>
+    <sheet name="DiagnosticReport" sheetId="9" r:id="rId7"/>
+    <sheet name="MedicationRegime" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="249">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -677,6 +678,9 @@
     <t>ObservationBodySite</t>
   </si>
   <si>
+    <t>Specimen</t>
+  </si>
+  <si>
     <t>ComponentObsCode / Value</t>
   </si>
   <si>
@@ -696,6 +700,84 @@
   </si>
   <si>
     <t>report.component.battery etc.</t>
+  </si>
+  <si>
+    <t>PrimaryCare-DiagnosticReport</t>
+  </si>
+  <si>
+    <t>DiagnosticReport</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>imagingStudy</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>conclusion</t>
+  </si>
+  <si>
+    <t>codedDiagnosis</t>
+  </si>
+  <si>
+    <t>presentedForm</t>
+  </si>
+  <si>
+    <t>DiagnosticReportCode</t>
+  </si>
+  <si>
+    <t>DiagnosticReportDate</t>
+  </si>
+  <si>
+    <t>RequestReference</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>event.report.reportLabId, event.report.messageId etc.</t>
+  </si>
+  <si>
+    <t>event.report.abnormal</t>
+  </si>
+  <si>
+    <t>event.report.issueDate</t>
+  </si>
+  <si>
+    <t>event.report.dataType</t>
+  </si>
+  <si>
+    <t>event.report.serviceOrganisation</t>
+  </si>
+  <si>
+    <t>event.report.receivedDate</t>
+  </si>
+  <si>
+    <t>event.associatedText (comment type)</t>
+  </si>
+  <si>
+    <t>event.report.serviceLocation</t>
+  </si>
+  <si>
+    <t>event.report.servicePerson</t>
+  </si>
+  <si>
+    <t>event.report.messageInterchange</t>
+  </si>
+  <si>
+    <t>event.report.orderHeader</t>
+  </si>
+  <si>
+    <t>event.report.component.specimen</t>
+  </si>
+  <si>
+    <t>event.report.reportSummary</t>
+  </si>
+  <si>
+    <t>event.report.component.battery / test</t>
   </si>
 </sst>
 </file>
@@ -3387,7 +3469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -3660,7 +3742,7 @@
         <v>38</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E24" t="s">
         <v>213</v>
@@ -3684,7 +3766,7 @@
         <v>38</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -3725,7 +3807,7 @@
         <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -3744,7 +3826,7 @@
         <v>37</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
@@ -3755,7 +3837,7 @@
         <v>37</v>
       </c>
       <c r="D33" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
@@ -3766,10 +3848,10 @@
         <v>37</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E34" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3784,6 +3866,320 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="45.5" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>238</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>240</v>
+      </c>
+      <c r="E13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
+        <v>245</v>
+      </c>
+      <c r="E16" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>246</v>
+      </c>
+      <c r="E17" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>225</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>248</v>
+      </c>
+      <c r="E18" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="23" t="s">
+        <v>227</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>229</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D25" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>247</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F46"/>
   <sheetViews>

</xml_diff>

<commit_message>
Encounter latest + resource map
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-60" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Observation" sheetId="8" r:id="rId6"/>
     <sheet name="DiagnosticReport" sheetId="9" r:id="rId7"/>
     <sheet name="MedicationRegime" sheetId="7" r:id="rId8"/>
+    <sheet name="Encounter" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="278">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -778,6 +779,93 @@
   </si>
   <si>
     <t>event.report.component.battery / test</t>
+  </si>
+  <si>
+    <t>PrimaryCare-Encounter</t>
+  </si>
+  <si>
+    <t>Encounter</t>
+  </si>
+  <si>
+    <t>statusHIstory</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>episodeOfCare</t>
+  </si>
+  <si>
+    <t>incomingReferral</t>
+  </si>
+  <si>
+    <t>participant</t>
+  </si>
+  <si>
+    <t>appointment</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>indication</t>
+  </si>
+  <si>
+    <t>hospitalization</t>
+  </si>
+  <si>
+    <t>purpose</t>
+  </si>
+  <si>
+    <t>individual</t>
+  </si>
+  <si>
+    <t>serviceProvider</t>
+  </si>
+  <si>
+    <t>partOf</t>
+  </si>
+  <si>
+    <t>primarycare-encounter-purpose-extension</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>encounter.patient</t>
+  </si>
+  <si>
+    <t>encounter.effectiveTime</t>
+  </si>
+  <si>
+    <t>encounter.authorisingUserInRole / accompanyingHCP</t>
+  </si>
+  <si>
+    <t>encounter.organisation</t>
+  </si>
+  <si>
+    <t>encounter.location</t>
+  </si>
+  <si>
+    <t>encounter.loacationType</t>
+  </si>
+  <si>
+    <t>encounter.duration</t>
+  </si>
+  <si>
+    <t>encounter.clinicalPurpose</t>
   </si>
 </sst>
 </file>
@@ -891,7 +979,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -962,6 +1050,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2122,8 +2213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2176,7 +2267,7 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
@@ -2575,8 +2666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2645,7 +2736,7 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
@@ -3102,7 +3193,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3147,7 +3238,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>0</v>
+        <v>137</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -3470,7 +3561,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3515,7 +3606,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>0</v>
+        <v>198</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -3869,8 +3960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3915,7 +4006,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>0</v>
+        <v>223</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -4184,7 +4275,7 @@
   <dimension ref="B1:F46"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4229,7 +4320,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -4524,4 +4615,348 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="E19" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="E21" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="E26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="35"/>
+      <c r="B27" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
EncounterComposition latest + resource map
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="-60" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="DiagnosticReport" sheetId="9" r:id="rId7"/>
     <sheet name="MedicationRegime" sheetId="7" r:id="rId8"/>
     <sheet name="Encounter" sheetId="10" r:id="rId9"/>
+    <sheet name="EncounterComposition" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="299">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -866,6 +867,69 @@
   </si>
   <si>
     <t>encounter.clinicalPurpose</t>
+  </si>
+  <si>
+    <t>PrimaryCare-EncounterComposition</t>
+  </si>
+  <si>
+    <t>Composition</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>confidentiality</t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>attester</t>
+  </si>
+  <si>
+    <t>custodian</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>section</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>orderedBy</t>
+  </si>
+  <si>
+    <t>entry</t>
+  </si>
+  <si>
+    <t>emptyReason</t>
+  </si>
+  <si>
+    <t>Fixed: http://snomed.info/sct</t>
+  </si>
+  <si>
+    <t>Fixed: 25671000000102</t>
+  </si>
+  <si>
+    <t>Fixed: Surgery consultation note (record artifact)</t>
+  </si>
+  <si>
+    <t>encounter.authorisingUserInRole</t>
+  </si>
+  <si>
+    <t>encounter.comonent.problemPage</t>
+  </si>
+  <si>
+    <t>encounter.comonent.heading.displayName</t>
+  </si>
+  <si>
+    <t>encounter.comonent.heading</t>
+  </si>
+  <si>
+    <t>encounter.comonent.event</t>
   </si>
 </sst>
 </file>
@@ -979,7 +1043,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1053,6 +1117,21 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1833,6 +1912,429 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="45.33203125" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="32"/>
+      <c r="F10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="5"/>
+      <c r="E13" s="32"/>
+      <c r="F13" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="32"/>
+      <c r="F14" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="32"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="32"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="32"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="E21" s="32"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="E22" s="32"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="32"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="32"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="32"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="32"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>286</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="32"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>295</v>
+      </c>
+      <c r="E28" s="32"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="32"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="36" t="s">
+        <v>287</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" s="32"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="30" t="s">
+        <v>288</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="32"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="32"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="36" t="s">
+        <v>290</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="32"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="30" t="s">
+        <v>286</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" s="32"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>296</v>
+      </c>
+      <c r="E35" s="32"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" t="s">
+        <v>297</v>
+      </c>
+      <c r="E36" s="32"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="38" t="s">
+        <v>287</v>
+      </c>
+      <c r="C37" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" s="32"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="37" t="s">
+        <v>288</v>
+      </c>
+      <c r="C38" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E38" s="32"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="37" t="s">
+        <v>289</v>
+      </c>
+      <c r="C39" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>298</v>
+      </c>
+      <c r="E39" s="32"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="38" t="s">
+        <v>290</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="E40" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="E7:E40"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
@@ -2667,7 +3169,7 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3193,7 +3695,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E7" sqref="E7:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4274,8 +4776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4333,7 +4835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -4341,7 +4843,9 @@
         <v>37</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="32"/>
+      <c r="E7" s="32" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
@@ -4419,6 +4923,7 @@
       <c r="C14" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="E14" s="32"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
@@ -4427,6 +4932,7 @@
       <c r="C15" s="10" t="s">
         <v>38</v>
       </c>
+      <c r="E15" s="32"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
@@ -4435,16 +4941,18 @@
       <c r="C16" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>148</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
         <v>169</v>
       </c>
@@ -4454,8 +4962,9 @@
       <c r="D18" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="32"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>170</v>
       </c>
@@ -4465,8 +4974,9 @@
       <c r="D19" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="32"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="12" t="s">
         <v>174</v>
       </c>
@@ -4476,131 +4986,152 @@
       <c r="D20" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="32"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C21" s="10"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="40"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="40"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E23" s="40"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E24" s="40"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="40"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E26" s="40"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E27" s="40"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E28" s="40"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E29" s="40"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E30" s="40"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E31" s="40"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="40"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="40"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E34" s="40"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E35" s="40"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E36" s="40"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D37" s="30" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E37" s="40"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D38" s="30" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="40"/>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D39" s="30" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E39" s="40"/>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D40" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E40" s="40"/>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D41" s="31" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D43" s="30" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D44" s="30" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D45" s="30" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D46" s="30" t="s">
         <v>197</v>
       </c>
@@ -4610,7 +5141,7 @@
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="E7:E13"/>
+    <mergeCell ref="E7:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4621,8 +5152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Specimen latest + resource map
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="Observation" sheetId="8" r:id="rId6"/>
     <sheet name="DiagnosticOrder" sheetId="12" r:id="rId7"/>
     <sheet name="DiagnosticReport" sheetId="9" r:id="rId8"/>
-    <sheet name="MedicationRegime" sheetId="7" r:id="rId9"/>
-    <sheet name="Encounter" sheetId="10" r:id="rId10"/>
-    <sheet name="EncounterComposition" sheetId="11" r:id="rId11"/>
+    <sheet name="Specimen" sheetId="13" r:id="rId9"/>
+    <sheet name="MedicationRegime" sheetId="7" r:id="rId10"/>
+    <sheet name="Encounter" sheetId="10" r:id="rId11"/>
+    <sheet name="EncounterComposition" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="331">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -955,6 +956,78 @@
   </si>
   <si>
     <t>DiagnosticOrderCode</t>
+  </si>
+  <si>
+    <t>PrimaryCare-Specimen</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>accessionIdentifier</t>
+  </si>
+  <si>
+    <t>receivedTime</t>
+  </si>
+  <si>
+    <t>collection</t>
+  </si>
+  <si>
+    <t>collector</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>collected[x]</t>
+  </si>
+  <si>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>procedure</t>
+  </si>
+  <si>
+    <t>additive</t>
+  </si>
+  <si>
+    <t>container</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>specimenQuantity</t>
+  </si>
+  <si>
+    <t>additive[x]</t>
+  </si>
+  <si>
+    <t>event.report.component.specimen.labSpecimenReference</t>
+  </si>
+  <si>
+    <t>event.report.component.specimen.specimenType</t>
+  </si>
+  <si>
+    <t>event.report.component.specimen.fastingStatus</t>
+  </si>
+  <si>
+    <t>event.report.component.specimen.volume &amp; volumeUnits</t>
+  </si>
+  <si>
+    <t>event.report.component.specimen.collectionProcedure</t>
+  </si>
+  <si>
+    <t>event.report.component.specimen.anatomicalOrigin</t>
+  </si>
+  <si>
+    <t>event.report.component.specimen.dateTimeReceivedByLab</t>
+  </si>
+  <si>
+    <t>event.report.component.specimen.comment</t>
+  </si>
+  <si>
+    <t>event.report.component.specimen.sampleDateTime - or - collectionStartDate &amp; collectionEndDate</t>
   </si>
 </sst>
 </file>
@@ -1945,6 +2018,382 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F46"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="32"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>173</v>
+      </c>
+      <c r="E19" s="32"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>175</v>
+      </c>
+      <c r="E20" s="32"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C21" s="10"/>
+      <c r="E21" s="40"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="40"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>171</v>
+      </c>
+      <c r="E23" s="40"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>172</v>
+      </c>
+      <c r="E24" s="40"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>176</v>
+      </c>
+      <c r="E25" s="40"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>177</v>
+      </c>
+      <c r="E26" s="40"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>178</v>
+      </c>
+      <c r="E27" s="40"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>179</v>
+      </c>
+      <c r="E28" s="40"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>180</v>
+      </c>
+      <c r="E29" s="40"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>182</v>
+      </c>
+      <c r="E30" s="40"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>183</v>
+      </c>
+      <c r="E31" s="40"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>184</v>
+      </c>
+      <c r="E32" s="40"/>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>185</v>
+      </c>
+      <c r="E33" s="40"/>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>186</v>
+      </c>
+      <c r="E34" s="40"/>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>187</v>
+      </c>
+      <c r="E35" s="40"/>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>188</v>
+      </c>
+      <c r="E36" s="40"/>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D37" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="E37" s="40"/>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D38" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="E38" s="40"/>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D39" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="E39" s="40"/>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>191</v>
+      </c>
+      <c r="E40" s="40"/>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D41" s="31" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D43" s="30" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D44" s="30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D45" s="30" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D46" s="30" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="E7:E20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2287,7 +2736,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F40"/>
   <sheetViews>
@@ -4837,7 +5286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -4846,7 +5295,7 @@
     <col min="1" max="1" width="4.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="30.5" customWidth="1"/>
+    <col min="4" max="4" width="27.5" customWidth="1"/>
     <col min="5" max="5" width="31.1640625" customWidth="1"/>
     <col min="6" max="6" width="41.5" customWidth="1"/>
   </cols>
@@ -5444,10 +5893,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F46"/>
+  <dimension ref="B1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5455,8 +5904,8 @@
     <col min="1" max="1" width="4.6640625" customWidth="1"/>
     <col min="2" max="2" width="28.6640625" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="56" customWidth="1"/>
-    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="4" max="4" width="82" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
     <col min="6" max="6" width="41.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5465,7 +5914,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>161</v>
+        <v>307</v>
       </c>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -5475,7 +5924,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>162</v>
+        <v>215</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
@@ -5484,15 +5933,13 @@
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>64</v>
-      </c>
+      <c r="C3" s="14"/>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>161</v>
+        <v>307</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -5506,7 +5953,7 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -5518,77 +5965,76 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="12" t="s">
-        <v>9</v>
+      <c r="B8" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>46</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="32"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="12" t="s">
-        <v>163</v>
+      <c r="B9" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>49</v>
+        <v>323</v>
       </c>
       <c r="E9" s="32"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>164</v>
+      <c r="B10" s="24" t="s">
+        <v>308</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>47</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D10" s="5"/>
       <c r="E10" s="32"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="12" t="s">
-        <v>78</v>
+      <c r="B11" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
-        <v>181</v>
+      <c r="D11" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="E11" s="32"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>165</v>
+      <c r="B12" s="24" t="s">
+        <v>309</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>47</v>
+      <c r="D12" s="2" t="s">
+        <v>322</v>
       </c>
       <c r="E12" s="32"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>166</v>
+      <c r="B13" s="24" t="s">
+        <v>310</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>328</v>
       </c>
       <c r="E13" s="32"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>167</v>
+      <c r="B14" s="24" t="s">
+        <v>311</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>38</v>
@@ -5596,8 +6042,8 @@
       <c r="E14" s="32"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>168</v>
+      <c r="B15" s="25" t="s">
+        <v>312</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>38</v>
@@ -5605,205 +6051,172 @@
       <c r="E15" s="32"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>82</v>
+      <c r="B16" s="25" t="s">
+        <v>313</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>329</v>
       </c>
       <c r="E16" s="32"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>148</v>
+      <c r="B17" s="25" t="s">
+        <v>314</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>330</v>
       </c>
       <c r="E17" s="32"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="12" t="s">
-        <v>169</v>
+      <c r="B18" s="25" t="s">
+        <v>174</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>50</v>
+        <v>38</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>325</v>
       </c>
       <c r="E18" s="32"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>170</v>
+      <c r="B19" s="25" t="s">
+        <v>205</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" t="s">
-        <v>173</v>
+        <v>38</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>326</v>
       </c>
       <c r="E19" s="32"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="12" t="s">
-        <v>174</v>
+      <c r="B20" s="25" t="s">
+        <v>22</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" t="s">
-        <v>175</v>
+        <v>38</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>327</v>
       </c>
       <c r="E20" s="32"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C21" s="10"/>
-      <c r="E21" s="40"/>
+      <c r="B21" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="32"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="40"/>
+      <c r="B22" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="32"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D23" t="s">
-        <v>171</v>
-      </c>
-      <c r="E23" s="40"/>
+      <c r="B23" s="25" t="s">
+        <v>316</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="32"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D24" t="s">
-        <v>172</v>
-      </c>
-      <c r="E24" s="40"/>
+      <c r="B24" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="32"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D25" t="s">
-        <v>176</v>
-      </c>
-      <c r="E25" s="40"/>
+      <c r="B25" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="32"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D26" t="s">
-        <v>177</v>
-      </c>
-      <c r="E26" s="40"/>
+      <c r="B26" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="32"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D27" t="s">
-        <v>178</v>
-      </c>
-      <c r="E27" s="40"/>
+      <c r="B27" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="32"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D28" t="s">
-        <v>179</v>
-      </c>
-      <c r="E28" s="40"/>
+      <c r="B28" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="32"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D29" t="s">
-        <v>180</v>
-      </c>
-      <c r="E29" s="40"/>
+      <c r="B29" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="32"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D30" t="s">
-        <v>182</v>
-      </c>
-      <c r="E30" s="40"/>
+      <c r="B30" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="32"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D31" t="s">
-        <v>183</v>
-      </c>
-      <c r="E31" s="40"/>
+      <c r="B31" s="25" t="s">
+        <v>321</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="32"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D32" t="s">
-        <v>184</v>
-      </c>
-      <c r="E32" s="40"/>
-    </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D33" t="s">
-        <v>185</v>
-      </c>
-      <c r="E33" s="40"/>
-    </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D34" t="s">
-        <v>186</v>
-      </c>
-      <c r="E34" s="40"/>
-    </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D35" t="s">
-        <v>187</v>
-      </c>
-      <c r="E35" s="40"/>
-    </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D36" t="s">
-        <v>188</v>
-      </c>
-      <c r="E36" s="40"/>
-    </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D37" s="30" t="s">
-        <v>189</v>
-      </c>
-      <c r="E37" s="40"/>
-    </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D38" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="E38" s="40"/>
-    </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D39" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="E39" s="40"/>
-    </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D40" t="s">
-        <v>191</v>
-      </c>
-      <c r="E40" s="40"/>
-    </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D41" s="31" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D42" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D43" s="30" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D44" s="30" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D45" s="30" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D46" s="30" t="s">
-        <v>197</v>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="1"/>
+      <c r="D33" s="2" t="s">
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -5811,7 +6224,7 @@
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="E7:E20"/>
+    <mergeCell ref="E7:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Procedure Request latest + resource map
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Procedure" sheetId="4" r:id="rId3"/>
     <sheet name="FamilyMemberHistory" sheetId="5" r:id="rId4"/>
     <sheet name="ReferralRequest" sheetId="6" r:id="rId5"/>
-    <sheet name="Observation" sheetId="8" r:id="rId6"/>
-    <sheet name="DiagnosticOrder" sheetId="12" r:id="rId7"/>
-    <sheet name="DiagnosticReport" sheetId="9" r:id="rId8"/>
-    <sheet name="Specimen" sheetId="13" r:id="rId9"/>
-    <sheet name="MedicationRegime" sheetId="7" r:id="rId10"/>
-    <sheet name="Encounter" sheetId="10" r:id="rId11"/>
-    <sheet name="EncounterComposition" sheetId="11" r:id="rId12"/>
+    <sheet name="ProcedureRequest" sheetId="14" r:id="rId6"/>
+    <sheet name="Observation" sheetId="8" r:id="rId7"/>
+    <sheet name="DiagnosticOrder" sheetId="12" r:id="rId8"/>
+    <sheet name="DiagnosticReport" sheetId="9" r:id="rId9"/>
+    <sheet name="Specimen" sheetId="13" r:id="rId10"/>
+    <sheet name="MedicationRegime" sheetId="7" r:id="rId11"/>
+    <sheet name="Encounter" sheetId="10" r:id="rId12"/>
+    <sheet name="EncounterComposition" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="337">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -1028,6 +1029,24 @@
   </si>
   <si>
     <t>event.report.component.specimen.sampleDateTime - or - collectionStartDate &amp; collectionEndDate</t>
+  </si>
+  <si>
+    <t>PrimaryCare-ProcedureRequest</t>
+  </si>
+  <si>
+    <t>ProcedureRequest</t>
+  </si>
+  <si>
+    <t>scheduled[x]</t>
+  </si>
+  <si>
+    <t>asNeeded[x]</t>
+  </si>
+  <si>
+    <t>orderedOn</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -2018,9 +2037,349 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="82" customWidth="1"/>
+    <col min="5" max="5" width="28" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="24" t="s">
+        <v>308</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="24" t="s">
+        <v>310</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="25" t="s">
+        <v>313</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="25" t="s">
+        <v>314</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E18" s="32"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="E19" s="32"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E20" s="32"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="32"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="32"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="25" t="s">
+        <v>316</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="32"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="25" t="s">
+        <v>317</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="32"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="32"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="32"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="32"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="32"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="32"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="32"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="25" t="s">
+        <v>321</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="32"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="1"/>
+      <c r="D33" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="E7:E31"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E7" sqref="E7:E20"/>
     </sheetView>
   </sheetViews>
@@ -2392,7 +2751,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
@@ -2736,7 +3095,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F40"/>
   <sheetViews>
@@ -4884,10 +5243,339 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="32"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="32"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="32"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="32"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>336</v>
+      </c>
+      <c r="E22" s="32"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="32"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="32"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="32"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>336</v>
+      </c>
+      <c r="E26" s="32"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>336</v>
+      </c>
+      <c r="E27" s="32"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="32"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="40"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E30" s="40"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E31" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="E7:E28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C3" sqref="C3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5282,7 +5970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F27"/>
   <sheetViews>
@@ -5577,7 +6265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F33"/>
   <sheetViews>
@@ -5889,344 +6577,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F33"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="82" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="41.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="32" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="32"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="E9" s="32"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="24" t="s">
-        <v>308</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="32"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="32"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="24" t="s">
-        <v>309</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="E12" s="32"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="24" t="s">
-        <v>310</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E13" s="32"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="24" t="s">
-        <v>311</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="32"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="25" t="s">
-        <v>312</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="32"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="25" t="s">
-        <v>313</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>329</v>
-      </c>
-      <c r="E16" s="32"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="25" t="s">
-        <v>314</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E17" s="32"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="25" t="s">
-        <v>174</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="E18" s="32"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="25" t="s">
-        <v>205</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="E19" s="32"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="E20" s="32"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="24" t="s">
-        <v>315</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="32"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="32"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="25" t="s">
-        <v>316</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="32"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="25" t="s">
-        <v>317</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="32"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="24" t="s">
-        <v>318</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="32"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="32"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="32"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="32"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="25" t="s">
-        <v>319</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="32"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="25" t="s">
-        <v>320</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E30" s="32"/>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="25" t="s">
-        <v>321</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="32"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="1"/>
-      <c r="D33" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="E7:E31"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Medication Order + resource map
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,9 @@
     <sheet name="DiagnosticReport" sheetId="9" r:id="rId9"/>
     <sheet name="Specimen" sheetId="13" r:id="rId10"/>
     <sheet name="MedicationRegime" sheetId="7" r:id="rId11"/>
-    <sheet name="Encounter" sheetId="10" r:id="rId12"/>
-    <sheet name="EncounterComposition" sheetId="11" r:id="rId13"/>
+    <sheet name="MedicationOrder" sheetId="15" r:id="rId12"/>
+    <sheet name="Encounter" sheetId="10" r:id="rId13"/>
+    <sheet name="EncounterComposition" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="387">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -1047,6 +1048,156 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>PrimaryCare-MedicationOrder</t>
+  </si>
+  <si>
+    <t>MedicationOrder</t>
+  </si>
+  <si>
+    <t>dateWritten</t>
+  </si>
+  <si>
+    <t>dateEnded</t>
+  </si>
+  <si>
+    <t>reasonEnded</t>
+  </si>
+  <si>
+    <t>perscriber</t>
+  </si>
+  <si>
+    <t>dosageInstruction</t>
+  </si>
+  <si>
+    <t>additionalInstructions</t>
+  </si>
+  <si>
+    <t>timing</t>
+  </si>
+  <si>
+    <t>site[x]</t>
+  </si>
+  <si>
+    <t>route</t>
+  </si>
+  <si>
+    <t>dose[x]</t>
+  </si>
+  <si>
+    <t>rate[x]</t>
+  </si>
+  <si>
+    <t>maxDosePerPeriod</t>
+  </si>
+  <si>
+    <t>dispenseRequest</t>
+  </si>
+  <si>
+    <t>validityPeriod</t>
+  </si>
+  <si>
+    <t>numberOfRepeatsAllowed</t>
+  </si>
+  <si>
+    <t>expectedSupplyDuration</t>
+  </si>
+  <si>
+    <t>substitution</t>
+  </si>
+  <si>
+    <t>priorPrescription</t>
+  </si>
+  <si>
+    <t>PrescriptionIdentifier</t>
+  </si>
+  <si>
+    <t>PrescriptionDate</t>
+  </si>
+  <si>
+    <t>PrescriptionAuthor</t>
+  </si>
+  <si>
+    <t>IsRepeat</t>
+  </si>
+  <si>
+    <t>FirstRepeatDate</t>
+  </si>
+  <si>
+    <t>LastIssueDate</t>
+  </si>
+  <si>
+    <t>NumberOfIssues</t>
+  </si>
+  <si>
+    <t>DateEnd</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>QuantityText</t>
+  </si>
+  <si>
+    <t>DosageInstructions</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Medication&gt;&gt;</t>
+  </si>
+  <si>
+    <t>medication</t>
+  </si>
+  <si>
+    <t>quantityUnit</t>
+  </si>
+  <si>
+    <t>quantityRepresentation</t>
+  </si>
+  <si>
+    <t>durationOfIssue</t>
+  </si>
+  <si>
+    <t>prescriptionType</t>
+  </si>
+  <si>
+    <t>estimatedNHSCost</t>
+  </si>
+  <si>
+    <t>pharmacyStamp</t>
+  </si>
+  <si>
+    <t>issueMethod</t>
+  </si>
+  <si>
+    <t>pharmacyText</t>
+  </si>
+  <si>
+    <t>patientText</t>
+  </si>
+  <si>
+    <t>pharmacyMessage</t>
+  </si>
+  <si>
+    <t>patientMessage</t>
+  </si>
+  <si>
+    <t>private</t>
+  </si>
+  <si>
+    <t>cancelled</t>
+  </si>
+  <si>
+    <t>prescribedAsContraceptive</t>
+  </si>
+  <si>
+    <t>repeatDispensingInterval</t>
+  </si>
+  <si>
+    <t>repeatDispensingIssueCount</t>
+  </si>
+  <si>
+    <t>batchNumber</t>
   </si>
 </sst>
 </file>
@@ -1543,7 +1694,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2377,10 +2528,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F46"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E20"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2505,9 +2656,7 @@
       <c r="C12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="D12" s="5"/>
       <c r="E12" s="32"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
@@ -2546,7 +2695,7 @@
       </c>
       <c r="E16" s="32"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>148</v>
       </c>
@@ -2555,7 +2704,7 @@
       </c>
       <c r="E17" s="32"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
         <v>169</v>
       </c>
@@ -2567,7 +2716,7 @@
       </c>
       <c r="E18" s="32"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>170</v>
       </c>
@@ -2579,7 +2728,10 @@
       </c>
       <c r="E19" s="32"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="B20" s="12" t="s">
         <v>174</v>
       </c>
@@ -2591,71 +2743,71 @@
       </c>
       <c r="E20" s="32"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C21" s="10"/>
       <c r="E21" s="40"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
         <v>56</v>
       </c>
       <c r="E22" s="40"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
         <v>171</v>
       </c>
       <c r="E23" s="40"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
         <v>172</v>
       </c>
       <c r="E24" s="40"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
         <v>176</v>
       </c>
       <c r="E25" s="40"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
         <v>177</v>
       </c>
       <c r="E26" s="40"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
         <v>178</v>
       </c>
       <c r="E27" s="40"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
         <v>179</v>
       </c>
       <c r="E28" s="40"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
         <v>180</v>
       </c>
       <c r="E29" s="40"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
         <v>182</v>
       </c>
       <c r="E30" s="40"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
         <v>183</v>
       </c>
       <c r="E31" s="40"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
         <v>184</v>
       </c>
@@ -2752,6 +2904,526 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="40"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="40"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="40"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="40"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="35"/>
+      <c r="B20" s="41" t="s">
+        <v>344</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="40"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="40"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="41" t="s">
+        <v>334</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="40"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="41" t="s">
+        <v>346</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="40"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="41" t="s">
+        <v>347</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="40"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="40"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="41" t="s">
+        <v>348</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="40"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="41" t="s">
+        <v>349</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="40"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="41" t="s">
+        <v>350</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="40"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="40"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="40"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="41" t="s">
+        <v>352</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="40"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="41" t="s">
+        <v>353</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="40"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="40"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="41" t="s">
+        <v>354</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="40"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="40"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="40"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="30"/>
+      <c r="E37" s="40"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="30"/>
+      <c r="E38" s="40"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D39" s="30"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>369</v>
+      </c>
+      <c r="E40" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D41" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="E41" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D42" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="E42" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D43" s="31" t="s">
+        <v>370</v>
+      </c>
+      <c r="E43" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D44" s="31" t="s">
+        <v>371</v>
+      </c>
+      <c r="E44" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D45" s="31" t="s">
+        <v>372</v>
+      </c>
+      <c r="E45" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D46" s="31" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D47" s="31" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D48" s="31" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D49" s="31" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D50" s="31" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D51" s="31" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D52" s="31" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D53" s="31" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D54" s="31" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D55" s="31" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D56" s="31" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D57" s="31" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D58" s="31" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D59" s="31" t="s">
+        <v>386</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
@@ -3095,11 +3767,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -5245,7 +5917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Interpretation and Comments ext added to Diagnostic Report
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" activeTab="1"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="393">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -762,9 +762,6 @@
     <t>event.report.receivedDate</t>
   </si>
   <si>
-    <t>event.associatedText (comment type)</t>
-  </si>
-  <si>
     <t>event.report.serviceLocation</t>
   </si>
   <si>
@@ -1045,9 +1042,6 @@
   </si>
   <si>
     <t>orderedOn</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>PrimaryCare-MedicationOrder</t>
@@ -1804,7 +1798,7 @@
     <row r="9" spans="2:6">
       <c r="B9" s="4"/>
       <c r="C9" s="38" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
@@ -2260,7 +2254,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
@@ -2285,7 +2279,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -2328,13 +2322,13 @@
         <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E9" s="41"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="21" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>37</v>
@@ -2356,31 +2350,31 @@
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="21" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E12" s="41"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="21" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E13" s="41"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="21" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>38</v>
@@ -2389,7 +2383,7 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>38</v>
@@ -2398,25 +2392,25 @@
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E16" s="41"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E17" s="41"/>
     </row>
@@ -2428,7 +2422,7 @@
         <v>38</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E18" s="41"/>
     </row>
@@ -2440,7 +2434,7 @@
         <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E19" s="41"/>
     </row>
@@ -2452,13 +2446,13 @@
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E20" s="41"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="21" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>37</v>
@@ -2476,7 +2470,7 @@
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>38</v>
@@ -2485,7 +2479,7 @@
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="22" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>37</v>
@@ -2494,7 +2488,7 @@
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="21" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>37</v>
@@ -2531,7 +2525,7 @@
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="22" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>38</v>
@@ -2540,7 +2534,7 @@
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>38</v>
@@ -2549,7 +2543,7 @@
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>38</v>
@@ -2562,7 +2556,7 @@
     <row r="33" spans="2:4">
       <c r="B33" s="1"/>
       <c r="D33" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -2581,7 +2575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2958,7 +2952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -2977,7 +2971,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
@@ -2987,7 +2981,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -3004,7 +2998,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -3026,12 +3020,12 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>38</v>
@@ -3040,7 +3034,7 @@
         <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -3057,19 +3051,19 @@
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>38</v>
@@ -3090,7 +3084,7 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="11" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>36</v>
@@ -3099,7 +3093,7 @@
         <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="2:6">
@@ -3145,19 +3139,19 @@
         <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3168,13 +3162,13 @@
         <v>38</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="30"/>
       <c r="B20" s="36" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>38</v>
@@ -3183,7 +3177,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="36" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
@@ -3192,7 +3186,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>38</v>
@@ -3201,7 +3195,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="B23" s="36" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>38</v>
@@ -3210,7 +3204,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="36" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>38</v>
@@ -3228,7 +3222,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="B26" s="36" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>38</v>
@@ -3236,7 +3230,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="B27" s="36" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>38</v>
@@ -3245,7 +3239,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="36" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>38</v>
@@ -3254,7 +3248,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>38</v>
@@ -3272,7 +3266,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="36" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>38</v>
@@ -3281,7 +3275,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="36" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>38</v>
@@ -3296,15 +3290,15 @@
         <v>38</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E33" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="36" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>38</v>
@@ -3313,7 +3307,7 @@
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>38</v>
@@ -3341,7 +3335,7 @@
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>38</v>
@@ -3354,102 +3348,102 @@
     </row>
     <row r="40" spans="2:5">
       <c r="D40" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="E40" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="D41" s="28" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E41" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="D42" s="28" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E42" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="D43" s="28" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E43" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="D44" s="28" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E44" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="D45" s="28" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="D46" s="28" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="47" spans="2:5">
       <c r="D47" s="28" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="D48" s="28" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="49" spans="4:4">
       <c r="D49" s="28" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="50" spans="4:4">
       <c r="D50" s="28" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="51" spans="4:4">
       <c r="D51" s="28" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="52" spans="4:4">
       <c r="D52" s="28" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="53" spans="4:4">
       <c r="D53" s="28" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="54" spans="4:4">
       <c r="D54" s="28" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="55" spans="4:4">
       <c r="D55" s="28" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="56" spans="4:4">
       <c r="D56" s="28" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -3486,7 +3480,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
@@ -3496,7 +3490,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -3506,14 +3500,14 @@
         <v>5</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -3552,7 +3546,7 @@
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>39</v>
@@ -3561,7 +3555,7 @@
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>38</v>
@@ -3576,10 +3570,10 @@
         <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -3599,7 +3593,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E13" t="s">
         <v>41</v>
@@ -3607,7 +3601,7 @@
     </row>
     <row r="14" spans="2:6">
       <c r="B14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>38</v>
@@ -3617,7 +3611,7 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>37</v>
@@ -3626,13 +3620,13 @@
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -3645,12 +3639,12 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>38</v>
@@ -3660,21 +3654,21 @@
     </row>
     <row r="19" spans="1:5">
       <c r="B19" s="22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>38</v>
@@ -3683,27 +3677,27 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E22" s="2"/>
     </row>
@@ -3719,7 +3713,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>37</v>
@@ -3729,7 +3723,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="B25" s="16" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>39</v>
@@ -3745,7 +3739,7 @@
         <v>37</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E26" t="s">
         <v>116</v>
@@ -3754,19 +3748,19 @@
     <row r="27" spans="1:5">
       <c r="A27" s="30"/>
       <c r="B27" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>39</v>
@@ -3779,13 +3773,13 @@
         <v>6</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3830,7 +3824,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
@@ -3840,7 +3834,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -3855,7 +3849,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -3888,7 +3882,7 @@
         <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E8" s="41"/>
     </row>
@@ -3912,7 +3906,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="41"/>
       <c r="F10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="2:6">
@@ -3945,7 +3939,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="41"/>
       <c r="F13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="2:6">
@@ -3958,7 +3952,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="41"/>
       <c r="F14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="2:6">
@@ -3983,7 +3977,7 @@
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>39</v>
@@ -3992,7 +3986,7 @@
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>36</v>
@@ -4010,7 +4004,7 @@
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>39</v>
@@ -4025,25 +4019,25 @@
         <v>36</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E21" s="41"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E22" s="41"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>39</v>
@@ -4052,7 +4046,7 @@
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>39</v>
@@ -4061,7 +4055,7 @@
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>39</v>
@@ -4082,7 +4076,7 @@
     </row>
     <row r="27" spans="2:5">
       <c r="B27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>37</v>
@@ -4091,13 +4085,13 @@
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="27" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E28" s="41"/>
     </row>
@@ -4112,7 +4106,7 @@
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="31" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>39</v>
@@ -4121,7 +4115,7 @@
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="27" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>38</v>
@@ -4130,7 +4124,7 @@
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>37</v>
@@ -4139,7 +4133,7 @@
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="31" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>39</v>
@@ -4148,7 +4142,7 @@
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>37</v>
@@ -4157,13 +4151,13 @@
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C35" s="34" t="s">
         <v>38</v>
       </c>
       <c r="D35" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E35" s="41"/>
     </row>
@@ -4175,13 +4169,13 @@
         <v>38</v>
       </c>
       <c r="D36" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E36" s="41"/>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="33" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C37" s="34" t="s">
         <v>39</v>
@@ -4190,7 +4184,7 @@
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C38" s="34" t="s">
         <v>38</v>
@@ -4199,19 +4193,19 @@
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="32" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C39" s="34" t="s">
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E39" s="41"/>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="33" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C40" s="34" t="s">
         <v>39</v>
@@ -4234,7 +4228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -4610,7 +4604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -5063,7 +5057,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -5589,8 +5583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5942,33 +5936,33 @@
       <c r="E31" s="41"/>
     </row>
     <row r="33" spans="4:4">
-      <c r="D33" t="s">
+      <c r="D33" s="20" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="20" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4">
+      <c r="D35" s="20" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="34" spans="4:4">
-      <c r="D34" t="s">
+    <row r="36" spans="4:4">
+      <c r="D36" s="20" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="35" spans="4:4">
-      <c r="D35" t="s">
+    <row r="37" spans="4:4">
+      <c r="D37" s="20" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="36" spans="4:4">
-      <c r="D36" t="s">
+    <row r="38" spans="4:4">
+      <c r="D38" s="20" t="s">
         <v>391</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4">
-      <c r="D37" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4">
-      <c r="D38" t="s">
-        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -6006,7 +6000,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
@@ -6016,7 +6010,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6033,7 +6027,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -6197,7 +6191,7 @@
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="13" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>38</v>
@@ -6223,9 +6217,6 @@
       <c r="C22" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D22" t="s">
-        <v>336</v>
-      </c>
       <c r="E22" s="41"/>
     </row>
     <row r="23" spans="2:5">
@@ -6251,7 +6242,7 @@
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>38</v>
@@ -6260,25 +6251,19 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="13" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="D26" t="s">
-        <v>336</v>
       </c>
       <c r="E26" s="41"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>38</v>
-      </c>
-      <c r="D27" t="s">
-        <v>336</v>
       </c>
       <c r="E27" s="41"/>
     </row>
@@ -6316,8 +6301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6735,7 +6720,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
@@ -6745,7 +6730,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6760,7 +6745,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -6789,14 +6774,14 @@
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="41"/>
       <c r="E8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -6869,12 +6854,12 @@
       </c>
       <c r="D15" s="41"/>
       <c r="E15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>37</v>
@@ -6901,7 +6886,7 @@
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="37" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>36</v>
@@ -6919,7 +6904,7 @@
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
@@ -6935,7 +6920,7 @@
       </c>
       <c r="D22" s="41"/>
       <c r="E22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="23" spans="2:5">
@@ -6976,7 +6961,7 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>37</v>
@@ -7009,10 +6994,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F33"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -7117,7 +7102,9 @@
       <c r="C10" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
       <c r="E10" t="s">
         <v>231</v>
       </c>
@@ -7191,13 +7178,13 @@
         <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E16" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="1:5">
       <c r="B17" t="s">
         <v>206</v>
       </c>
@@ -7205,13 +7192,13 @@
         <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E17" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="1:5">
       <c r="B18" t="s">
         <v>225</v>
       </c>
@@ -7219,29 +7206,29 @@
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E18" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="20" t="s">
+    <row r="19" spans="1:5">
+      <c r="B19" s="1" t="s">
         <v>226</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" s="1" t="s">
         <v>227</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="B21" t="s">
         <v>228</v>
       </c>
@@ -7249,7 +7236,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="1:5">
       <c r="B22" t="s">
         <v>229</v>
       </c>
@@ -7257,57 +7244,78 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="20" t="s">
+    <row r="23" spans="1:5">
+      <c r="B23" s="1" t="s">
         <v>230</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="D25" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>203</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>204</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="30"/>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="30"/>
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="D28" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="2:5">
-      <c r="D26" t="s">
+    <row r="29" spans="1:5">
+      <c r="D29" s="20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:5">
-      <c r="D27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="D28" t="s">
+    <row r="30" spans="1:5">
+      <c r="D30" s="20" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="2:5">
-      <c r="D29" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="D30" t="s">
+    <row r="31" spans="1:5">
+      <c r="D31" s="20" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="31" spans="2:5">
-      <c r="D31" t="s">
+    <row r="32" spans="1:5">
+      <c r="D32" s="20" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="2:5">
-      <c r="D32" t="s">
-        <v>244</v>
-      </c>
-    </row>
     <row r="33" spans="4:4">
-      <c r="D33" t="s">
-        <v>247</v>
+      <c r="D33" s="20" t="s">
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fasting status added to Specimen
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="394">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -1216,6 +1216,9 @@
   </si>
   <si>
     <t>primarycare-condition-related-extension</t>
+  </si>
+  <si>
+    <t>fasting</t>
   </si>
 </sst>
 </file>
@@ -2233,10 +2236,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2402,7 +2405,7 @@
       </c>
       <c r="E16" s="41"/>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="1:5">
       <c r="B17" s="22" t="s">
         <v>313</v>
       </c>
@@ -2414,7 +2417,7 @@
       </c>
       <c r="E17" s="41"/>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="1:5">
       <c r="B18" s="22" t="s">
         <v>174</v>
       </c>
@@ -2426,7 +2429,7 @@
       </c>
       <c r="E18" s="41"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="1:5">
       <c r="B19" s="22" t="s">
         <v>205</v>
       </c>
@@ -2438,7 +2441,7 @@
       </c>
       <c r="E19" s="41"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="1:5">
       <c r="B20" s="22" t="s">
         <v>22</v>
       </c>
@@ -2450,121 +2453,133 @@
       </c>
       <c r="E20" s="41"/>
     </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="21" t="s">
+    <row r="21" spans="1:5">
+      <c r="A21" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>393</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="E21" s="41"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" s="21" t="s">
         <v>314</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="41"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="22" t="s">
+      <c r="C22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="41"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="41"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="22" t="s">
+      <c r="C23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="41"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" s="22" t="s">
         <v>315</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="41"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="22" t="s">
+      <c r="C24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="41"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" s="22" t="s">
         <v>316</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="41"/>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="21" t="s">
+      <c r="C25" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="41"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" s="21" t="s">
         <v>317</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="41"/>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="22" t="s">
+      <c r="C26" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="41"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="41"/>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="22" t="s">
+      <c r="C27" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="41"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="41"/>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="22" t="s">
+      <c r="C28" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="41"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="41"/>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="22" t="s">
+      <c r="C29" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="41"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="41"/>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="B30" s="22" t="s">
+      <c r="C30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="41"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" s="22" t="s">
         <v>319</v>
       </c>
-      <c r="C30" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E30" s="41"/>
-    </row>
-    <row r="31" spans="2:5">
-      <c r="B31" s="22" t="s">
+      <c r="C31" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="41"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" s="22" t="s">
         <v>320</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="41"/>
-    </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="2:4">
+      <c r="C32" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="41"/>
+    </row>
+    <row r="33" spans="2:2">
       <c r="B33" s="1"/>
-      <c r="D33" s="2" t="s">
-        <v>323</v>
-      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="E7:E31"/>
+    <mergeCell ref="E7:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -6996,8 +7011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Purpose ext. removed from Encounter
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="382">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -783,9 +783,6 @@
   </si>
   <si>
     <t>hospitalization</t>
-  </si>
-  <si>
-    <t>purpose</t>
   </si>
   <si>
     <t>individual</t>
@@ -1767,7 +1764,7 @@
     <row r="9" spans="2:6">
       <c r="B9" s="4"/>
       <c r="C9" s="38" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
@@ -2223,7 +2220,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
@@ -2248,7 +2245,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -2291,13 +2288,13 @@
         <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E9" s="41"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>37</v>
@@ -2319,31 +2316,31 @@
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E12" s="41"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E13" s="41"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>38</v>
@@ -2352,7 +2349,7 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>38</v>
@@ -2361,25 +2358,25 @@
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E16" s="41"/>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E17" s="41"/>
     </row>
@@ -2391,7 +2388,7 @@
         <v>38</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E18" s="41"/>
     </row>
@@ -2403,7 +2400,7 @@
         <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E19" s="41"/>
     </row>
@@ -2415,7 +2412,7 @@
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E20" s="41"/>
     </row>
@@ -2424,19 +2421,19 @@
         <v>6</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E21" s="41"/>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>37</v>
@@ -2454,7 +2451,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>38</v>
@@ -2463,7 +2460,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="B25" s="22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>37</v>
@@ -2472,7 +2469,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="B26" s="21" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>37</v>
@@ -2509,7 +2506,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="22" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>38</v>
@@ -2518,7 +2515,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="22" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>38</v>
@@ -2527,7 +2524,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="22" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>38</v>
@@ -2556,7 +2553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D59" sqref="D59:D83"/>
     </sheetView>
   </sheetViews>
@@ -2575,7 +2572,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
@@ -2585,7 +2582,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -2602,7 +2599,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -2624,12 +2621,12 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>38</v>
@@ -2638,7 +2635,7 @@
         <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -2655,19 +2652,19 @@
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>38</v>
@@ -2688,7 +2685,7 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>36</v>
@@ -2697,7 +2694,7 @@
         <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" spans="2:6">
@@ -2743,19 +2740,19 @@
         <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2766,13 +2763,13 @@
         <v>38</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="30"/>
       <c r="B20" s="36" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>38</v>
@@ -2781,7 +2778,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="36" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
@@ -2790,7 +2787,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="36" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>38</v>
@@ -2799,7 +2796,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="B23" s="36" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>38</v>
@@ -2808,7 +2805,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="36" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>38</v>
@@ -2826,7 +2823,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="B26" s="36" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>38</v>
@@ -2834,7 +2831,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="B27" s="36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>38</v>
@@ -2843,7 +2840,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="36" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>38</v>
@@ -2852,7 +2849,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>38</v>
@@ -2870,7 +2867,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="36" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>38</v>
@@ -2879,7 +2876,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="36" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>38</v>
@@ -2894,15 +2891,15 @@
         <v>38</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E33" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="36" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>38</v>
@@ -2911,7 +2908,7 @@
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>38</v>
@@ -2939,7 +2936,7 @@
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>38</v>
@@ -2952,102 +2949,102 @@
     </row>
     <row r="40" spans="2:5">
       <c r="D40" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E40" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="D41" s="28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E41" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="D42" s="28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E42" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="D43" s="28" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E43" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="D44" s="28" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E44" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="D45" s="28" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="D46" s="28" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" spans="2:5">
       <c r="D47" s="28" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="D48" s="28" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="49" spans="4:4">
       <c r="D49" s="28" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="50" spans="4:4">
       <c r="D50" s="28" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="51" spans="4:4">
       <c r="D51" s="28" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="52" spans="4:4">
       <c r="D52" s="28" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="53" spans="4:4">
       <c r="D53" s="28" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="54" spans="4:4">
       <c r="D54" s="28" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="55" spans="4:4">
       <c r="D55" s="28" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="56" spans="4:4">
       <c r="D56" s="28" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="59" spans="4:4">
@@ -3188,10 +3185,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3229,7 +3226,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
@@ -3299,10 +3296,10 @@
         <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -3322,7 +3319,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E13" t="s">
         <v>41</v>
@@ -3355,7 +3352,7 @@
         <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -3368,7 +3365,7 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3383,16 +3380,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="B19" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3412,10 +3409,10 @@
         <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3426,7 +3423,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E22" s="2"/>
     </row>
@@ -3437,7 +3434,9 @@
       <c r="C23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>264</v>
+      </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
@@ -3468,7 +3467,7 @@
         <v>37</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E26" t="s">
         <v>116</v>
@@ -3477,19 +3476,19 @@
     <row r="27" spans="1:5">
       <c r="A27" s="30"/>
       <c r="B27" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>39</v>
@@ -3498,26 +3497,12 @@
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>265</v>
-      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="D31" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3553,7 +3538,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
@@ -3563,7 +3548,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -3578,7 +3563,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -3611,7 +3596,7 @@
         <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E8" s="41"/>
     </row>
@@ -3635,7 +3620,7 @@
       <c r="D10" s="5"/>
       <c r="E10" s="41"/>
       <c r="F10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="2:6">
@@ -3668,7 +3653,7 @@
       <c r="D13" s="5"/>
       <c r="E13" s="41"/>
       <c r="F13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="2:6">
@@ -3681,7 +3666,7 @@
       <c r="D14" s="5"/>
       <c r="E14" s="41"/>
       <c r="F14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="2:6">
@@ -3715,7 +3700,7 @@
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>36</v>
@@ -3733,7 +3718,7 @@
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>39</v>
@@ -3748,25 +3733,25 @@
         <v>36</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E21" s="41"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="11" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E22" s="41"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>39</v>
@@ -3775,7 +3760,7 @@
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>39</v>
@@ -3784,7 +3769,7 @@
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>39</v>
@@ -3805,7 +3790,7 @@
     </row>
     <row r="27" spans="2:5">
       <c r="B27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>37</v>
@@ -3814,13 +3799,13 @@
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E28" s="41"/>
     </row>
@@ -3835,7 +3820,7 @@
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="31" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>39</v>
@@ -3844,7 +3829,7 @@
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>38</v>
@@ -3853,7 +3838,7 @@
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="27" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>37</v>
@@ -3862,7 +3847,7 @@
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="31" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>39</v>
@@ -3871,7 +3856,7 @@
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>37</v>
@@ -3880,13 +3865,13 @@
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C35" s="34" t="s">
         <v>38</v>
       </c>
       <c r="D35" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E35" s="41"/>
     </row>
@@ -3898,13 +3883,13 @@
         <v>38</v>
       </c>
       <c r="D36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E36" s="41"/>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C37" s="34" t="s">
         <v>39</v>
@@ -3913,7 +3898,7 @@
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="32" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C38" s="34" t="s">
         <v>38</v>
@@ -3922,19 +3907,19 @@
     </row>
     <row r="39" spans="2:5">
       <c r="B39" s="32" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C39" s="34" t="s">
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E39" s="41"/>
     </row>
     <row r="40" spans="2:5">
       <c r="B40" s="33" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C40" s="34" t="s">
         <v>39</v>
@@ -5666,32 +5651,32 @@
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="20" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="34" spans="4:4">
       <c r="D34" s="20" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="35" spans="4:4">
       <c r="D35" s="20" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="36" spans="4:4">
       <c r="D36" s="20" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="37" spans="4:4">
       <c r="D37" s="20" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="38" spans="4:4">
       <c r="D38" s="20" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -5729,7 +5714,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
@@ -5739,7 +5724,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -5756,7 +5741,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -5920,7 +5905,7 @@
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>38</v>
@@ -5971,7 +5956,7 @@
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="13" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>38</v>
@@ -5980,7 +5965,7 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>38</v>
@@ -5989,7 +5974,7 @@
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>38</v>
@@ -6449,7 +6434,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D1" s="39"/>
       <c r="E1" s="39"/>
@@ -6459,7 +6444,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="39"/>
@@ -6474,7 +6459,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -6503,14 +6488,14 @@
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="41"/>
       <c r="E8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -6583,12 +6568,12 @@
       </c>
       <c r="D15" s="41"/>
       <c r="E15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>37</v>
@@ -6615,7 +6600,7 @@
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="37" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>36</v>
@@ -6633,7 +6618,7 @@
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
@@ -6649,7 +6634,7 @@
       </c>
       <c r="D22" s="41"/>
       <c r="E22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="2:5">
@@ -6690,7 +6675,7 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="36" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Primary Care Composition added
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="6" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Specimen" sheetId="13" r:id="rId10"/>
     <sheet name="MedicationOrder" sheetId="15" r:id="rId11"/>
     <sheet name="Encounter" sheetId="10" r:id="rId12"/>
-    <sheet name="EncounterComposition" sheetId="11" r:id="rId13"/>
+    <sheet name="Composition" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="381">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -794,9 +794,6 @@
     <t>partOf</t>
   </si>
   <si>
-    <t>primarycare-encounter-purpose-extension</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -833,9 +830,6 @@
     <t>encounter.clinicalPurpose</t>
   </si>
   <si>
-    <t>PrimaryCare-EncounterComposition</t>
-  </si>
-  <si>
     <t>Composition</t>
   </si>
   <si>
@@ -872,15 +866,6 @@
     <t>emptyReason</t>
   </si>
   <si>
-    <t>Fixed: http://snomed.info/sct</t>
-  </si>
-  <si>
-    <t>Fixed: 25671000000102</t>
-  </si>
-  <si>
-    <t>Fixed: Surgery consultation note (record artifact)</t>
-  </si>
-  <si>
     <t>encounter.authorisingUserInRole</t>
   </si>
   <si>
@@ -1182,6 +1167,18 @@
   </si>
   <si>
     <t>fasting</t>
+  </si>
+  <si>
+    <t>primarycare-diagnostic-report-interpretation-extension</t>
+  </si>
+  <si>
+    <t>primarycare-diagnostic-report-comment-extension</t>
+  </si>
+  <si>
+    <t>primarycare-specimen-fasting-extension</t>
+  </si>
+  <si>
+    <t>PrimaryCare-Composition</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1286,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1355,13 +1352,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1387,6 +1378,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1695,85 +1689,85 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="4"/>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="4"/>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="4"/>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="4"/>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="4"/>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="4"/>
-      <c r="C9" s="38" t="s">
-        <v>380</v>
-      </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
+      <c r="C9" s="36" t="s">
+        <v>375</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="18"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="3" t="s">
@@ -2201,8 +2195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2219,33 +2213,35 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
-        <v>294</v>
-      </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="C1" s="37" t="s">
+        <v>289</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="C3" s="36" t="s">
+        <v>379</v>
+      </c>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -2266,7 +2262,7 @@
         <v>37</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="39" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2278,7 +2274,7 @@
         <v>38</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="41"/>
+      <c r="E8" s="39"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="1" t="s">
@@ -2288,19 +2284,19 @@
         <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E9" s="41"/>
+        <v>305</v>
+      </c>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="21" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="41"/>
+      <c r="E10" s="39"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="12" t="s">
@@ -2312,73 +2308,73 @@
       <c r="D11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="41"/>
+      <c r="E11" s="39"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="21" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="E12" s="41"/>
+        <v>304</v>
+      </c>
+      <c r="E12" s="39"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="21" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="E13" s="41"/>
+        <v>310</v>
+      </c>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="21" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="41"/>
+      <c r="E14" s="39"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="22" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="41"/>
+      <c r="E15" s="39"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="22" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="E16" s="41"/>
+        <v>311</v>
+      </c>
+      <c r="E16" s="39"/>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="22" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="E17" s="41"/>
+        <v>312</v>
+      </c>
+      <c r="E17" s="39"/>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="22" t="s">
@@ -2388,9 +2384,9 @@
         <v>38</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="E18" s="41"/>
+        <v>307</v>
+      </c>
+      <c r="E18" s="39"/>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" s="22" t="s">
@@ -2400,9 +2396,9 @@
         <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="E19" s="41"/>
+        <v>308</v>
+      </c>
+      <c r="E19" s="39"/>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="22" t="s">
@@ -2412,33 +2408,33 @@
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="E20" s="41"/>
+        <v>309</v>
+      </c>
+      <c r="E20" s="39"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="E21" s="41"/>
+        <v>306</v>
+      </c>
+      <c r="E21" s="39"/>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="21" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="41"/>
+      <c r="E22" s="39"/>
     </row>
     <row r="23" spans="1:5">
       <c r="B23" s="22" t="s">
@@ -2447,35 +2443,35 @@
       <c r="C23" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="41"/>
+      <c r="E23" s="39"/>
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="22" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="41"/>
+      <c r="E24" s="39"/>
     </row>
     <row r="25" spans="1:5">
       <c r="B25" s="22" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="41"/>
+      <c r="E25" s="39"/>
     </row>
     <row r="26" spans="1:5">
       <c r="B26" s="21" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="41"/>
+      <c r="E26" s="39"/>
     </row>
     <row r="27" spans="1:5">
       <c r="B27" s="22" t="s">
@@ -2484,7 +2480,7 @@
       <c r="C27" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="41"/>
+      <c r="E27" s="39"/>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="22" t="s">
@@ -2493,7 +2489,7 @@
       <c r="C28" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="41"/>
+      <c r="E28" s="39"/>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="22" t="s">
@@ -2502,34 +2498,34 @@
       <c r="C29" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="41"/>
+      <c r="E29" s="39"/>
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="22" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="41"/>
+      <c r="E30" s="39"/>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="22" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="41"/>
+      <c r="E31" s="39"/>
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="22" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="41"/>
+      <c r="E32" s="39"/>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="1"/>
@@ -2553,7 +2549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D59" sqref="D59:D83"/>
     </sheetView>
   </sheetViews>
@@ -2571,35 +2567,35 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
-        <v>323</v>
-      </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="C1" s="37" t="s">
+        <v>318</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
-        <v>324</v>
-      </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="C2" s="37" t="s">
+        <v>319</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -2621,12 +2617,12 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>38</v>
@@ -2635,7 +2631,7 @@
         <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -2652,24 +2648,24 @@
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="1" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="35"/>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="11" t="s">
@@ -2681,11 +2677,11 @@
       <c r="D12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="33"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="11" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>36</v>
@@ -2694,7 +2690,7 @@
         <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="2:6">
@@ -2704,7 +2700,7 @@
       <c r="C14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="35"/>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="1" t="s">
@@ -2713,7 +2709,7 @@
       <c r="C15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="1" t="s">
@@ -2740,311 +2736,311 @@
         <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="34" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="30"/>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="33"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" s="34" t="s">
+        <v>326</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="33"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="B22" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="33"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="33"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="33"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" s="34" t="s">
+        <v>194</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="33"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" s="34" t="s">
+        <v>329</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" s="34" t="s">
         <v>330</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="35"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" s="36" t="s">
+      <c r="C27" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="33"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="34" t="s">
         <v>331</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="35"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="B22" s="36" t="s">
-        <v>321</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="35"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" s="36" t="s">
-        <v>332</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="35"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" s="36" t="s">
-        <v>333</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="35"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" s="36" t="s">
-        <v>194</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="35"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" s="36" t="s">
-        <v>334</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" s="36" t="s">
-        <v>335</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E27" s="35"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" s="36" t="s">
-        <v>336</v>
-      </c>
       <c r="C28" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="35"/>
+      <c r="E28" s="33"/>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="1" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="35"/>
+      <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="34" t="s">
         <v>162</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E30" s="35"/>
+      <c r="E30" s="33"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="B31" s="36" t="s">
-        <v>338</v>
+      <c r="B31" s="34" t="s">
+        <v>333</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="35"/>
+      <c r="E31" s="33"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32" s="36" t="s">
-        <v>339</v>
+      <c r="B32" s="34" t="s">
+        <v>334</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="35"/>
+      <c r="E32" s="33"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="34" t="s">
         <v>165</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E33" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="34" spans="2:5">
-      <c r="B34" s="36" t="s">
-        <v>340</v>
+      <c r="B34" s="34" t="s">
+        <v>335</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E34" s="35"/>
+      <c r="E34" s="33"/>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="35"/>
+      <c r="E35" s="33"/>
     </row>
     <row r="36" spans="2:5">
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="35" t="s">
         <v>80</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="35"/>
+      <c r="E36" s="33"/>
     </row>
     <row r="37" spans="2:5">
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="34" t="s">
         <v>145</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D37" s="27"/>
-      <c r="E37" s="35"/>
+      <c r="E37" s="33"/>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="1" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D38" s="27"/>
-      <c r="E38" s="35"/>
+      <c r="E38" s="33"/>
     </row>
     <row r="39" spans="2:5">
       <c r="D39" s="27"/>
     </row>
     <row r="40" spans="2:5">
       <c r="D40" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="E40" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="D41" s="28" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="E41" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="D42" s="28" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="E42" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="D43" s="28" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="E43" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="D44" s="28" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="E44" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="D45" s="28" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="D46" s="28" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="47" spans="2:5">
       <c r="D47" s="28" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="D48" s="28" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="49" spans="4:4">
       <c r="D49" s="28" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="50" spans="4:4">
       <c r="D50" s="28" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="51" spans="4:4">
       <c r="D51" s="28" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="52" spans="4:4">
       <c r="D52" s="28" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="53" spans="4:4">
       <c r="D53" s="28" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="54" spans="4:4">
       <c r="D54" s="28" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="55" spans="4:4">
       <c r="D55" s="28" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56" spans="4:4">
       <c r="D56" s="28" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="59" spans="4:4">
@@ -3187,8 +3183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3205,31 +3201,29 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>237</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>238</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
-        <v>252</v>
-      </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
@@ -3296,10 +3290,10 @@
         <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -3319,7 +3313,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E13" t="s">
         <v>41</v>
@@ -3352,7 +3346,7 @@
         <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -3365,7 +3359,7 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3386,10 +3380,10 @@
         <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3409,10 +3403,10 @@
         <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3423,7 +3417,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E22" s="2"/>
     </row>
@@ -3435,7 +3429,7 @@
         <v>37</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E23" s="2"/>
     </row>
@@ -3467,7 +3461,7 @@
         <v>37</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E26" t="s">
         <v>116</v>
@@ -3482,7 +3476,7 @@
         <v>38</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E27" s="2"/>
     </row>
@@ -3517,10 +3511,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F40"/>
+  <dimension ref="B1:F33"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3537,33 +3531,33 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
-        <v>265</v>
-      </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="C1" s="37" t="s">
+        <v>380</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
-        <v>266</v>
-      </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="C2" s="37" t="s">
+        <v>264</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>265</v>
+        <v>380</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -3584,7 +3578,7 @@
         <v>37</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="39" t="s">
         <v>150</v>
       </c>
     </row>
@@ -3596,9 +3590,9 @@
         <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="E8" s="41"/>
+        <v>257</v>
+      </c>
+      <c r="E8" s="39"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="11" t="s">
@@ -3608,330 +3602,251 @@
         <v>36</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="41"/>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="14" t="s">
-        <v>29</v>
+      <c r="B10" s="1" t="s">
+        <v>240</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="41"/>
-      <c r="F10" t="s">
-        <v>278</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E10" s="39"/>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="25" t="s">
-        <v>30</v>
+      <c r="B11" s="11" t="s">
+        <v>265</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="41"/>
+      <c r="E11" s="39"/>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="24" t="s">
-        <v>31</v>
+      <c r="B12" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="39"/>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="20" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="41"/>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="41"/>
-      <c r="F13" t="s">
-        <v>279</v>
-      </c>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="25" t="s">
-        <v>32</v>
+      <c r="B14" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="41"/>
-      <c r="F14" t="s">
+      <c r="D14" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E14" s="39"/>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E15" s="39"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="39"/>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="39"/>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="39"/>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="39"/>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" t="s">
+        <v>271</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="39"/>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>277</v>
+      </c>
+      <c r="E21" s="39"/>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="39"/>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="39"/>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="39"/>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="39"/>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="39"/>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="39"/>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>278</v>
+      </c>
+      <c r="E28" s="39"/>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>279</v>
+      </c>
+      <c r="E29" s="39"/>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="39"/>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="31" t="s">
+        <v>273</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="39"/>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="B15" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="41"/>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="41"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="41"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="41"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="41"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="20" t="s">
-        <v>268</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="41"/>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="E21" s="41"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="E22" s="41"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="41"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="41"/>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="20" t="s">
-        <v>272</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="41"/>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="41"/>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" t="s">
-        <v>273</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" s="41"/>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" t="s">
-        <v>282</v>
-      </c>
-      <c r="E28" s="41"/>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="41"/>
-    </row>
-    <row r="30" spans="2:5">
-      <c r="B30" s="31" t="s">
-        <v>274</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="41"/>
-    </row>
-    <row r="31" spans="2:5">
-      <c r="B31" s="27" t="s">
+      <c r="E32" s="39"/>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="42" t="s">
         <v>275</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E31" s="41"/>
-    </row>
-    <row r="32" spans="2:5">
-      <c r="B32" s="27" t="s">
-        <v>276</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E32" s="41"/>
-    </row>
-    <row r="33" spans="2:5">
-      <c r="B33" s="31" t="s">
-        <v>277</v>
-      </c>
       <c r="C33" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="41"/>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="27" t="s">
-        <v>273</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="41"/>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" t="s">
-        <v>283</v>
-      </c>
-      <c r="E35" s="41"/>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" t="s">
-        <v>284</v>
-      </c>
-      <c r="E36" s="41"/>
-    </row>
-    <row r="37" spans="2:5">
-      <c r="B37" s="33" t="s">
-        <v>274</v>
-      </c>
-      <c r="C37" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="E37" s="41"/>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="B38" s="32" t="s">
-        <v>275</v>
-      </c>
-      <c r="C38" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="E38" s="41"/>
-    </row>
-    <row r="39" spans="2:5">
-      <c r="B39" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="C39" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="D39" t="s">
-        <v>285</v>
-      </c>
-      <c r="E39" s="41"/>
-    </row>
-    <row r="40" spans="2:5">
-      <c r="B40" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="C40" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="E40" s="41"/>
+        <v>38</v>
+      </c>
+      <c r="E33" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
-    <mergeCell ref="E7:E40"/>
+    <mergeCell ref="E7:E33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3942,8 +3857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3960,39 +3875,39 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="4"/>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="3" t="s">
@@ -4284,7 +4199,7 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="41" t="s">
         <v>85</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -4318,7 +4233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
@@ -4336,39 +4251,39 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="4"/>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="3" t="s">
@@ -4771,7 +4686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -4789,55 +4704,55 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="4"/>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="4"/>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="4"/>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="3" t="s">
@@ -4862,7 +4777,7 @@
         <v>37</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="38" t="s">
         <v>150</v>
       </c>
     </row>
@@ -4876,7 +4791,7 @@
       <c r="D11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="40"/>
+      <c r="E11" s="38"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="5" t="s">
@@ -4888,7 +4803,7 @@
       <c r="D12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="40"/>
+      <c r="E12" s="38"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="12" t="s">
@@ -4898,7 +4813,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="40"/>
+      <c r="E13" s="38"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="5" t="s">
@@ -4908,7 +4823,7 @@
         <v>38</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="40"/>
+      <c r="E14" s="38"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="12" t="s">
@@ -4920,7 +4835,7 @@
       <c r="D15" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E15" s="40"/>
+      <c r="E15" s="38"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="7" t="s">
@@ -4930,7 +4845,7 @@
         <v>37</v>
       </c>
       <c r="D16" s="5"/>
-      <c r="E16" s="40"/>
+      <c r="E16" s="38"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="8" t="s">
@@ -4942,7 +4857,7 @@
       <c r="D17" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E17" s="40"/>
+      <c r="E17" s="38"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="8" t="s">
@@ -4952,7 +4867,7 @@
         <v>38</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="40"/>
+      <c r="E18" s="38"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="8" t="s">
@@ -4964,7 +4879,7 @@
       <c r="D19" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="E19" s="40"/>
+      <c r="E19" s="38"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="8" t="s">
@@ -4976,7 +4891,7 @@
       <c r="D20" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E20" s="40"/>
+      <c r="E20" s="38"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="8" t="s">
@@ -4986,7 +4901,7 @@
         <v>38</v>
       </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="40"/>
+      <c r="E21" s="38"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="7" t="s">
@@ -4996,7 +4911,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="40"/>
+      <c r="E22" s="38"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="5" t="s">
@@ -5006,7 +4921,7 @@
         <v>38</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="40"/>
+      <c r="E23" s="38"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="21" t="s">
@@ -5016,7 +4931,7 @@
         <v>38</v>
       </c>
       <c r="D24" s="5"/>
-      <c r="E24" s="40"/>
+      <c r="E24" s="38"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="21" t="s">
@@ -5026,7 +4941,7 @@
         <v>38</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="40"/>
+      <c r="E25" s="38"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="5" t="s">
@@ -5036,7 +4951,7 @@
         <v>38</v>
       </c>
       <c r="D26" s="2"/>
-      <c r="E26" s="40"/>
+      <c r="E26" s="38"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="13" t="s">
@@ -5045,7 +4960,7 @@
       <c r="C27" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="40"/>
+      <c r="E27" s="38"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="15" t="s">
@@ -5054,7 +4969,7 @@
       <c r="C28" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E28" s="40"/>
+      <c r="E28" s="38"/>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="15" t="s">
@@ -5063,7 +4978,7 @@
       <c r="C29" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="40"/>
+      <c r="E29" s="38"/>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="14" t="s">
@@ -5073,7 +4988,7 @@
         <v>36</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="40"/>
+      <c r="E30" s="38"/>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="12" t="s">
@@ -5085,7 +5000,7 @@
       <c r="D31" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="40"/>
+      <c r="E31" s="38"/>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="22" t="s">
@@ -5095,7 +5010,7 @@
         <v>36</v>
       </c>
       <c r="D32" s="5"/>
-      <c r="E32" s="40"/>
+      <c r="E32" s="38"/>
     </row>
     <row r="33" spans="1:5">
       <c r="B33" s="8" t="s">
@@ -5107,7 +5022,7 @@
       <c r="D33" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="40"/>
+      <c r="E33" s="38"/>
     </row>
     <row r="34" spans="1:5">
       <c r="B34" s="23" t="s">
@@ -5119,7 +5034,7 @@
       <c r="D34" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="40"/>
+      <c r="E34" s="38"/>
     </row>
     <row r="35" spans="1:5">
       <c r="B35" s="23" t="s">
@@ -5129,7 +5044,7 @@
         <v>38</v>
       </c>
       <c r="D35" s="2"/>
-      <c r="E35" s="40"/>
+      <c r="E35" s="38"/>
     </row>
     <row r="36" spans="1:5">
       <c r="B36" s="23" t="s">
@@ -5141,7 +5056,7 @@
       <c r="D36" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="40"/>
+      <c r="E36" s="38"/>
     </row>
     <row r="37" spans="1:5">
       <c r="B37" s="23" t="s">
@@ -5153,7 +5068,7 @@
       <c r="D37" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E37" s="40"/>
+      <c r="E37" s="38"/>
     </row>
     <row r="38" spans="1:5">
       <c r="B38" s="23" t="s">
@@ -5163,7 +5078,7 @@
         <v>38</v>
       </c>
       <c r="D38" s="2"/>
-      <c r="E38" s="40"/>
+      <c r="E38" s="38"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="10" t="s">
@@ -5178,7 +5093,7 @@
       <c r="D39" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E39" s="40"/>
+      <c r="E39" s="38"/>
     </row>
     <row r="40" spans="1:5">
       <c r="B40" s="8" t="s">
@@ -5190,7 +5105,7 @@
       <c r="D40" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E40" s="40"/>
+      <c r="E40" s="38"/>
     </row>
     <row r="41" spans="1:5">
       <c r="B41" s="7" t="s">
@@ -5200,7 +5115,7 @@
         <v>38</v>
       </c>
       <c r="D41" s="5"/>
-      <c r="E41" s="40"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:5">
       <c r="B42" s="7" t="s">
@@ -5210,7 +5125,7 @@
         <v>38</v>
       </c>
       <c r="D42" s="5"/>
-      <c r="E42" s="40"/>
+      <c r="E42" s="38"/>
     </row>
     <row r="43" spans="1:5">
       <c r="B43" s="7" t="s">
@@ -5219,7 +5134,7 @@
       <c r="C43" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E43" s="40"/>
+      <c r="E43" s="38"/>
     </row>
     <row r="44" spans="1:5">
       <c r="B44" s="24" t="s">
@@ -5228,7 +5143,7 @@
       <c r="C44" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E44" s="40"/>
+      <c r="E44" s="38"/>
     </row>
     <row r="45" spans="1:5">
       <c r="B45" s="24" t="s">
@@ -5237,7 +5152,7 @@
       <c r="C45" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E45" s="40"/>
+      <c r="E45" s="38"/>
     </row>
     <row r="46" spans="1:5">
       <c r="B46" s="25" t="s">
@@ -5249,7 +5164,7 @@
       <c r="D46" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E46" s="40"/>
+      <c r="E46" s="38"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="10" t="s">
@@ -5264,7 +5179,7 @@
       <c r="D47" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E47" s="40"/>
+      <c r="E47" s="38"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="10" t="s">
@@ -5276,7 +5191,7 @@
       <c r="C48" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E48" s="40"/>
+      <c r="E48" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5297,7 +5212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
@@ -5315,31 +5230,31 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
@@ -5364,7 +5279,7 @@
         <v>36</v>
       </c>
       <c r="D7" s="26"/>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="39" t="s">
         <v>150</v>
       </c>
       <c r="F7" s="26"/>
@@ -5377,7 +5292,7 @@
         <v>37</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="41"/>
+      <c r="E8" s="39"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="27" t="s">
@@ -5389,7 +5304,7 @@
       <c r="D9" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E9" s="41"/>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="28" t="s">
@@ -5401,7 +5316,7 @@
       <c r="D10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="41"/>
+      <c r="E10" s="39"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="28" t="s">
@@ -5413,7 +5328,7 @@
       <c r="D11" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E11" s="41"/>
+      <c r="E11" s="39"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="28" t="s">
@@ -5425,7 +5340,7 @@
       <c r="D12" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="39"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="28" t="s">
@@ -5437,7 +5352,7 @@
       <c r="D13" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E13" s="41"/>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="11" t="s">
@@ -5449,7 +5364,7 @@
       <c r="D14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="41"/>
+      <c r="E14" s="39"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="11" t="s">
@@ -5461,7 +5376,7 @@
       <c r="D15" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E15" s="41"/>
+      <c r="E15" s="39"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="11" t="s">
@@ -5473,7 +5388,7 @@
       <c r="D16" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E16" s="41"/>
+      <c r="E16" s="39"/>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" t="s">
@@ -5483,7 +5398,7 @@
         <v>38</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="41"/>
+      <c r="E17" s="39"/>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
@@ -5495,7 +5410,7 @@
       <c r="D18" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="41"/>
+      <c r="E18" s="39"/>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" t="s">
@@ -5507,7 +5422,7 @@
       <c r="D19" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="41"/>
+      <c r="E19" s="39"/>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="7" t="s">
@@ -5519,7 +5434,7 @@
       <c r="D20" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="41"/>
+      <c r="E20" s="39"/>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="8" t="s">
@@ -5531,7 +5446,7 @@
       <c r="D21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="41"/>
+      <c r="E21" s="39"/>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="8" t="s">
@@ -5541,7 +5456,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="41"/>
+      <c r="E22" s="39"/>
     </row>
     <row r="23" spans="1:5">
       <c r="B23" s="8" t="s">
@@ -5553,7 +5468,7 @@
       <c r="D23" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="41"/>
+      <c r="E23" s="39"/>
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="8" t="s">
@@ -5565,7 +5480,7 @@
       <c r="D24" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="41"/>
+      <c r="E24" s="39"/>
     </row>
     <row r="25" spans="1:5">
       <c r="B25" s="8" t="s">
@@ -5575,7 +5490,7 @@
         <v>38</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="41"/>
+      <c r="E25" s="39"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="10" t="s">
@@ -5590,7 +5505,7 @@
       <c r="D26" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="41"/>
+      <c r="E26" s="39"/>
     </row>
     <row r="27" spans="1:5">
       <c r="B27" s="7" t="s">
@@ -5602,7 +5517,7 @@
       <c r="D27" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="41"/>
+      <c r="E27" s="39"/>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="13" t="s">
@@ -5614,7 +5529,7 @@
       <c r="D28" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E28" s="41"/>
+      <c r="E28" s="39"/>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="13" t="s">
@@ -5623,7 +5538,7 @@
       <c r="C29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="41"/>
+      <c r="E29" s="39"/>
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="13" t="s">
@@ -5635,7 +5550,7 @@
       <c r="D30" t="s">
         <v>160</v>
       </c>
-      <c r="E30" s="41"/>
+      <c r="E30" s="39"/>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="13" t="s">
@@ -5647,36 +5562,36 @@
       <c r="D31" t="s">
         <v>159</v>
       </c>
-      <c r="E31" s="41"/>
+      <c r="E31" s="39"/>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="20" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="34" spans="4:4">
       <c r="D34" s="20" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="35" spans="4:4">
       <c r="D35" s="20" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="36" spans="4:4">
       <c r="D36" s="20" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="37" spans="4:4">
       <c r="D37" s="20" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="38" spans="4:4">
       <c r="D38" s="20" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -5695,7 +5610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -5713,35 +5628,35 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
-        <v>318</v>
-      </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="C1" s="37" t="s">
+        <v>313</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
-        <v>319</v>
-      </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="C2" s="37" t="s">
+        <v>314</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="3" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -5762,7 +5677,7 @@
         <v>37</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="39" t="s">
         <v>150</v>
       </c>
     </row>
@@ -5776,7 +5691,7 @@
       <c r="D8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="41"/>
+      <c r="E8" s="39"/>
     </row>
     <row r="9" spans="1:6">
       <c r="B9" s="11" t="s">
@@ -5788,7 +5703,7 @@
       <c r="D9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="41"/>
+      <c r="E9" s="39"/>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" s="7" t="s">
@@ -5800,7 +5715,7 @@
       <c r="D10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="41"/>
+      <c r="E10" s="39"/>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" s="8" t="s">
@@ -5812,7 +5727,7 @@
       <c r="D11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="41"/>
+      <c r="E11" s="39"/>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" s="8" t="s">
@@ -5822,7 +5737,7 @@
         <v>38</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="41"/>
+      <c r="E12" s="39"/>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" s="8" t="s">
@@ -5834,7 +5749,7 @@
       <c r="D13" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="41"/>
+      <c r="E13" s="39"/>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" s="8" t="s">
@@ -5846,7 +5761,7 @@
       <c r="D14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="41"/>
+      <c r="E14" s="39"/>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="8" t="s">
@@ -5856,7 +5771,7 @@
         <v>38</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="41"/>
+      <c r="E15" s="39"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="10" t="s">
@@ -5871,7 +5786,7 @@
       <c r="D16" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E16" s="41"/>
+      <c r="E16" s="39"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="7" t="s">
@@ -5883,7 +5798,7 @@
       <c r="D17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="41"/>
+      <c r="E17" s="39"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="13" t="s">
@@ -5892,7 +5807,7 @@
       <c r="C18" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="41"/>
+      <c r="E18" s="39"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="13" t="s">
@@ -5901,11 +5816,11 @@
       <c r="C19" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="41"/>
+      <c r="E19" s="39"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="13" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>38</v>
@@ -5913,7 +5828,7 @@
       <c r="D20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="41"/>
+      <c r="E20" s="39"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="13" t="s">
@@ -5922,7 +5837,7 @@
       <c r="C21" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="41"/>
+      <c r="E21" s="39"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="13" t="s">
@@ -5931,7 +5846,7 @@
       <c r="C22" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="41"/>
+      <c r="E22" s="39"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="13" t="s">
@@ -5940,7 +5855,7 @@
       <c r="C23" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="41"/>
+      <c r="E23" s="39"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="13" t="s">
@@ -5952,34 +5867,34 @@
       <c r="D24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="41"/>
+      <c r="E24" s="39"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="13" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="41"/>
+      <c r="E25" s="39"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="13" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="41"/>
+      <c r="E26" s="39"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="13" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="41"/>
+      <c r="E27" s="39"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="13" t="s">
@@ -5988,16 +5903,16 @@
       <c r="C28" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="41"/>
+      <c r="E28" s="39"/>
     </row>
     <row r="29" spans="2:5">
-      <c r="E29" s="35"/>
+      <c r="E29" s="33"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="E30" s="35"/>
+      <c r="E30" s="33"/>
     </row>
     <row r="31" spans="2:5">
-      <c r="E31" s="35"/>
+      <c r="E31" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6015,7 +5930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -6033,31 +5948,31 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
@@ -6415,7 +6330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F27"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -6433,33 +6348,33 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
-        <v>286</v>
-      </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="C1" s="37" t="s">
+        <v>281</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
-        <v>287</v>
-      </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="C2" s="37" t="s">
+        <v>282</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -6479,7 +6394,7 @@
       <c r="C7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="39" t="s">
         <v>150</v>
       </c>
       <c r="E7" t="s">
@@ -6488,14 +6403,14 @@
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="41"/>
+      <c r="D8" s="39"/>
       <c r="E8" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -6505,7 +6420,7 @@
       <c r="C9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="41"/>
+      <c r="D9" s="39"/>
       <c r="E9" t="s">
         <v>40</v>
       </c>
@@ -6517,7 +6432,7 @@
       <c r="C10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="41"/>
+      <c r="D10" s="39"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="1" t="s">
@@ -6526,7 +6441,7 @@
       <c r="C11" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="41"/>
+      <c r="D11" s="39"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="1" t="s">
@@ -6535,7 +6450,7 @@
       <c r="C12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="41"/>
+      <c r="D12" s="39"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="2:6">
@@ -6545,7 +6460,7 @@
       <c r="C13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="41"/>
+      <c r="D13" s="39"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="1" t="s">
@@ -6554,7 +6469,7 @@
       <c r="C14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="41"/>
+      <c r="D14" s="39"/>
       <c r="E14" t="s">
         <v>45</v>
       </c>
@@ -6566,19 +6481,19 @@
       <c r="C15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="41"/>
+      <c r="D15" s="39"/>
       <c r="E15" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="21" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="41"/>
+      <c r="D16" s="39"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="14" t="s">
@@ -6587,7 +6502,7 @@
       <c r="C17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="41"/>
+      <c r="D17" s="39"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="22" t="s">
@@ -6596,34 +6511,34 @@
       <c r="C18" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="41"/>
+      <c r="D18" s="39"/>
     </row>
     <row r="19" spans="2:5">
-      <c r="B19" s="37" t="s">
-        <v>289</v>
+      <c r="B19" s="35" t="s">
+        <v>284</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="41"/>
+      <c r="D19" s="39"/>
     </row>
     <row r="20" spans="2:5">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="34" t="s">
         <v>101</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="41"/>
+      <c r="D20" s="39"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="21" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="41"/>
+      <c r="D21" s="39"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="14" t="s">
@@ -6632,55 +6547,55 @@
       <c r="C22" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="41"/>
+      <c r="D22" s="39"/>
       <c r="E22" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="23" spans="2:5">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="34" t="s">
         <v>195</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="41"/>
+      <c r="D23" s="39"/>
       <c r="E23" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="24" spans="2:5">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="34" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="41"/>
+      <c r="D24" s="39"/>
       <c r="E24" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="25" spans="2:5">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="34" t="s">
         <v>78</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="41"/>
+      <c r="D25" s="39"/>
       <c r="E25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="26" spans="2:5">
-      <c r="B26" s="36" t="s">
-        <v>272</v>
+      <c r="B26" s="34" t="s">
+        <v>270</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D26" s="41"/>
+      <c r="D26" s="39"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="1" t="s">
@@ -6689,7 +6604,7 @@
       <c r="C27" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="41"/>
+      <c r="D27" s="39"/>
       <c r="E27" t="s">
         <v>92</v>
       </c>
@@ -6708,10 +6623,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6728,256 +6643,258 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="3" t="s">
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="4"/>
+      <c r="C4" s="36" t="s">
+        <v>377</v>
+      </c>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="4"/>
+      <c r="C5" s="36" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
-      <c r="B7" t="s">
+    <row r="8" spans="2:6">
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="11" t="s">
+    <row r="9" spans="2:6">
+      <c r="B9" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="1" t="s">
+    <row r="10" spans="2:6">
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
         <v>227</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="12" t="s">
+    <row r="11" spans="2:6">
+      <c r="B11" s="12" t="s">
         <v>13</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11" s="11" t="s">
-        <v>96</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
-      <c r="B12" t="s">
+    <row r="13" spans="2:6">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="2:6">
-      <c r="B13" s="11" t="s">
-        <v>161</v>
-      </c>
       <c r="C13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>229</v>
-      </c>
-      <c r="E13" t="s">
-        <v>221</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="11" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>226</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>229</v>
+      </c>
+      <c r="E14" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="12" t="s">
-        <v>100</v>
+      <c r="B15" s="11" t="s">
+        <v>189</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D15" t="s">
+        <v>226</v>
+      </c>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6">
-      <c r="B16" t="s">
-        <v>109</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" t="s">
-        <v>233</v>
-      </c>
-      <c r="E16" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" t="s">
-        <v>195</v>
+        <v>109</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E17" t="s">
-        <v>204</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>234</v>
+      </c>
+      <c r="E18" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
         <v>214</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C19" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
         <v>236</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="B19" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="B21" t="s">
-        <v>217</v>
-      </c>
       <c r="C21" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" t="s">
+        <v>217</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" t="s">
         <v>218</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>192</v>
-      </c>
       <c r="C24" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" t="s">
-        <v>225</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -6985,58 +6902,74 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
+        <v>192</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
         <v>193</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C26" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="30"/>
-      <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="30"/>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="D28" s="6" t="s">
+      <c r="A28" s="30"/>
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="D29" s="6" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="D29" s="20" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="D30" s="20" t="s">
-        <v>230</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="D31" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="D32" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="20" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="20" t="s">
         <v>235</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
AllergyIntolerance constrained identity element
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="6" activeTab="12"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -22,21 +22,17 @@
     <sheet name="DiagnosticOrder" sheetId="12" r:id="rId8"/>
     <sheet name="DiagnosticReport" sheetId="9" r:id="rId9"/>
     <sheet name="Specimen" sheetId="13" r:id="rId10"/>
-    <sheet name="MedicationOrder" sheetId="15" r:id="rId11"/>
-    <sheet name="Encounter" sheetId="10" r:id="rId12"/>
-    <sheet name="Composition" sheetId="11" r:id="rId13"/>
+    <sheet name="MedicationAuthorization" sheetId="16" r:id="rId11"/>
+    <sheet name="MedicationOrder" sheetId="15" r:id="rId12"/>
+    <sheet name="Encounter" sheetId="10" r:id="rId13"/>
+    <sheet name="Composition" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="396">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -521,21 +517,51 @@
     <t>event.referral.referralActivity</t>
   </si>
   <si>
+    <t>PrimaryCare-MedicationRegime</t>
+  </si>
+  <si>
+    <t>MedicationStatement</t>
+  </si>
+  <si>
+    <t>informationSource</t>
+  </si>
+  <si>
+    <t>dateAsserted</t>
+  </si>
+  <si>
+    <t>wasNotTaken</t>
+  </si>
+  <si>
+    <t>reasonNotTaken</t>
+  </si>
+  <si>
+    <t>reasonForUse[x]</t>
+  </si>
+  <si>
     <t>effective[x]</t>
   </si>
   <si>
     <t>medication[x]</t>
   </si>
   <si>
+    <t>dosage</t>
+  </si>
+  <si>
     <t>event.medication.reviewDate</t>
   </si>
   <si>
     <t>event.medication.expiryDate</t>
   </si>
   <si>
+    <t>event.medication.dosage</t>
+  </si>
+  <si>
     <t>quantity</t>
   </si>
   <si>
+    <t>event.medication.quantity &amp; event.medication.quantityUnit</t>
+  </si>
+  <si>
     <t>event.medication.quantityRepresentation</t>
   </si>
   <si>
@@ -551,6 +577,9 @@
     <t>event.medication.patientText</t>
   </si>
   <si>
+    <t>event.medication.drugStatus</t>
+  </si>
+  <si>
     <t>event.medication.private</t>
   </si>
   <si>
@@ -1179,13 +1208,25 @@
   </si>
   <si>
     <t>PrimaryCare-Composition</t>
+  </si>
+  <si>
+    <t>PrimaryCare-MedicationAuthorization</t>
+  </si>
+  <si>
+    <t>certainty</t>
+  </si>
+  <si>
+    <t>manifestation</t>
+  </si>
+  <si>
+    <t>exposureRoute</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1245,6 +1286,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1286,7 +1335,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1381,6 +1430,44 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1671,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView showRowColHeaders="0" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1758,7 +1845,7 @@
     <row r="9" spans="2:6">
       <c r="B9" s="4"/>
       <c r="C9" s="36" t="s">
-        <v>375</v>
+        <v>386</v>
       </c>
       <c r="D9" s="36"/>
       <c r="E9" s="36"/>
@@ -2147,7 +2234,7 @@
         <v>6</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>37</v>
@@ -2214,7 +2301,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -2224,7 +2311,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -2234,14 +2321,14 @@
         <v>5</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
       <c r="D3" s="36"/>
       <c r="E3" s="36"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>289</v>
+        <v>300</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -2284,13 +2371,13 @@
         <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
       <c r="E9" s="39"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="21" t="s">
-        <v>290</v>
+        <v>301</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>37</v>
@@ -2312,31 +2399,31 @@
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="21" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="E12" s="39"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="21" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="E13" s="39"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="21" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>38</v>
@@ -2345,7 +2432,7 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="22" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>38</v>
@@ -2354,49 +2441,49 @@
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="22" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>311</v>
+        <v>322</v>
       </c>
       <c r="E16" s="39"/>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="22" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="E17" s="39"/>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="22" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="E18" s="39"/>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" s="22" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
       <c r="E19" s="39"/>
     </row>
@@ -2408,7 +2495,7 @@
         <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
       <c r="E20" s="39"/>
     </row>
@@ -2417,19 +2504,19 @@
         <v>6</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>376</v>
+        <v>387</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="E21" s="39"/>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="21" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>37</v>
@@ -2447,7 +2534,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="22" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>38</v>
@@ -2456,7 +2543,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="B25" s="22" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>37</v>
@@ -2465,7 +2552,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="B26" s="21" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>37</v>
@@ -2502,7 +2589,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="22" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>38</v>
@@ -2511,7 +2598,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="22" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>38</v>
@@ -2520,7 +2607,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="22" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>38</v>
@@ -2547,10 +2634,454 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E48"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="4.625" customWidth="1"/>
+    <col min="2" max="2" width="28.625" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="61.125" customWidth="1"/>
+    <col min="5" max="5" width="28.875" customWidth="1"/>
+    <col min="6" max="6" width="41.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5">
+      <c r="B1" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+    </row>
+    <row r="2" spans="2:5">
+      <c r="B2" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="46"/>
+      <c r="E7" s="39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="39"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="39"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="39"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" s="39"/>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="49"/>
+      <c r="E12" s="39"/>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="44"/>
+      <c r="E13" s="39"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="44"/>
+      <c r="E14" s="39"/>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="44"/>
+      <c r="E15" s="39"/>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="39"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="44"/>
+      <c r="B17" s="44" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="44"/>
+      <c r="E17" s="39"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="44"/>
+      <c r="B18" s="52" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="39"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="44"/>
+      <c r="B19" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="E19" s="39"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="E20" s="39"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>344</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="E21" s="59"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>345</v>
+      </c>
+      <c r="C22" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="44"/>
+      <c r="E22" s="59"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="43" t="s">
+        <v>346</v>
+      </c>
+      <c r="C23" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="44"/>
+      <c r="E23" s="59"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" s="44"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="59"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="E25" s="59"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="E26" s="59"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="55" t="s">
+        <v>176</v>
+      </c>
+      <c r="E27" s="59"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="E28" s="59"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44" t="s">
+        <v>178</v>
+      </c>
+      <c r="E29" s="59"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="E30" s="59"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" s="59"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="E32" s="59"/>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="E33" s="59"/>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="E34" s="59"/>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="D35" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="E35" s="59"/>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="D36" s="44" t="s">
+        <v>186</v>
+      </c>
+      <c r="E36" s="59"/>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="D37" s="44" t="s">
+        <v>187</v>
+      </c>
+      <c r="E37" s="59"/>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="D38" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="E38" s="59"/>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="D39" s="57" t="s">
+        <v>189</v>
+      </c>
+      <c r="E39" s="59"/>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="D40" s="57" t="s">
+        <v>157</v>
+      </c>
+      <c r="E40" s="59"/>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="D41" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="E41" s="59"/>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="D42" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="E42" s="59"/>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="D43" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="E43" s="44"/>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="D44" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="E44" s="44"/>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="D45" s="57" t="s">
+        <v>194</v>
+      </c>
+      <c r="E45" s="44"/>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="D46" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="E46" s="44"/>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="D47" s="57" t="s">
+        <v>196</v>
+      </c>
+      <c r="E47" s="44"/>
+    </row>
+    <row r="48" spans="2:5">
+      <c r="D48" s="57" t="s">
+        <v>197</v>
+      </c>
+      <c r="E48" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E7:E20"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F83"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59:D83"/>
+    <sheetView showRowColHeaders="0" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2568,7 +3099,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -2578,7 +3109,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>319</v>
+        <v>330</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -2595,7 +3126,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -2617,12 +3148,12 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s">
-        <v>338</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="1" t="s">
-        <v>320</v>
+        <v>331</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>38</v>
@@ -2631,7 +3162,7 @@
         <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -2648,19 +3179,19 @@
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="1" t="s">
-        <v>321</v>
+        <v>332</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" t="s">
-        <v>345</v>
+        <v>356</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="1" t="s">
-        <v>322</v>
+        <v>333</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>38</v>
@@ -2681,7 +3212,7 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="11" t="s">
-        <v>323</v>
+        <v>334</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>36</v>
@@ -2690,7 +3221,7 @@
         <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14" spans="2:6">
@@ -2727,7 +3258,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="11" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>36</v>
@@ -2736,19 +3267,19 @@
         <v>50</v>
       </c>
       <c r="E17" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="1" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" t="s">
-        <v>348</v>
+        <v>359</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2759,13 +3290,13 @@
         <v>38</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="30"/>
       <c r="B20" s="34" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>38</v>
@@ -2774,7 +3305,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="34" t="s">
-        <v>326</v>
+        <v>337</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
@@ -2783,7 +3314,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="34" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>38</v>
@@ -2792,7 +3323,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="B23" s="34" t="s">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>38</v>
@@ -2801,7 +3332,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="34" t="s">
-        <v>328</v>
+        <v>339</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>38</v>
@@ -2810,7 +3341,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="B25" s="34" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>38</v>
@@ -2819,7 +3350,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="B26" s="34" t="s">
-        <v>329</v>
+        <v>340</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>38</v>
@@ -2827,7 +3358,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="B27" s="34" t="s">
-        <v>330</v>
+        <v>341</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>38</v>
@@ -2836,7 +3367,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="34" t="s">
-        <v>331</v>
+        <v>342</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>38</v>
@@ -2845,7 +3376,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="1" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>38</v>
@@ -2854,7 +3385,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="34" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>38</v>
@@ -2863,7 +3394,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="34" t="s">
-        <v>333</v>
+        <v>344</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>38</v>
@@ -2872,7 +3403,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="34" t="s">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>38</v>
@@ -2881,21 +3412,21 @@
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="34" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
       <c r="E33" t="s">
-        <v>346</v>
+        <v>357</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="34" t="s">
-        <v>335</v>
+        <v>346</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>38</v>
@@ -2904,7 +3435,7 @@
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="1" t="s">
-        <v>336</v>
+        <v>347</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>38</v>
@@ -2932,7 +3463,7 @@
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="1" t="s">
-        <v>337</v>
+        <v>348</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>38</v>
@@ -2945,228 +3476,127 @@
     </row>
     <row r="40" spans="2:5">
       <c r="D40" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="E40" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="D41" s="28" t="s">
-        <v>352</v>
+        <v>363</v>
       </c>
       <c r="E41" t="s">
-        <v>342</v>
+        <v>353</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="D42" s="28" t="s">
-        <v>353</v>
+        <v>364</v>
       </c>
       <c r="E42" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="D43" s="28" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
       <c r="E43" t="s">
-        <v>344</v>
+        <v>355</v>
       </c>
     </row>
     <row r="44" spans="2:5">
       <c r="D44" s="28" t="s">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="E44" t="s">
-        <v>347</v>
+        <v>358</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="D45" s="28" t="s">
-        <v>356</v>
+        <v>367</v>
       </c>
     </row>
     <row r="46" spans="2:5">
       <c r="D46" s="28" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
     </row>
     <row r="47" spans="2:5">
       <c r="D47" s="28" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
     </row>
     <row r="48" spans="2:5">
       <c r="D48" s="28" t="s">
-        <v>359</v>
+        <v>370</v>
       </c>
     </row>
     <row r="49" spans="4:4">
       <c r="D49" s="28" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
     </row>
     <row r="50" spans="4:4">
       <c r="D50" s="28" t="s">
-        <v>361</v>
+        <v>372</v>
       </c>
     </row>
     <row r="51" spans="4:4">
       <c r="D51" s="28" t="s">
-        <v>362</v>
+        <v>373</v>
       </c>
     </row>
     <row r="52" spans="4:4">
       <c r="D52" s="28" t="s">
-        <v>363</v>
+        <v>374</v>
       </c>
     </row>
     <row r="53" spans="4:4">
       <c r="D53" s="28" t="s">
-        <v>364</v>
+        <v>375</v>
       </c>
     </row>
     <row r="54" spans="4:4">
       <c r="D54" s="28" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
     </row>
     <row r="55" spans="4:4">
       <c r="D55" s="28" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
     </row>
     <row r="56" spans="4:4">
       <c r="D56" s="28" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="59" spans="4:4">
-      <c r="D59" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="60" spans="4:4">
-      <c r="D60" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="61" spans="4:4">
-      <c r="D61" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="62" spans="4:4">
-      <c r="D62" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="63" spans="4:4">
-      <c r="D63" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="64" spans="4:4">
-      <c r="D64" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="65" spans="4:4">
-      <c r="D65" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="66" spans="4:4">
-      <c r="D66" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="67" spans="4:4">
-      <c r="D67" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="68" spans="4:4">
-      <c r="D68" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="69" spans="4:4">
-      <c r="D69" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="70" spans="4:4">
-      <c r="D70" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="71" spans="4:4">
-      <c r="D71" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="72" spans="4:4">
-      <c r="D72" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="73" spans="4:4">
-      <c r="D73" t="s">
-        <v>177</v>
+        <v>378</v>
       </c>
     </row>
     <row r="74" spans="4:4">
-      <c r="D74" s="27" t="s">
-        <v>178</v>
-      </c>
+      <c r="D74" s="27"/>
     </row>
     <row r="75" spans="4:4">
-      <c r="D75" s="27" t="s">
-        <v>157</v>
-      </c>
+      <c r="D75" s="27"/>
     </row>
     <row r="76" spans="4:4">
-      <c r="D76" s="27" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="77" spans="4:4">
-      <c r="D77" t="s">
-        <v>180</v>
-      </c>
+      <c r="D76" s="27"/>
     </row>
     <row r="78" spans="4:4">
-      <c r="D78" s="28" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="79" spans="4:4">
-      <c r="D79" t="s">
-        <v>182</v>
-      </c>
+      <c r="D78" s="28"/>
     </row>
     <row r="80" spans="4:4">
-      <c r="D80" s="27" t="s">
-        <v>183</v>
-      </c>
+      <c r="D80" s="27"/>
     </row>
     <row r="81" spans="4:4">
-      <c r="D81" s="27" t="s">
-        <v>184</v>
-      </c>
+      <c r="D81" s="27"/>
     </row>
     <row r="82" spans="4:4">
-      <c r="D82" s="27" t="s">
-        <v>185</v>
-      </c>
+      <c r="D82" s="27"/>
     </row>
     <row r="83" spans="4:4">
-      <c r="D83" s="27" t="s">
-        <v>186</v>
-      </c>
+      <c r="D83" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3179,7 +3609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
@@ -3202,7 +3632,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -3212,7 +3642,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -3227,7 +3657,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -3266,7 +3696,7 @@
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="20" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>39</v>
@@ -3275,7 +3705,7 @@
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>38</v>
@@ -3290,10 +3720,10 @@
         <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="E11" t="s">
-        <v>252</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -3313,7 +3743,7 @@
         <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="E13" t="s">
         <v>41</v>
@@ -3321,7 +3751,7 @@
     </row>
     <row r="14" spans="2:6">
       <c r="B14" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>38</v>
@@ -3331,7 +3761,7 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="21" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>37</v>
@@ -3340,13 +3770,13 @@
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="5" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -3359,12 +3789,12 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="7" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>38</v>
@@ -3374,21 +3804,21 @@
     </row>
     <row r="19" spans="1:5">
       <c r="B19" s="22" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="E19" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="21" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>38</v>
@@ -3397,27 +3827,27 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="13" t="s">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="E21" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="13" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="E22" s="2"/>
     </row>
@@ -3429,13 +3859,13 @@
         <v>37</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="13" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>37</v>
@@ -3445,7 +3875,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="B25" s="16" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>39</v>
@@ -3461,7 +3891,7 @@
         <v>37</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="E26" t="s">
         <v>116</v>
@@ -3470,19 +3900,19 @@
     <row r="27" spans="1:5">
       <c r="A27" s="30"/>
       <c r="B27" s="13" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="16" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>39</v>
@@ -3509,12 +3939,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F33"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3532,7 +3962,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -3542,7 +3972,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>264</v>
+        <v>275</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -3557,7 +3987,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>380</v>
+        <v>391</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -3590,7 +4020,7 @@
         <v>36</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>257</v>
+        <v>268</v>
       </c>
       <c r="E8" s="39"/>
     </row>
@@ -3605,17 +4035,17 @@
       <c r="E9" s="39"/>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="1" t="s">
-        <v>240</v>
+      <c r="B10" s="20" t="s">
+        <v>251</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E10" s="39"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="11" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>36</v>
@@ -3633,7 +4063,7 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="20" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>39</v>
@@ -3648,25 +4078,25 @@
         <v>36</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="E14" s="39"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="11" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>130</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>276</v>
+        <v>287</v>
       </c>
       <c r="E15" s="39"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="1" t="s">
-        <v>268</v>
+        <v>279</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>37</v>
@@ -3675,7 +4105,7 @@
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="1" t="s">
-        <v>269</v>
+        <v>280</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>38</v>
@@ -3684,7 +4114,7 @@
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="1" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>37</v>
@@ -3705,7 +4135,7 @@
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>37</v>
@@ -3714,13 +4144,13 @@
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="27" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>277</v>
+        <v>288</v>
       </c>
       <c r="E21" s="39"/>
     </row>
@@ -3735,7 +4165,7 @@
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="34" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>38</v>
@@ -3744,7 +4174,7 @@
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="27" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>38</v>
@@ -3753,7 +4183,7 @@
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="27" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>37</v>
@@ -3762,7 +4192,7 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="34" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>38</v>
@@ -3771,7 +4201,7 @@
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="27" t="s">
-        <v>271</v>
+        <v>282</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>37</v>
@@ -3780,13 +4210,13 @@
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="31" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="C28" s="32" t="s">
         <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
       <c r="E28" s="39"/>
     </row>
@@ -3798,13 +4228,13 @@
         <v>38</v>
       </c>
       <c r="D29" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
       <c r="E29" s="39"/>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="42" t="s">
-        <v>272</v>
+        <v>283</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>38</v>
@@ -3813,7 +4243,7 @@
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="31" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="C31" s="32" t="s">
         <v>38</v>
@@ -3822,19 +4252,19 @@
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="31" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="C32" s="32" t="s">
         <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="E32" s="39"/>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="42" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>38</v>
@@ -3855,10 +4285,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4206,14 +4636,78 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="10" t="s">
+    <row r="33" spans="1:3" s="44" customFormat="1">
+      <c r="B33" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" s="50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="44" customFormat="1">
+      <c r="B34" s="56" t="s">
+        <v>393</v>
+      </c>
+      <c r="C34" s="50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="44" customFormat="1">
+      <c r="B35" s="53" t="s">
+        <v>394</v>
+      </c>
+      <c r="C35" s="54" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="44" customFormat="1">
+      <c r="B36" s="56" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36" s="50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="44" customFormat="1">
+      <c r="B37" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="44" customFormat="1">
+      <c r="B38" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="44" customFormat="1">
+      <c r="B39" s="56" t="s">
+        <v>395</v>
+      </c>
+      <c r="C39" s="50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="44" customFormat="1">
+      <c r="B40" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="50" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B41" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C41" s="9" t="s">
         <v>38</v>
       </c>
     </row>
@@ -4225,7 +4719,7 @@
     <mergeCell ref="C3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4233,8 +4727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView showRowColHeaders="0" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4571,11 +5065,11 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>39</v>
+      <c r="C32" s="50" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -4678,7 +5172,7 @@
     <mergeCell ref="C4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4686,7 +5180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -5212,7 +5706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
@@ -5566,32 +6060,32 @@
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="20" t="s">
-        <v>369</v>
+        <v>380</v>
       </c>
     </row>
     <row r="34" spans="4:4">
       <c r="D34" s="20" t="s">
-        <v>370</v>
+        <v>381</v>
       </c>
     </row>
     <row r="35" spans="4:4">
       <c r="D35" s="20" t="s">
-        <v>371</v>
+        <v>382</v>
       </c>
     </row>
     <row r="36" spans="4:4">
       <c r="D36" s="20" t="s">
-        <v>372</v>
+        <v>383</v>
       </c>
     </row>
     <row r="37" spans="4:4">
       <c r="D37" s="20" t="s">
-        <v>373</v>
+        <v>384</v>
       </c>
     </row>
     <row r="38" spans="4:4">
       <c r="D38" s="20" t="s">
-        <v>374</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -5629,7 +6123,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -5639,7 +6133,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -5656,7 +6150,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="3" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -5820,7 +6314,7 @@
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="13" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>38</v>
@@ -5871,7 +6365,7 @@
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="13" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>38</v>
@@ -5880,7 +6374,7 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="13" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>38</v>
@@ -5889,7 +6383,7 @@
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="13" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>38</v>
@@ -5949,7 +6443,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -5959,7 +6453,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -5976,7 +6470,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>187</v>
+        <v>198</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -6033,7 +6527,7 @@
         <v>50</v>
       </c>
       <c r="E10" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="2:6">
@@ -6157,7 +6651,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
@@ -6166,12 +6660,12 @@
         <v>47</v>
       </c>
       <c r="E21" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>38</v>
@@ -6197,21 +6691,21 @@
     </row>
     <row r="24" spans="1:5">
       <c r="B24" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>206</v>
+        <v>217</v>
       </c>
       <c r="E24" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="B25" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>38</v>
@@ -6221,18 +6715,18 @@
     </row>
     <row r="26" spans="1:5">
       <c r="B26" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="B27" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>38</v>
@@ -6249,12 +6743,12 @@
         <v>38</v>
       </c>
       <c r="E28" t="s">
-        <v>203</v>
+        <v>214</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>38</v>
@@ -6262,18 +6756,18 @@
     </row>
     <row r="30" spans="1:5">
       <c r="B30" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>38</v>
@@ -6281,38 +6775,38 @@
     </row>
     <row r="32" spans="1:5">
       <c r="B32" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D33" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="E34" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -6349,7 +6843,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -6359,7 +6853,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -6374,7 +6868,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -6403,14 +6897,14 @@
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="1" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="39"/>
       <c r="E8" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -6455,7 +6949,7 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="1" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>37</v>
@@ -6483,12 +6977,12 @@
       </c>
       <c r="D15" s="39"/>
       <c r="E15" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="21" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>37</v>
@@ -6515,7 +7009,7 @@
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="35" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>36</v>
@@ -6533,7 +7027,7 @@
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="21" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>38</v>
@@ -6549,19 +7043,19 @@
       </c>
       <c r="D22" s="39"/>
       <c r="E22" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="34" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="39"/>
       <c r="E23" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="2:5">
@@ -6590,7 +7084,7 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="34" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>37</v>
@@ -6644,7 +7138,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -6654,7 +7148,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -6672,7 +7166,7 @@
     <row r="4" spans="2:6">
       <c r="B4" s="4"/>
       <c r="C4" s="36" t="s">
-        <v>377</v>
+        <v>388</v>
       </c>
       <c r="D4" s="36"/>
       <c r="E4" s="36"/>
@@ -6680,14 +7174,14 @@
     <row r="5" spans="2:6">
       <c r="B5" s="4"/>
       <c r="C5" s="36" t="s">
-        <v>378</v>
+        <v>389</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="36"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="3" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
@@ -6708,7 +7202,7 @@
         <v>37</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
@@ -6734,7 +7228,7 @@
         <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="E10" t="s">
         <v>43</v>
@@ -6751,7 +7245,7 @@
         <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -6780,27 +7274,27 @@
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="11" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="E14" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="11" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -6812,7 +7306,7 @@
         <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -6823,43 +7317,43 @@
         <v>37</v>
       </c>
       <c r="D17" t="s">
+        <v>244</v>
+      </c>
+      <c r="E17" t="s">
         <v>233</v>
-      </c>
-      <c r="E17" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="E18" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="E19" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="1" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>37</v>
@@ -6867,7 +7361,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="1" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>37</v>
@@ -6875,7 +7369,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="B22" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>38</v>
@@ -6883,7 +7377,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="B23" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>37</v>
@@ -6891,7 +7385,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="1" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>37</v>
@@ -6902,13 +7396,13 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -6916,7 +7410,7 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>37</v>
@@ -6945,22 +7439,22 @@
     </row>
     <row r="31" spans="1:5">
       <c r="D31" s="20" t="s">
-        <v>230</v>
+        <v>241</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="D32" s="20" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="20" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
     </row>
     <row r="34" spans="4:4">
       <c r="D34" s="20" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ProcedureRequest constrained identity and notes element
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" activeTab="1"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="397">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -1220,6 +1220,9 @@
   </si>
   <si>
     <t>exposureRoute</t>
+  </si>
+  <si>
+    <t>OpenHR (Diary Event Type)</t>
   </si>
 </sst>
 </file>
@@ -4287,7 +4290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -4727,7 +4730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
@@ -5180,7 +5183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -6104,8 +6107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6154,7 +6157,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>1</v>
+        <v>396</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Diagnostic Report constrained identity element
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" activeTab="1"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -2191,10 +2191,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:E3"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2498,36 +2498,32 @@
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="30"/>
-      <c r="C28" s="9"/>
+      <c r="D28" s="6" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="D29" s="6" t="s">
-        <v>46</v>
+      <c r="D29" s="20" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="D30" s="20" t="s">
-        <v>48</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="D31" s="20" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="D32" s="20" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="20" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4">
-      <c r="D34" s="20" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4553,7 +4549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C6" sqref="C6:E6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
authorization -> authorisation + Resource map
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="6" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="DiagnosticOrder" sheetId="12" r:id="rId9"/>
     <sheet name="DiagnosticReport" sheetId="9" r:id="rId10"/>
     <sheet name="Specimen" sheetId="13" r:id="rId11"/>
-    <sheet name="MedicationAuthorization" sheetId="16" r:id="rId12"/>
+    <sheet name="MedicationAuthorisation" sheetId="16" r:id="rId12"/>
     <sheet name="MedicationOrder" sheetId="15" r:id="rId13"/>
     <sheet name="Encounter" sheetId="10" r:id="rId14"/>
     <sheet name="Composition" sheetId="11" r:id="rId15"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="409">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -488,9 +488,6 @@
     <t>event.referral.UBRN</t>
   </si>
   <si>
-    <t>authorisingUserInRole</t>
-  </si>
-  <si>
     <t>event.authorisingUserInRole /  event.referral.sourceOrganisation</t>
   </si>
   <si>
@@ -500,9 +497,6 @@
     <t>event.referral.referralActivity</t>
   </si>
   <si>
-    <t>PrimaryCare-MedicationRegime</t>
-  </si>
-  <si>
     <t>MedicationStatement</t>
   </si>
   <si>
@@ -581,15 +575,6 @@
     <t>event.medication.numberOfIssues</t>
   </si>
   <si>
-    <t>event.medication.authorisedIssues</t>
-  </si>
-  <si>
-    <t>authorisedDate</t>
-  </si>
-  <si>
-    <t>authorisedIssues</t>
-  </si>
-  <si>
     <t>event.medication.mostRecentIssueMethod</t>
   </si>
   <si>
@@ -599,18 +584,6 @@
     <t>event.medication.cancellation</t>
   </si>
   <si>
-    <t>cancelledByUserInRole</t>
-  </si>
-  <si>
-    <t>cancellationDateTime</t>
-  </si>
-  <si>
-    <t>cancellationText</t>
-  </si>
-  <si>
-    <t>linkedEvent</t>
-  </si>
-  <si>
     <t>PrimaryCare-Observation</t>
   </si>
   <si>
@@ -1151,9 +1124,6 @@
     <t>event.medicationIssue.repeatDispensingIssueCount</t>
   </si>
   <si>
-    <t>event.medicationIssue.batchNumber</t>
-  </si>
-  <si>
     <t>event.medicationIssue.quantity &amp; quantityUnit</t>
   </si>
   <si>
@@ -1190,9 +1160,6 @@
     <t>PrimaryCare-Composition</t>
   </si>
   <si>
-    <t>PrimaryCare-MedicationAuthorization</t>
-  </si>
-  <si>
     <t>certainty</t>
   </si>
   <si>
@@ -1239,6 +1206,60 @@
   </si>
   <si>
     <t>primarycare-problem-related-extension</t>
+  </si>
+  <si>
+    <t>event.effectiveTime + event.medication.durationOfIssue</t>
+  </si>
+  <si>
+    <t>event.medication.authorisedIssues.authorisedIssues</t>
+  </si>
+  <si>
+    <t>pharmacyText</t>
+  </si>
+  <si>
+    <t>patientText</t>
+  </si>
+  <si>
+    <t>private</t>
+  </si>
+  <si>
+    <t>firstIssueDate</t>
+  </si>
+  <si>
+    <t>mostRecentIssueDate</t>
+  </si>
+  <si>
+    <t>prescribedAsContraception</t>
+  </si>
+  <si>
+    <t>cancellation</t>
+  </si>
+  <si>
+    <t>event.medication.cancellation.cancelledByUserInRole</t>
+  </si>
+  <si>
+    <t>event.medication.cancellation.cancellationDateTime</t>
+  </si>
+  <si>
+    <t>event.medication.cancellation.cancellationText</t>
+  </si>
+  <si>
+    <t>PrimaryCare-MedicationAuthorisation</t>
+  </si>
+  <si>
+    <t>numberOfRepeatsIssued</t>
+  </si>
+  <si>
+    <t>authorisation</t>
+  </si>
+  <si>
+    <t>event.code (use Medication resource when recording event.medicationIssue.batchNumber)</t>
+  </si>
+  <si>
+    <t>estimatedNHSCost</t>
+  </si>
+  <si>
+    <t>prescribedAsContraceptive</t>
   </si>
 </sst>
 </file>
@@ -1354,7 +1375,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1491,14 +1512,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1834,11 +1864,11 @@
     </row>
     <row r="4" spans="2:6" s="43" customFormat="1">
       <c r="B4" s="47"/>
-      <c r="C4" s="67" t="s">
-        <v>396</v>
-      </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
+      <c r="C4" s="69" t="s">
+        <v>385</v>
+      </c>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
@@ -2141,7 +2171,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="48" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="C31" s="52" t="s">
         <v>37</v>
@@ -2153,25 +2183,25 @@
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="56" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="C32" s="52" t="s">
         <v>35</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="56" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="C33" s="52" t="s">
         <v>35</v>
       </c>
       <c r="D33" s="48" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="E33" s="2"/>
     </row>
@@ -2193,7 +2223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
@@ -2212,7 +2242,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -2222,7 +2252,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -2240,7 +2270,7 @@
     <row r="4" spans="2:6">
       <c r="B4" s="4"/>
       <c r="C4" s="36" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="D4" s="36"/>
       <c r="E4" s="36"/>
@@ -2248,14 +2278,14 @@
     <row r="5" spans="2:6">
       <c r="B5" s="4"/>
       <c r="C5" s="36" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="36"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="3" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
@@ -2276,7 +2306,7 @@
         <v>36</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="E8" t="s">
         <v>39</v>
@@ -2302,7 +2332,7 @@
         <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="E10" t="s">
         <v>42</v>
@@ -2319,7 +2349,7 @@
         <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -2348,27 +2378,27 @@
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="E14" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="11" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -2380,7 +2410,7 @@
         <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2391,43 +2421,43 @@
         <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="E17" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
+        <v>191</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>230</v>
+      </c>
+      <c r="E18" t="s">
         <v>200</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" t="s">
-        <v>239</v>
-      </c>
-      <c r="E18" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" t="s">
+        <v>210</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>232</v>
+      </c>
+      <c r="E19" t="s">
         <v>219</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" t="s">
-        <v>241</v>
-      </c>
-      <c r="E19" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="1" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>36</v>
@@ -2435,7 +2465,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="1" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>36</v>
@@ -2443,7 +2473,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="B22" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>37</v>
@@ -2451,7 +2481,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="B23" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>36</v>
@@ -2459,7 +2489,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="1" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>36</v>
@@ -2470,13 +2500,13 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2484,7 +2514,7 @@
         <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>36</v>
@@ -2509,22 +2539,22 @@
     </row>
     <row r="30" spans="1:5">
       <c r="D30" s="20" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="D31" s="20" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="D32" s="20" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="20" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2563,7 +2593,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -2573,7 +2603,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -2583,14 +2613,14 @@
         <v>5</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="D3" s="36"/>
       <c r="E3" s="36"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -2633,13 +2663,13 @@
         <v>37</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="E9" s="39"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="21" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>36</v>
@@ -2661,31 +2691,31 @@
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="21" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="E12" s="39"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="21" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E13" s="39"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="21" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>37</v>
@@ -2694,7 +2724,7 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="22" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>37</v>
@@ -2703,49 +2733,49 @@
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="22" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="E16" s="39"/>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="22" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="E17" s="39"/>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="E18" s="39"/>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" s="22" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="E19" s="39"/>
     </row>
@@ -2757,7 +2787,7 @@
         <v>37</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="E20" s="39"/>
     </row>
@@ -2766,19 +2796,19 @@
         <v>6</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="E21" s="39"/>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="21" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>36</v>
@@ -2796,7 +2826,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="22" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>37</v>
@@ -2805,7 +2835,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="B25" s="22" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>36</v>
@@ -2814,7 +2844,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="B26" s="21" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>36</v>
@@ -2851,7 +2881,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="22" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>37</v>
@@ -2860,7 +2890,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="22" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>37</v>
@@ -2869,7 +2899,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="22" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>37</v>
@@ -2896,10 +2926,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2917,7 +2947,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>385</v>
+        <v>403</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -2927,7 +2957,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -2944,7 +2974,7 @@
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="46" t="s">
-        <v>155</v>
+        <v>403</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="46" t="s">
@@ -2954,7 +2984,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" ht="15.75" customHeight="1">
       <c r="B7" s="43" t="s">
         <v>8</v>
       </c>
@@ -2980,7 +3010,7 @@
     </row>
     <row r="9" spans="2:5">
       <c r="B9" s="54" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C9" s="52" t="s">
         <v>35</v>
@@ -2992,7 +3022,7 @@
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="44" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C10" s="52" t="s">
         <v>37</v>
@@ -3010,13 +3040,13 @@
         <v>35</v>
       </c>
       <c r="D11" s="43" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E11" s="39"/>
     </row>
     <row r="12" spans="2:5">
       <c r="B12" s="43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C12" s="52" t="s">
         <v>37</v>
@@ -3026,7 +3056,7 @@
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C13" s="52" t="s">
         <v>36</v>
@@ -3036,7 +3066,7 @@
     </row>
     <row r="14" spans="2:5">
       <c r="B14" s="43" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C14" s="52" t="s">
         <v>37</v>
@@ -3046,12 +3076,14 @@
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="43" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C15" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="43"/>
+      <c r="D15" s="48" t="s">
+        <v>391</v>
+      </c>
       <c r="E15" s="39"/>
     </row>
     <row r="16" spans="2:5">
@@ -3080,7 +3112,7 @@
     <row r="18" spans="1:5">
       <c r="A18" s="43"/>
       <c r="B18" s="54" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C18" s="52" t="s">
         <v>35</v>
@@ -3093,13 +3125,13 @@
     <row r="19" spans="1:5">
       <c r="A19" s="43"/>
       <c r="B19" s="43" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C19" s="52" t="s">
         <v>36</v>
       </c>
       <c r="D19" s="43" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E19" s="39"/>
     </row>
@@ -3107,14 +3139,14 @@
       <c r="A20" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="54" t="s">
-        <v>168</v>
+      <c r="B20" s="44" t="s">
+        <v>166</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D20" s="43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E20" s="39"/>
     </row>
@@ -3123,212 +3155,259 @@
         <v>6</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C21" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="43" t="s">
-        <v>166</v>
-      </c>
-      <c r="E21" s="64"/>
+      <c r="D21" s="44" t="s">
+        <v>392</v>
+      </c>
+      <c r="E21" s="39"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="53" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="C22" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="43"/>
-      <c r="E22" s="64"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="D22" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="E22" s="39"/>
+    </row>
+    <row r="23" spans="1:5" s="43" customFormat="1">
       <c r="A23" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="42" t="s">
-        <v>340</v>
+      <c r="B23" s="43" t="s">
+        <v>393</v>
       </c>
       <c r="C23" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="43"/>
-      <c r="E23" s="64"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="B24" s="43"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="64"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" s="43"/>
-      <c r="C25" s="43"/>
-      <c r="E25" s="64"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
+      <c r="D23" s="43" t="s">
+        <v>171</v>
+      </c>
+      <c r="E23" s="39"/>
+    </row>
+    <row r="24" spans="1:5" s="43" customFormat="1">
+      <c r="A24" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="43" t="s">
+        <v>394</v>
+      </c>
+      <c r="C24" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="E24" s="39"/>
+    </row>
+    <row r="25" spans="1:5" s="43" customFormat="1">
+      <c r="A25" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="43" t="s">
+        <v>395</v>
+      </c>
+      <c r="C25" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="43" t="s">
+        <v>174</v>
+      </c>
+      <c r="E25" s="39"/>
+    </row>
+    <row r="26" spans="1:5" s="43" customFormat="1">
+      <c r="A26" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="43" t="s">
+        <v>396</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>37</v>
+      </c>
       <c r="D26" s="43" t="s">
-        <v>165</v>
-      </c>
-      <c r="E26" s="64"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="59" t="s">
+        <v>177</v>
+      </c>
+      <c r="E26" s="39"/>
+    </row>
+    <row r="27" spans="1:5" s="43" customFormat="1">
+      <c r="A27" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="43" t="s">
+        <v>397</v>
+      </c>
+      <c r="C27" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="E27" s="39"/>
+    </row>
+    <row r="28" spans="1:5" s="43" customFormat="1">
+      <c r="A28" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>404</v>
+      </c>
+      <c r="C28" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="E28" s="39"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="63" t="s">
+        <v>398</v>
+      </c>
+      <c r="C29" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="63" t="s">
+        <v>181</v>
+      </c>
+      <c r="E29" s="39"/>
+    </row>
+    <row r="30" spans="1:5" s="43" customFormat="1">
+      <c r="A30" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="43" t="s">
+        <v>399</v>
+      </c>
+      <c r="C30" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="E30" s="39"/>
+    </row>
+    <row r="31" spans="1:5" s="43" customFormat="1">
+      <c r="A31" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="63" t="s">
+        <v>400</v>
+      </c>
+      <c r="E31" s="39"/>
+    </row>
+    <row r="32" spans="1:5" s="43" customFormat="1">
+      <c r="A32" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="63" t="s">
+        <v>401</v>
+      </c>
+      <c r="E32" s="39"/>
+    </row>
+    <row r="33" spans="1:5" s="43" customFormat="1">
+      <c r="A33" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="63" t="s">
+        <v>402</v>
+      </c>
+      <c r="E33" s="39"/>
+    </row>
+    <row r="34" spans="1:5" s="43" customFormat="1">
+      <c r="B34" s="63"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="65"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="B35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="65"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="E36" s="65"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="B37" s="43"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="E37" s="65"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="B38" s="43"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="59" t="s">
         <v>170</v>
       </c>
-      <c r="E27" s="64"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43" t="s">
-        <v>171</v>
-      </c>
-      <c r="E28" s="64"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43" t="s">
-        <v>172</v>
-      </c>
-      <c r="E29" s="64"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" s="43"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43" t="s">
-        <v>173</v>
-      </c>
-      <c r="E30" s="64"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43" t="s">
-        <v>174</v>
-      </c>
-      <c r="E31" s="64"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43" t="s">
+      <c r="E38" s="65"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="B39" s="43"/>
+      <c r="C39" s="43"/>
+      <c r="D39" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="E39" s="65"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="E32" s="64"/>
-    </row>
-    <row r="33" spans="2:5">
-      <c r="B33" s="43"/>
-      <c r="C33" s="43"/>
-      <c r="D33" s="43" t="s">
-        <v>177</v>
-      </c>
-      <c r="E33" s="64"/>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="43"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43" t="s">
-        <v>178</v>
-      </c>
-      <c r="E34" s="64"/>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="D35" s="43" t="s">
-        <v>179</v>
-      </c>
-      <c r="E35" s="64"/>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="D36" s="43" t="s">
+      <c r="E40" s="65"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="D41" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="E36" s="64"/>
-    </row>
-    <row r="37" spans="2:5">
-      <c r="D37" s="43" t="s">
-        <v>181</v>
-      </c>
-      <c r="E37" s="64"/>
-    </row>
-    <row r="38" spans="2:5">
-      <c r="D38" s="43" t="s">
-        <v>182</v>
-      </c>
-      <c r="E38" s="64"/>
-    </row>
-    <row r="39" spans="2:5">
-      <c r="D39" s="62" t="s">
-        <v>183</v>
-      </c>
-      <c r="E39" s="64"/>
-    </row>
-    <row r="40" spans="2:5">
-      <c r="D40" s="62" t="s">
-        <v>151</v>
-      </c>
-      <c r="E40" s="64"/>
-    </row>
-    <row r="41" spans="2:5">
-      <c r="D41" s="62" t="s">
-        <v>184</v>
-      </c>
-      <c r="E41" s="64"/>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="D42" s="43" t="s">
-        <v>185</v>
-      </c>
-      <c r="E42" s="64"/>
-    </row>
-    <row r="43" spans="2:5">
-      <c r="D43" s="63" t="s">
-        <v>186</v>
-      </c>
-      <c r="E43" s="43"/>
-    </row>
-    <row r="44" spans="2:5">
-      <c r="D44" s="43" t="s">
-        <v>187</v>
-      </c>
-      <c r="E44" s="43"/>
-    </row>
-    <row r="45" spans="2:5">
-      <c r="D45" s="62" t="s">
-        <v>188</v>
-      </c>
-      <c r="E45" s="43"/>
-    </row>
-    <row r="46" spans="2:5">
-      <c r="D46" s="62" t="s">
-        <v>189</v>
-      </c>
-      <c r="E46" s="43"/>
-    </row>
-    <row r="47" spans="2:5">
-      <c r="D47" s="62" t="s">
-        <v>190</v>
-      </c>
-      <c r="E47" s="43"/>
-    </row>
-    <row r="48" spans="2:5">
-      <c r="D48" s="62" t="s">
-        <v>191</v>
-      </c>
-      <c r="E48" s="43"/>
+      <c r="E41" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="E7:E20"/>
+    <mergeCell ref="E7:E33"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
@@ -3340,10 +3419,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:E34"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3351,7 +3430,7 @@
     <col min="1" max="1" width="4.625" customWidth="1"/>
     <col min="2" max="2" width="28.625" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="61.125" customWidth="1"/>
+    <col min="4" max="4" width="78.75" customWidth="1"/>
     <col min="5" max="5" width="28.875" customWidth="1"/>
     <col min="6" max="6" width="41.5" customWidth="1"/>
   </cols>
@@ -3361,7 +3440,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -3371,7 +3450,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -3388,7 +3467,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -3410,12 +3489,12 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>37</v>
@@ -3424,7 +3503,7 @@
         <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -3434,26 +3513,28 @@
       <c r="C9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="28" t="s">
+        <v>359</v>
+      </c>
       <c r="E9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="1" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>37</v>
@@ -3474,7 +3555,7 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="11" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>35</v>
@@ -3483,7 +3564,7 @@
         <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="2:6">
@@ -3520,28 +3601,28 @@
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>406</v>
       </c>
       <c r="E17" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="1" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3552,13 +3633,13 @@
         <v>37</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="30"/>
       <c r="B20" s="34" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>37</v>
@@ -3567,7 +3648,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="34" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>37</v>
@@ -3576,7 +3657,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="34" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>37</v>
@@ -3585,7 +3666,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="B23" s="34" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>37</v>
@@ -3594,7 +3675,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="34" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>37</v>
@@ -3603,7 +3684,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="B25" s="34" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>37</v>
@@ -3612,7 +3693,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="B26" s="34" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>37</v>
@@ -3620,7 +3701,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="B27" s="34" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>37</v>
@@ -3629,7 +3710,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="34" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>37</v>
@@ -3638,7 +3719,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="1" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>37</v>
@@ -3647,7 +3728,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="34" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>37</v>
@@ -3656,7 +3737,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="34" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>37</v>
@@ -3665,46 +3746,49 @@
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="34" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E32" s="33"/>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="1:5">
       <c r="B33" s="34" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="E33" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="B34" s="34" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>37</v>
       </c>
+      <c r="D34" s="28" t="s">
+        <v>349</v>
+      </c>
       <c r="E34" s="33"/>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="1:5">
       <c r="B35" s="1" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E35" s="33"/>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="1:5">
       <c r="B36" s="35" t="s">
         <v>74</v>
       </c>
@@ -3713,7 +3797,7 @@
       </c>
       <c r="E36" s="33"/>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="1:5">
       <c r="B37" s="34" t="s">
         <v>139</v>
       </c>
@@ -3723,9 +3807,9 @@
       <c r="D37" s="27"/>
       <c r="E37" s="33"/>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="1:5">
       <c r="B38" s="1" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>37</v>
@@ -3733,132 +3817,171 @@
       <c r="D38" s="27"/>
       <c r="E38" s="33"/>
     </row>
-    <row r="39" spans="2:5">
-      <c r="D39" s="27"/>
-    </row>
-    <row r="40" spans="2:5">
-      <c r="D40" t="s">
+    <row r="39" spans="1:5">
+      <c r="A39" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>405</v>
+      </c>
+      <c r="C39" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="43" customFormat="1">
+      <c r="A40" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>407</v>
+      </c>
+      <c r="C40" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="42" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="43" customFormat="1">
+      <c r="A41" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="63" t="s">
+        <v>393</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="63" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="43" customFormat="1">
+      <c r="A42" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="63" t="s">
+        <v>394</v>
+      </c>
+      <c r="C42" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="63" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="43" customFormat="1">
+      <c r="A43" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="63" t="s">
+        <v>395</v>
+      </c>
+      <c r="C43" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="63" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="43" customFormat="1">
+      <c r="A44" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="63" t="s">
+        <v>408</v>
+      </c>
+      <c r="C44" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="63" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="43" customFormat="1">
+      <c r="A45" s="64"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="D46" s="70" t="s">
+        <v>348</v>
+      </c>
+      <c r="E46" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="D47" s="70" t="s">
+        <v>350</v>
+      </c>
+      <c r="E47" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="D48" s="70" t="s">
+        <v>352</v>
+      </c>
+      <c r="E48" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5">
+      <c r="D49" s="70" t="s">
+        <v>353</v>
+      </c>
+      <c r="E49" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5">
+      <c r="D50" s="70" t="s">
         <v>356</v>
       </c>
-      <c r="E40" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5">
-      <c r="D41" s="28" t="s">
+      <c r="E50" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5">
+      <c r="D51" s="70" t="s">
         <v>357</v>
       </c>
-      <c r="E41" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5">
-      <c r="D42" s="28" t="s">
-        <v>358</v>
-      </c>
-      <c r="E42" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5">
-      <c r="D43" s="28" t="s">
-        <v>359</v>
-      </c>
-      <c r="E43" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5">
-      <c r="D44" s="28" t="s">
-        <v>360</v>
-      </c>
-      <c r="E44" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5">
-      <c r="D45" s="28" t="s">
+    </row>
+    <row r="52" spans="4:5">
+      <c r="D52" s="70" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="46" spans="2:5">
-      <c r="D46" s="28" t="s">
+    <row r="53" spans="4:5">
+      <c r="D53" s="70" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="47" spans="2:5">
-      <c r="D47" s="28" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="48" spans="2:5">
-      <c r="D48" s="28" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="49" spans="4:4">
-      <c r="D49" s="28" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="50" spans="4:4">
-      <c r="D50" s="28" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="51" spans="4:4">
-      <c r="D51" s="28" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="52" spans="4:4">
-      <c r="D52" s="28" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="53" spans="4:4">
-      <c r="D53" s="28" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="54" spans="4:4">
-      <c r="D54" s="28" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="55" spans="4:4">
-      <c r="D55" s="28" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="56" spans="4:4">
-      <c r="D56" s="28" t="s">
-        <v>372</v>
-      </c>
+    <row r="70" spans="4:4">
+      <c r="D70" s="27"/>
+    </row>
+    <row r="71" spans="4:4">
+      <c r="D71" s="27"/>
+    </row>
+    <row r="72" spans="4:4">
+      <c r="D72" s="27"/>
     </row>
     <row r="74" spans="4:4">
-      <c r="D74" s="27"/>
-    </row>
-    <row r="75" spans="4:4">
-      <c r="D75" s="27"/>
+      <c r="D74" s="28"/>
     </row>
     <row r="76" spans="4:4">
       <c r="D76" s="27"/>
     </row>
+    <row r="77" spans="4:4">
+      <c r="D77" s="27"/>
+    </row>
     <row r="78" spans="4:4">
-      <c r="D78" s="28"/>
-    </row>
-    <row r="80" spans="4:4">
-      <c r="D80" s="27"/>
-    </row>
-    <row r="81" spans="4:4">
-      <c r="D81" s="27"/>
-    </row>
-    <row r="82" spans="4:4">
-      <c r="D82" s="27"/>
-    </row>
-    <row r="83" spans="4:4">
-      <c r="D83" s="27"/>
+      <c r="D78" s="27"/>
+    </row>
+    <row r="79" spans="4:4">
+      <c r="D79" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3894,7 +4017,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -3904,7 +4027,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -3919,7 +4042,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -3958,7 +4081,7 @@
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="20" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>38</v>
@@ -3967,7 +4090,7 @@
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>37</v>
@@ -3982,10 +4105,10 @@
         <v>37</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="E11" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -4005,7 +4128,7 @@
         <v>35</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
@@ -4013,7 +4136,7 @@
     </row>
     <row r="14" spans="2:6">
       <c r="B14" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>37</v>
@@ -4023,7 +4146,7 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="21" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>36</v>
@@ -4032,13 +4155,13 @@
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="5" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="E16" s="2"/>
     </row>
@@ -4051,12 +4174,12 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="7" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>37</v>
@@ -4066,21 +4189,21 @@
     </row>
     <row r="19" spans="1:5">
       <c r="B19" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>263</v>
-      </c>
       <c r="E19" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="21" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>37</v>
@@ -4089,27 +4212,27 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="13" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="E21" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="13" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="E22" s="2"/>
     </row>
@@ -4121,13 +4244,13 @@
         <v>36</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="13" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>36</v>
@@ -4137,7 +4260,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="B25" s="16" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>38</v>
@@ -4153,7 +4276,7 @@
         <v>36</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="E26" t="s">
         <v>110</v>
@@ -4162,19 +4285,19 @@
     <row r="27" spans="1:5">
       <c r="A27" s="30"/>
       <c r="B27" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>264</v>
       </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="16" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>38</v>
@@ -4224,7 +4347,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -4234,7 +4357,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -4249,7 +4372,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -4282,7 +4405,7 @@
         <v>35</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="E8" s="39"/>
     </row>
@@ -4298,7 +4421,7 @@
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="20" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>38</v>
@@ -4307,7 +4430,7 @@
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="11" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>35</v>
@@ -4325,7 +4448,7 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="20" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>38</v>
@@ -4340,25 +4463,25 @@
         <v>35</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="E14" s="39"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="11" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>124</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="E15" s="39"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="1" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>36</v>
@@ -4367,7 +4490,7 @@
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="1" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>37</v>
@@ -4376,7 +4499,7 @@
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="1" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>36</v>
@@ -4397,7 +4520,7 @@
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>36</v>
@@ -4406,13 +4529,13 @@
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="27" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="E21" s="39"/>
     </row>
@@ -4427,7 +4550,7 @@
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="34" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>37</v>
@@ -4436,7 +4559,7 @@
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="27" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>37</v>
@@ -4445,7 +4568,7 @@
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="27" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>36</v>
@@ -4454,7 +4577,7 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="34" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>37</v>
@@ -4463,7 +4586,7 @@
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="27" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>36</v>
@@ -4472,13 +4595,13 @@
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="31" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C28" s="32" t="s">
         <v>37</v>
       </c>
       <c r="D28" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="E28" s="39"/>
     </row>
@@ -4490,13 +4613,13 @@
         <v>37</v>
       </c>
       <c r="D29" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="E29" s="39"/>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="41" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>37</v>
@@ -4505,7 +4628,7 @@
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="31" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C31" s="32" t="s">
         <v>37</v>
@@ -4514,19 +4637,19 @@
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="31" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="C32" s="32" t="s">
         <v>36</v>
       </c>
       <c r="D32" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="E32" s="39"/>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" s="41" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>37</v>
@@ -4569,7 +4692,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -4597,7 +4720,7 @@
     <row r="4" spans="2:6">
       <c r="B4" s="47"/>
       <c r="C4" s="36" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="D4" s="36"/>
       <c r="E4" s="36"/>
@@ -4605,7 +4728,7 @@
     <row r="5" spans="2:6">
       <c r="B5" s="47"/>
       <c r="C5" s="36" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="36"/>
@@ -4613,7 +4736,7 @@
     <row r="6" spans="2:6">
       <c r="B6" s="47"/>
       <c r="C6" s="36" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="D6" s="36"/>
       <c r="E6" s="36"/>
@@ -4621,7 +4744,7 @@
     <row r="7" spans="2:6">
       <c r="B7" s="47"/>
       <c r="C7" s="36" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="36"/>
@@ -4629,20 +4752,20 @@
     <row r="8" spans="2:6">
       <c r="B8" s="47"/>
       <c r="C8" s="36" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="D8" s="36"/>
       <c r="E8" s="36"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="58"/>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="46" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="C11" s="46"/>
       <c r="D11" s="46" t="s">
@@ -5003,7 +5126,7 @@
         <v>6</v>
       </c>
       <c r="B40" s="48" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C40" s="52" t="s">
         <v>36</v>
@@ -5409,7 +5532,7 @@
     </row>
     <row r="34" spans="1:3" s="43" customFormat="1">
       <c r="B34" s="61" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="C34" s="52" t="s">
         <v>37</v>
@@ -5417,7 +5540,7 @@
     </row>
     <row r="35" spans="1:3" s="43" customFormat="1">
       <c r="B35" s="56" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="C35" s="57" t="s">
         <v>124</v>
@@ -5449,7 +5572,7 @@
     </row>
     <row r="39" spans="1:3" s="43" customFormat="1">
       <c r="B39" s="61" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="C39" s="52" t="s">
         <v>37</v>
@@ -5828,7 +5951,7 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32" s="66" t="s">
+      <c r="B32" s="68" t="s">
         <v>100</v>
       </c>
       <c r="C32" s="52" t="s">
@@ -6631,7 +6754,7 @@
         <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E15" s="39"/>
     </row>
@@ -6805,7 +6928,7 @@
         <v>36</v>
       </c>
       <c r="D30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E30" s="39"/>
     </row>
@@ -6817,38 +6940,38 @@
         <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E31" s="39"/>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="20" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
     </row>
     <row r="34" spans="4:4">
       <c r="D34" s="20" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
     </row>
     <row r="35" spans="4:4">
       <c r="D35" s="20" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
     </row>
     <row r="36" spans="4:4">
       <c r="D36" s="20" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
     </row>
     <row r="37" spans="4:4">
       <c r="D37" s="20" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
     </row>
     <row r="38" spans="4:4">
       <c r="D38" s="20" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -6886,7 +7009,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -6896,7 +7019,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -6913,11 +7036,11 @@
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="3" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>7</v>
@@ -7077,7 +7200,7 @@
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="13" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>37</v>
@@ -7128,7 +7251,7 @@
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="13" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>37</v>
@@ -7137,7 +7260,7 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="13" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>37</v>
@@ -7146,7 +7269,7 @@
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="13" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>37</v>
@@ -7188,7 +7311,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -7206,7 +7329,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -7216,7 +7339,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -7233,7 +7356,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -7290,7 +7413,7 @@
         <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="2:6">
@@ -7414,7 +7537,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>37</v>
@@ -7423,12 +7546,12 @@
         <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>37</v>
@@ -7454,21 +7577,21 @@
     </row>
     <row r="24" spans="1:5">
       <c r="B24" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="E24" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="B25" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>37</v>
@@ -7478,18 +7601,18 @@
     </row>
     <row r="26" spans="1:5">
       <c r="B26" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="B27" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>37</v>
@@ -7506,12 +7629,12 @@
         <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>37</v>
@@ -7519,18 +7642,18 @@
     </row>
     <row r="30" spans="1:5">
       <c r="B30" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>37</v>
@@ -7538,38 +7661,38 @@
     </row>
     <row r="32" spans="1:5">
       <c r="B32" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" spans="2:5">
       <c r="B33" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="E34" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -7606,7 +7729,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
@@ -7616,7 +7739,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -7631,7 +7754,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
@@ -7660,14 +7783,14 @@
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="1" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>37</v>
       </c>
       <c r="D8" s="39"/>
       <c r="E8" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="2:6">
@@ -7712,7 +7835,7 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>36</v>
@@ -7740,12 +7863,12 @@
       </c>
       <c r="D15" s="39"/>
       <c r="E15" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="21" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>36</v>
@@ -7772,7 +7895,7 @@
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="35" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>35</v>
@@ -7790,7 +7913,7 @@
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="21" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>37</v>
@@ -7806,19 +7929,19 @@
       </c>
       <c r="D22" s="39"/>
       <c r="E22" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="34" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D23" s="39"/>
       <c r="E23" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="2:5">
@@ -7847,7 +7970,7 @@
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="34" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Notes added to Authorisation cancellation
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -2928,8 +2928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3165,33 +3165,33 @@
       </c>
       <c r="E21" s="39"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" s="43" customFormat="1">
       <c r="A22" s="53" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="42" t="s">
-        <v>331</v>
+        <v>404</v>
       </c>
       <c r="C22" s="52" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="E22" s="39"/>
     </row>
-    <row r="23" spans="1:5" s="43" customFormat="1">
+    <row r="23" spans="1:5">
       <c r="A23" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="43" t="s">
-        <v>393</v>
+      <c r="B23" s="42" t="s">
+        <v>331</v>
       </c>
       <c r="C23" s="52" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="43" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E23" s="39"/>
     </row>
@@ -3200,13 +3200,13 @@
         <v>6</v>
       </c>
       <c r="B24" s="43" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C24" s="52" t="s">
         <v>37</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E24" s="39"/>
     </row>
@@ -3215,13 +3215,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C25" s="52" t="s">
         <v>37</v>
       </c>
       <c r="D25" s="43" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E25" s="39"/>
     </row>
@@ -3230,13 +3230,13 @@
         <v>6</v>
       </c>
       <c r="B26" s="43" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C26" s="52" t="s">
         <v>37</v>
       </c>
       <c r="D26" s="43" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E26" s="39"/>
     </row>
@@ -3245,13 +3245,13 @@
         <v>6</v>
       </c>
       <c r="B27" s="43" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C27" s="52" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E27" s="39"/>
     </row>
@@ -3259,14 +3259,14 @@
       <c r="A28" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="42" t="s">
-        <v>404</v>
+      <c r="B28" s="43" t="s">
+        <v>397</v>
       </c>
       <c r="C28" s="52" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E28" s="39"/>
     </row>
@@ -3335,7 +3335,7 @@
         <v>6</v>
       </c>
       <c r="B33" s="62" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="C33" s="52" t="s">
         <v>37</v>
@@ -3421,8 +3421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Update mapping spreadsheet and organization resource
</commit_message>
<xml_diff>
--- a/Docs/PrimaryCareResourceMap.xlsx
+++ b/Docs/PrimaryCareResourceMap.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Source\Endeavour\FHIR-Profiles\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Code\GitHub\FHIR-Profiles\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="6" activeTab="12"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="12375" windowHeight="6630" tabRatio="685" firstSheet="4" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Condition" sheetId="1" r:id="rId1"/>
@@ -27,13 +27,15 @@
     <sheet name="MedicationOrder" sheetId="15" r:id="rId13"/>
     <sheet name="Encounter" sheetId="10" r:id="rId14"/>
     <sheet name="Composition" sheetId="11" r:id="rId15"/>
+    <sheet name="Organization" sheetId="19" r:id="rId16"/>
+    <sheet name="Schedule" sheetId="18" r:id="rId17"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="438">
   <si>
     <t>PrimaryCare-Condition</t>
   </si>
@@ -1260,6 +1262,93 @@
   </si>
   <si>
     <t>prescribedAsContraceptive</t>
+  </si>
+  <si>
+    <t>PrimaryCare-Organization</t>
+  </si>
+  <si>
+    <t>primarycare-date-extension</t>
+  </si>
+  <si>
+    <t>primarycare-location-extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (1st slice) odsCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    system</t>
+  </si>
+  <si>
+    <t>Fixed value: http://endeavourhealth.org/fhir/identifier#odscode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    value</t>
+  </si>
+  <si>
+    <t>organisation.nationalPracticeCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (2nd slice) systemSupplierIdentifier</t>
+  </si>
+  <si>
+    <t>organisation.cdb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    openDate</t>
+  </si>
+  <si>
+    <t>organisation.openDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    closeDate</t>
+  </si>
+  <si>
+    <t>organisation.closeDate</t>
+  </si>
+  <si>
+    <t>organisation.closeDate is null or is &gt; getdate()</t>
+  </si>
+  <si>
+    <t>Example value:  http://emishealth.com/fhir/identifier#cdb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  coding</t>
+  </si>
+  <si>
+    <t>Fixed value:  http://endeavourhealth.org/fhir/ValueSet/primarycare-organization-type</t>
+  </si>
+  <si>
+    <t>organisation.organisationType.code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    display</t>
+  </si>
+  <si>
+    <t>organisation.organisationType.displayName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  text</t>
+  </si>
+  <si>
+    <t>When coded value unavailable</t>
+  </si>
+  <si>
+    <t>organisation.name</t>
+  </si>
+  <si>
+    <t>part of</t>
+  </si>
+  <si>
+    <t>organisation.parentOrganisation</t>
+  </si>
+  <si>
+    <t>mainLocation</t>
+  </si>
+  <si>
+    <t>organisation.mainLocation</t>
   </si>
 </sst>
 </file>
@@ -1456,14 +1545,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1528,6 +1609,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1836,39 +1925,39 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-    </row>
-    <row r="4" spans="2:6" s="43" customFormat="1">
-      <c r="B4" s="47"/>
-      <c r="C4" s="69" t="s">
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+    </row>
+    <row r="4" spans="2:6" s="39" customFormat="1">
+      <c r="B4" s="43"/>
+      <c r="C4" s="65" t="s">
         <v>385</v>
       </c>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
@@ -2170,22 +2259,22 @@
       <c r="A31" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="44" t="s">
         <v>380</v>
       </c>
-      <c r="C31" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="48" t="s">
+      <c r="C31" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="45"/>
+      <c r="E31" s="41"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="52" t="s">
         <v>381</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="48" t="s">
         <v>35</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -2194,13 +2283,13 @@
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="56" t="s">
+      <c r="B33" s="52" t="s">
         <v>382</v>
       </c>
-      <c r="C33" s="52" t="s">
+      <c r="C33" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D33" s="48" t="s">
+      <c r="D33" s="44" t="s">
         <v>383</v>
       </c>
       <c r="E33" s="2"/>
@@ -2241,47 +2330,47 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>208</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>209</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="4"/>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="68" t="s">
         <v>371</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="4"/>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="68" t="s">
         <v>372</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="3" t="s">
@@ -2592,31 +2681,31 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>285</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>200</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="68" t="s">
         <v>373</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
@@ -2641,7 +2730,7 @@
         <v>36</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="70" t="s">
         <v>144</v>
       </c>
     </row>
@@ -2653,7 +2742,7 @@
         <v>37</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="39"/>
+      <c r="E8" s="70"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="1" t="s">
@@ -2665,7 +2754,7 @@
       <c r="D9" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="70"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="21" t="s">
@@ -2675,7 +2764,7 @@
         <v>36</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="39"/>
+      <c r="E10" s="70"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="12" t="s">
@@ -2687,7 +2776,7 @@
       <c r="D11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="70"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="21" t="s">
@@ -2699,7 +2788,7 @@
       <c r="D12" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="70"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="21" t="s">
@@ -2711,7 +2800,7 @@
       <c r="D13" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="E13" s="39"/>
+      <c r="E13" s="70"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="21" t="s">
@@ -2720,7 +2809,7 @@
       <c r="C14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="39"/>
+      <c r="E14" s="70"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="22" t="s">
@@ -2729,7 +2818,7 @@
       <c r="C15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="39"/>
+      <c r="E15" s="70"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="22" t="s">
@@ -2741,7 +2830,7 @@
       <c r="D16" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="E16" s="39"/>
+      <c r="E16" s="70"/>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" s="22" t="s">
@@ -2753,7 +2842,7 @@
       <c r="D17" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="E17" s="39"/>
+      <c r="E17" s="70"/>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" s="22" t="s">
@@ -2765,7 +2854,7 @@
       <c r="D18" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="E18" s="39"/>
+      <c r="E18" s="70"/>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" s="22" t="s">
@@ -2777,7 +2866,7 @@
       <c r="D19" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="E19" s="39"/>
+      <c r="E19" s="70"/>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="22" t="s">
@@ -2789,7 +2878,7 @@
       <c r="D20" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="E20" s="39"/>
+      <c r="E20" s="70"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="10" t="s">
@@ -2804,7 +2893,7 @@
       <c r="D21" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="E21" s="39"/>
+      <c r="E21" s="70"/>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="21" t="s">
@@ -2813,7 +2902,7 @@
       <c r="C22" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="39"/>
+      <c r="E22" s="70"/>
     </row>
     <row r="23" spans="1:5">
       <c r="B23" s="22" t="s">
@@ -2822,7 +2911,7 @@
       <c r="C23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="39"/>
+      <c r="E23" s="70"/>
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="22" t="s">
@@ -2831,7 +2920,7 @@
       <c r="C24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="39"/>
+      <c r="E24" s="70"/>
     </row>
     <row r="25" spans="1:5">
       <c r="B25" s="22" t="s">
@@ -2840,7 +2929,7 @@
       <c r="C25" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="39"/>
+      <c r="E25" s="70"/>
     </row>
     <row r="26" spans="1:5">
       <c r="B26" s="21" t="s">
@@ -2850,7 +2939,7 @@
         <v>36</v>
       </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="39"/>
+      <c r="E26" s="70"/>
     </row>
     <row r="27" spans="1:5">
       <c r="B27" s="22" t="s">
@@ -2859,7 +2948,7 @@
       <c r="C27" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="39"/>
+      <c r="E27" s="70"/>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="22" t="s">
@@ -2868,7 +2957,7 @@
       <c r="C28" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="39"/>
+      <c r="E28" s="70"/>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="22" t="s">
@@ -2877,7 +2966,7 @@
       <c r="C29" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="39"/>
+      <c r="E29" s="70"/>
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="22" t="s">
@@ -2886,7 +2975,7 @@
       <c r="C30" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="39"/>
+      <c r="E30" s="70"/>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="22" t="s">
@@ -2895,7 +2984,7 @@
       <c r="C31" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="39"/>
+      <c r="E31" s="70"/>
     </row>
     <row r="32" spans="1:5">
       <c r="B32" s="22" t="s">
@@ -2904,7 +2993,7 @@
       <c r="C32" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="39"/>
+      <c r="E32" s="70"/>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="1"/>
@@ -2943,467 +3032,467 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>403</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:5">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>154</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="42" t="s">
         <v>403</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46" t="s">
+      <c r="C6" s="42"/>
+      <c r="D6" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="42" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" customHeight="1">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="45"/>
-      <c r="E7" s="39" t="s">
+      <c r="D7" s="41"/>
+      <c r="E7" s="70" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="70"/>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="70"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="C10" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="48" t="s">
+      <c r="C10" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="70"/>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="54" t="s">
+      <c r="B11" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="70"/>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="C12" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="39"/>
+      <c r="C12" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="44"/>
+      <c r="E12" s="70"/>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="70"/>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="C14" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="39"/>
+      <c r="C14" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="39"/>
+      <c r="E14" s="70"/>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="C15" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="48" t="s">
+      <c r="C15" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="44" t="s">
         <v>391</v>
       </c>
-      <c r="E15" s="39"/>
+      <c r="E15" s="70"/>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="43" t="s">
+      <c r="C16" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="39"/>
+      <c r="E16" s="70"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="43"/>
-      <c r="B17" s="43" t="s">
+      <c r="A17" s="39"/>
+      <c r="B17" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="70"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="43"/>
-      <c r="B18" s="54" t="s">
+      <c r="A18" s="39"/>
+      <c r="B18" s="50" t="s">
         <v>161</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="39"/>
+      <c r="E18" s="70"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43" t="s">
+      <c r="A19" s="39"/>
+      <c r="B19" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="C19" s="52" t="s">
+      <c r="C19" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="E19" s="39"/>
+      <c r="E19" s="70"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="C20" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="43" t="s">
+      <c r="C20" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="E20" s="39"/>
+      <c r="E20" s="70"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="53" t="s">
+      <c r="A21" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="38" t="s">
         <v>330</v>
       </c>
-      <c r="C21" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="44" t="s">
+      <c r="C21" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="40" t="s">
         <v>392</v>
       </c>
-      <c r="E21" s="39"/>
-    </row>
-    <row r="22" spans="1:5" s="43" customFormat="1">
-      <c r="A22" s="53" t="s">
+      <c r="E21" s="70"/>
+    </row>
+    <row r="22" spans="1:5" s="39" customFormat="1">
+      <c r="A22" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="38" t="s">
         <v>404</v>
       </c>
-      <c r="C22" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="43" t="s">
+      <c r="C22" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="E22" s="39"/>
+      <c r="E22" s="70"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="53" t="s">
+      <c r="A23" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="38" t="s">
         <v>331</v>
       </c>
-      <c r="C23" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="43" t="s">
+      <c r="C23" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="E23" s="39"/>
-    </row>
-    <row r="24" spans="1:5" s="43" customFormat="1">
-      <c r="A24" s="53" t="s">
+      <c r="E23" s="70"/>
+    </row>
+    <row r="24" spans="1:5" s="39" customFormat="1">
+      <c r="A24" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="39" t="s">
         <v>393</v>
       </c>
-      <c r="C24" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="43" t="s">
+      <c r="C24" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="E24" s="39"/>
-    </row>
-    <row r="25" spans="1:5" s="43" customFormat="1">
-      <c r="A25" s="53" t="s">
+      <c r="E24" s="70"/>
+    </row>
+    <row r="25" spans="1:5" s="39" customFormat="1">
+      <c r="A25" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="39" t="s">
         <v>394</v>
       </c>
-      <c r="C25" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="43" t="s">
+      <c r="C25" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="E25" s="39"/>
-    </row>
-    <row r="26" spans="1:5" s="43" customFormat="1">
-      <c r="A26" s="53" t="s">
+      <c r="E25" s="70"/>
+    </row>
+    <row r="26" spans="1:5" s="39" customFormat="1">
+      <c r="A26" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="39" t="s">
         <v>395</v>
       </c>
-      <c r="C26" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="43" t="s">
+      <c r="C26" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="E26" s="39"/>
-    </row>
-    <row r="27" spans="1:5" s="43" customFormat="1">
-      <c r="A27" s="53" t="s">
+      <c r="E26" s="70"/>
+    </row>
+    <row r="27" spans="1:5" s="39" customFormat="1">
+      <c r="A27" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="39" t="s">
         <v>396</v>
       </c>
-      <c r="C27" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" s="43" t="s">
+      <c r="C27" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="E27" s="39"/>
-    </row>
-    <row r="28" spans="1:5" s="43" customFormat="1">
-      <c r="A28" s="53" t="s">
+      <c r="E27" s="70"/>
+    </row>
+    <row r="28" spans="1:5" s="39" customFormat="1">
+      <c r="A28" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="43" t="s">
+      <c r="B28" s="39" t="s">
         <v>397</v>
       </c>
-      <c r="C28" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D28" s="43" t="s">
+      <c r="C28" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="E28" s="39"/>
+      <c r="E28" s="70"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="63" t="s">
+      <c r="B29" s="59" t="s">
         <v>398</v>
       </c>
-      <c r="C29" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="63" t="s">
+      <c r="C29" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="E29" s="39"/>
-    </row>
-    <row r="30" spans="1:5" s="43" customFormat="1">
-      <c r="A30" s="53" t="s">
+      <c r="E29" s="70"/>
+    </row>
+    <row r="30" spans="1:5" s="39" customFormat="1">
+      <c r="A30" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="43" t="s">
+      <c r="B30" s="39" t="s">
         <v>399</v>
       </c>
-      <c r="C30" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="43" t="s">
+      <c r="C30" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="E30" s="39"/>
-    </row>
-    <row r="31" spans="1:5" s="43" customFormat="1">
-      <c r="A31" s="53" t="s">
+      <c r="E30" s="70"/>
+    </row>
+    <row r="31" spans="1:5" s="39" customFormat="1">
+      <c r="A31" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="52" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="52" t="s">
+      <c r="C31" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="63" t="s">
+      <c r="D31" s="59" t="s">
         <v>400</v>
       </c>
-      <c r="E31" s="39"/>
-    </row>
-    <row r="32" spans="1:5" s="43" customFormat="1">
-      <c r="A32" s="53" t="s">
+      <c r="E31" s="70"/>
+    </row>
+    <row r="32" spans="1:5" s="39" customFormat="1">
+      <c r="A32" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B32" s="66" t="s">
+      <c r="B32" s="62" t="s">
         <v>116</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="63" t="s">
+      <c r="D32" s="59" t="s">
         <v>401</v>
       </c>
-      <c r="E32" s="39"/>
-    </row>
-    <row r="33" spans="1:5" s="43" customFormat="1">
-      <c r="A33" s="53" t="s">
+      <c r="E32" s="70"/>
+    </row>
+    <row r="33" spans="1:5" s="39" customFormat="1">
+      <c r="A33" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="62" t="s">
+      <c r="B33" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="63" t="s">
+      <c r="C33" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="59" t="s">
         <v>402</v>
       </c>
-      <c r="E33" s="39"/>
-    </row>
-    <row r="34" spans="1:5" s="43" customFormat="1">
-      <c r="B34" s="63"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="65"/>
+      <c r="E33" s="70"/>
+    </row>
+    <row r="34" spans="1:5" s="39" customFormat="1">
+      <c r="B34" s="59"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="61"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="59" t="s">
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="55" t="s">
         <v>164</v>
       </c>
-      <c r="E35" s="65"/>
+      <c r="E35" s="61"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="59" t="s">
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="55" t="s">
         <v>163</v>
       </c>
-      <c r="E36" s="65"/>
+      <c r="E36" s="61"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="B37" s="43"/>
-      <c r="C37" s="43"/>
-      <c r="D37" s="59" t="s">
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="55" t="s">
         <v>168</v>
       </c>
-      <c r="E37" s="65"/>
+      <c r="E37" s="61"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="59" t="s">
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="55" t="s">
         <v>170</v>
       </c>
-      <c r="E38" s="65"/>
+      <c r="E38" s="61"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="59" t="s">
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="55" t="s">
         <v>175</v>
       </c>
-      <c r="E39" s="65"/>
+      <c r="E39" s="61"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="B40" s="43"/>
-      <c r="C40" s="43"/>
-      <c r="D40" s="59" t="s">
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="E40" s="65"/>
+      <c r="E40" s="61"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="D41" s="59" t="s">
+      <c r="D41" s="55" t="s">
         <v>180</v>
       </c>
-      <c r="E41" s="65"/>
+      <c r="E41" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3421,7 +3510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -3439,31 +3528,31 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>314</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>315</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
@@ -3818,94 +3907,94 @@
       <c r="E38" s="33"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="53" t="s">
+      <c r="A39" s="49" t="s">
         <v>6</v>
       </c>
       <c r="B39" t="s">
         <v>405</v>
       </c>
-      <c r="C39" s="52" t="s">
+      <c r="C39" s="48" t="s">
         <v>37</v>
       </c>
       <c r="D39" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="40" spans="1:5" s="43" customFormat="1">
-      <c r="A40" s="53" t="s">
+    <row r="40" spans="1:5" s="39" customFormat="1">
+      <c r="A40" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="38" t="s">
         <v>407</v>
       </c>
-      <c r="C40" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40" s="42" t="s">
+      <c r="C40" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="38" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="41" spans="1:5" s="43" customFormat="1">
-      <c r="A41" s="53" t="s">
+    <row r="41" spans="1:5" s="39" customFormat="1">
+      <c r="A41" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="63" t="s">
+      <c r="B41" s="59" t="s">
         <v>393</v>
       </c>
-      <c r="C41" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41" s="63" t="s">
+      <c r="C41" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D41" s="59" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="43" customFormat="1">
-      <c r="A42" s="53" t="s">
+    <row r="42" spans="1:5" s="39" customFormat="1">
+      <c r="A42" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="63" t="s">
+      <c r="B42" s="59" t="s">
         <v>394</v>
       </c>
-      <c r="C42" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" s="63" t="s">
+      <c r="C42" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" s="59" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="43" customFormat="1">
-      <c r="A43" s="53" t="s">
+    <row r="43" spans="1:5" s="39" customFormat="1">
+      <c r="A43" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B43" s="63" t="s">
+      <c r="B43" s="59" t="s">
         <v>395</v>
       </c>
-      <c r="C43" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" s="63" t="s">
+      <c r="C43" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="59" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="43" customFormat="1">
-      <c r="A44" s="53" t="s">
+    <row r="44" spans="1:5" s="39" customFormat="1">
+      <c r="A44" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="63" t="s">
+      <c r="B44" s="59" t="s">
         <v>408</v>
       </c>
-      <c r="C44" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D44" s="63" t="s">
+      <c r="C44" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="59" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="43" customFormat="1">
-      <c r="A45" s="64"/>
+    <row r="45" spans="1:5" s="39" customFormat="1">
+      <c r="A45" s="60"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="D46" s="70" t="s">
+      <c r="D46" s="66" t="s">
         <v>348</v>
       </c>
       <c r="E46" t="s">
@@ -3913,7 +4002,7 @@
       </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="D47" s="70" t="s">
+      <c r="D47" s="66" t="s">
         <v>350</v>
       </c>
       <c r="E47" t="s">
@@ -3921,7 +4010,7 @@
       </c>
     </row>
     <row r="48" spans="1:5">
-      <c r="D48" s="70" t="s">
+      <c r="D48" s="66" t="s">
         <v>352</v>
       </c>
       <c r="E48" t="s">
@@ -3929,7 +4018,7 @@
       </c>
     </row>
     <row r="49" spans="4:5">
-      <c r="D49" s="70" t="s">
+      <c r="D49" s="66" t="s">
         <v>353</v>
       </c>
       <c r="E49" t="s">
@@ -3937,7 +4026,7 @@
       </c>
     </row>
     <row r="50" spans="4:5">
-      <c r="D50" s="70" t="s">
+      <c r="D50" s="66" t="s">
         <v>356</v>
       </c>
       <c r="E50" t="s">
@@ -3945,17 +4034,17 @@
       </c>
     </row>
     <row r="51" spans="4:5">
-      <c r="D51" s="70" t="s">
+      <c r="D51" s="66" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="52" spans="4:5">
-      <c r="D52" s="70" t="s">
+      <c r="D52" s="66" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="53" spans="4:5">
-      <c r="D53" s="70" t="s">
+      <c r="D53" s="66" t="s">
         <v>362</v>
       </c>
     </row>
@@ -3999,7 +4088,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E1"/>
+      <selection sqref="A1:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4016,29 +4105,29 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>233</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>234</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
@@ -4346,29 +4435,29 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>374</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>260</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
@@ -4393,7 +4482,7 @@
         <v>36</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="70" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4407,7 +4496,7 @@
       <c r="D8" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="70"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="11" t="s">
@@ -4417,7 +4506,7 @@
         <v>35</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="39"/>
+      <c r="E9" s="70"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="20" t="s">
@@ -4426,7 +4515,7 @@
       <c r="C10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="70"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="11" t="s">
@@ -4435,7 +4524,7 @@
       <c r="C11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="70"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="11" t="s">
@@ -4444,7 +4533,7 @@
       <c r="C12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="70"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="20" t="s">
@@ -4453,7 +4542,7 @@
       <c r="C13" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="39"/>
+      <c r="E13" s="70"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="11" t="s">
@@ -4465,7 +4554,7 @@
       <c r="D14" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="E14" s="39"/>
+      <c r="E14" s="70"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="11" t="s">
@@ -4477,7 +4566,7 @@
       <c r="D15" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="E15" s="39"/>
+      <c r="E15" s="70"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="1" t="s">
@@ -4486,7 +4575,7 @@
       <c r="C16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="39"/>
+      <c r="E16" s="70"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="1" t="s">
@@ -4495,7 +4584,7 @@
       <c r="C17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="39"/>
+      <c r="E17" s="70"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="1" t="s">
@@ -4504,7 +4593,7 @@
       <c r="C18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="39"/>
+      <c r="E18" s="70"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="1" t="s">
@@ -4516,7 +4605,7 @@
       <c r="D19" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="39"/>
+      <c r="E19" s="70"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" t="s">
@@ -4525,7 +4614,7 @@
       <c r="C20" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E20" s="39"/>
+      <c r="E20" s="70"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="27" t="s">
@@ -4537,7 +4626,7 @@
       <c r="D21" t="s">
         <v>273</v>
       </c>
-      <c r="E21" s="39"/>
+      <c r="E21" s="70"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="27" t="s">
@@ -4546,7 +4635,7 @@
       <c r="C22" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="39"/>
+      <c r="E22" s="70"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="34" t="s">
@@ -4555,7 +4644,7 @@
       <c r="C23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="39"/>
+      <c r="E23" s="70"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="27" t="s">
@@ -4564,7 +4653,7 @@
       <c r="C24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="39"/>
+      <c r="E24" s="70"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="27" t="s">
@@ -4573,7 +4662,7 @@
       <c r="C25" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="39"/>
+      <c r="E25" s="70"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="34" t="s">
@@ -4582,7 +4671,7 @@
       <c r="C26" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="39"/>
+      <c r="E26" s="70"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="27" t="s">
@@ -4591,7 +4680,7 @@
       <c r="C27" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="39"/>
+      <c r="E27" s="70"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="31" t="s">
@@ -4603,7 +4692,7 @@
       <c r="D28" t="s">
         <v>274</v>
       </c>
-      <c r="E28" s="39"/>
+      <c r="E28" s="70"/>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="31" t="s">
@@ -4615,16 +4704,16 @@
       <c r="D29" t="s">
         <v>275</v>
       </c>
-      <c r="E29" s="39"/>
+      <c r="E29" s="70"/>
     </row>
     <row r="30" spans="2:5">
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="37" t="s">
         <v>268</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E30" s="39"/>
+      <c r="E30" s="70"/>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="31" t="s">
@@ -4633,7 +4722,7 @@
       <c r="C31" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="39"/>
+      <c r="E31" s="70"/>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="31" t="s">
@@ -4645,16 +4734,16 @@
       <c r="D32" t="s">
         <v>276</v>
       </c>
-      <c r="E32" s="39"/>
+      <c r="E32" s="70"/>
     </row>
     <row r="33" spans="2:5">
-      <c r="B33" s="41" t="s">
+      <c r="B33" s="37" t="s">
         <v>271</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="39"/>
+      <c r="E33" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4665,6 +4754,408 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="2" max="2" width="33.875" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="43" customWidth="1"/>
+    <col min="5" max="5" width="77" customWidth="1"/>
+    <col min="6" max="6" width="22.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="39"/>
+      <c r="B1" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>409</v>
+      </c>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="39"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="39"/>
+      <c r="B2" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="67" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="39"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="39"/>
+      <c r="B3" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>410</v>
+      </c>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="39"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="39"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="68" t="s">
+        <v>411</v>
+      </c>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="39"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="39"/>
+      <c r="B6" s="42" t="s">
+        <v>409</v>
+      </c>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="39"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="39"/>
+      <c r="B7" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="48"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="39"/>
+      <c r="B8" s="40" t="s">
+        <v>412</v>
+      </c>
+      <c r="C8" s="48"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="39"/>
+      <c r="B9" s="40" t="s">
+        <v>413</v>
+      </c>
+      <c r="C9" s="48"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="39" t="s">
+        <v>414</v>
+      </c>
+      <c r="F9" s="39"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="39"/>
+      <c r="B10" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="C10" s="48"/>
+      <c r="D10" s="41" t="s">
+        <v>416</v>
+      </c>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="39"/>
+      <c r="B11" s="56" t="s">
+        <v>417</v>
+      </c>
+      <c r="C11" s="48"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="39"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="39"/>
+      <c r="B12" s="40" t="s">
+        <v>413</v>
+      </c>
+      <c r="C12" s="48"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="41" t="s">
+        <v>425</v>
+      </c>
+      <c r="F12" s="39"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="39"/>
+      <c r="B13" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="C13" s="48"/>
+      <c r="D13" s="39" t="s">
+        <v>418</v>
+      </c>
+      <c r="E13" s="41"/>
+      <c r="F13" s="39"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="39"/>
+      <c r="B14" s="56" t="s">
+        <v>419</v>
+      </c>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39" t="s">
+        <v>424</v>
+      </c>
+      <c r="E14" s="41"/>
+      <c r="F14" s="39"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="56" t="s">
+        <v>420</v>
+      </c>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39" t="s">
+        <v>421</v>
+      </c>
+      <c r="E15" s="41"/>
+      <c r="F15" s="39"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="56" t="s">
+        <v>422</v>
+      </c>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39" t="s">
+        <v>423</v>
+      </c>
+      <c r="E16" s="41"/>
+      <c r="F16" s="39"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="B17" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="48"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="39"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="39"/>
+      <c r="B18" s="56" t="s">
+        <v>426</v>
+      </c>
+      <c r="C18" s="48"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="39"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="39"/>
+      <c r="B19" s="56" t="s">
+        <v>413</v>
+      </c>
+      <c r="C19" s="48"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="39" t="s">
+        <v>427</v>
+      </c>
+      <c r="F19" s="39"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="39"/>
+      <c r="B20" s="56" t="s">
+        <v>415</v>
+      </c>
+      <c r="C20" s="48"/>
+      <c r="D20" s="41" t="s">
+        <v>428</v>
+      </c>
+      <c r="E20" s="41"/>
+      <c r="F20" s="39"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="39"/>
+      <c r="B21" s="56" t="s">
+        <v>429</v>
+      </c>
+      <c r="C21" s="48"/>
+      <c r="D21" s="44" t="s">
+        <v>430</v>
+      </c>
+      <c r="E21" s="39"/>
+      <c r="F21" s="39"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="39"/>
+      <c r="B22" s="56" t="s">
+        <v>431</v>
+      </c>
+      <c r="C22" s="48"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="41" t="s">
+        <v>432</v>
+      </c>
+      <c r="F22" s="39"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="39"/>
+      <c r="B23" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="48"/>
+      <c r="D23" s="41" t="s">
+        <v>433</v>
+      </c>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="39"/>
+      <c r="B24" s="56" t="s">
+        <v>434</v>
+      </c>
+      <c r="C24" s="48"/>
+      <c r="D24" s="44" t="s">
+        <v>435</v>
+      </c>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="56" t="s">
+        <v>436</v>
+      </c>
+      <c r="C25" s="48"/>
+      <c r="D25" s="44" t="s">
+        <v>437</v>
+      </c>
+      <c r="E25" s="41"/>
+      <c r="F25" s="39"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="39"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="39"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="39"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="39"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="39"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="39"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="39"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="39"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="48"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="39"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4678,388 +5169,388 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="4.625" style="43" customWidth="1"/>
-    <col min="2" max="2" width="28.625" style="43" customWidth="1"/>
-    <col min="3" max="3" width="5" style="43" customWidth="1"/>
-    <col min="4" max="4" width="35.375" style="43" customWidth="1"/>
-    <col min="5" max="5" width="33.875" style="43" customWidth="1"/>
-    <col min="6" max="6" width="41.5" style="43" customWidth="1"/>
-    <col min="7" max="16384" width="11" style="43"/>
+    <col min="1" max="1" width="4.625" style="39" customWidth="1"/>
+    <col min="2" max="2" width="28.625" style="39" customWidth="1"/>
+    <col min="3" max="3" width="5" style="39" customWidth="1"/>
+    <col min="4" max="4" width="35.375" style="39" customWidth="1"/>
+    <col min="5" max="5" width="33.875" style="39" customWidth="1"/>
+    <col min="6" max="6" width="41.5" style="39" customWidth="1"/>
+    <col min="7" max="16384" width="11" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>379</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:6">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="47"/>
-      <c r="C4" s="36" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="68" t="s">
         <v>386</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="47"/>
-      <c r="C5" s="36" t="s">
+      <c r="B5" s="43"/>
+      <c r="C5" s="68" t="s">
         <v>387</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="47"/>
-      <c r="C6" s="36" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="68" t="s">
         <v>388</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="47"/>
-      <c r="C7" s="36" t="s">
+      <c r="B7" s="43"/>
+      <c r="C7" s="68" t="s">
         <v>389</v>
       </c>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="47"/>
-      <c r="C8" s="36" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="68" t="s">
         <v>390</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="58"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="42" t="s">
         <v>379</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46" t="s">
+      <c r="C11" s="42"/>
+      <c r="D11" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="46" t="s">
+      <c r="E11" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="46" t="s">
+      <c r="F11" s="42" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="43" t="s">
+      <c r="D12" s="41"/>
+      <c r="E12" s="39" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="39" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
+      <c r="C14" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="39" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="45" t="s">
+      <c r="C16" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="45"/>
+      <c r="E16" s="41"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="39" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="45"/>
+      <c r="E18" s="41"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="B19" s="51" t="s">
+      <c r="B19" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="48" t="s">
+      <c r="C19" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="45"/>
+      <c r="E19" s="41"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="B20" s="51" t="s">
+      <c r="B20" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
+      <c r="C20" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="B21" s="51" t="s">
+      <c r="B21" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="48" t="s">
+      <c r="C21" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="45"/>
+      <c r="E21" s="41"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="48" t="s">
+      <c r="C22" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="45"/>
+      <c r="E22" s="41"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
+      <c r="C23" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="52" t="s">
+      <c r="C24" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="48" t="s">
+      <c r="D24" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="E24" s="45"/>
+      <c r="E24" s="41"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="48" t="s">
+      <c r="C25" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="E25" s="45"/>
+      <c r="E25" s="41"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="B26" s="48" t="s">
+      <c r="B26" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C26" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D26" s="45"/>
-      <c r="E26" s="43" t="s">
+      <c r="C26" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="41"/>
+      <c r="E26" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="52" t="s">
+      <c r="C27" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="48" t="s">
+      <c r="D27" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E27" s="39" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="52" t="s">
+      <c r="C28" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
+      <c r="C29" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="B30" s="48" t="s">
+      <c r="B30" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="45" t="s">
+      <c r="C30" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="45"/>
+      <c r="E30" s="41"/>
     </row>
     <row r="31" spans="1:5">
-      <c r="B31" s="48" t="s">
+      <c r="B31" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="45" t="s">
+      <c r="C31" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="45"/>
+      <c r="E31" s="41"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32" s="49" t="s">
+      <c r="B32" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="52" t="s">
+      <c r="C33" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
+      <c r="C34" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="B35" s="48" t="s">
+      <c r="B35" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="45" t="s">
+      <c r="C35" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="43" t="s">
+      <c r="E35" s="39" t="s">
         <v>27</v>
       </c>
     </row>
@@ -5067,91 +5558,91 @@
       <c r="A36" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="55" t="s">
+      <c r="B36" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="52" t="s">
+      <c r="C36" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="45" t="s">
+      <c r="D36" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="45"/>
+      <c r="E36" s="41"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="48" t="s">
+      <c r="B37" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="45" t="s">
+      <c r="C37" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="45"/>
+      <c r="E37" s="41"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="52" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
+      <c r="C38" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="48" t="s">
+      <c r="B39" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="52" t="s">
+      <c r="C39" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="45" t="s">
+      <c r="D39" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="45"/>
+      <c r="E39" s="41"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="48" t="s">
+      <c r="B40" s="44" t="s">
         <v>194</v>
       </c>
-      <c r="C40" s="52" t="s">
+      <c r="C40" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="D40" s="60" t="s">
+      <c r="D40" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="45"/>
+      <c r="E40" s="41"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="C41" s="45"/>
-      <c r="E41" s="45"/>
+      <c r="C41" s="41"/>
+      <c r="E41" s="41"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="C42" s="45"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="41"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="C43" s="45"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
+      <c r="C43" s="41"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="41"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="D44" s="45"/>
+      <c r="D44" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5191,39 +5682,39 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="4"/>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="3" t="s">
@@ -5515,74 +6006,74 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="36" t="s">
         <v>79</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="43" customFormat="1">
-      <c r="B33" s="61" t="s">
+    <row r="33" spans="1:3" s="39" customFormat="1">
+      <c r="B33" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="43" customFormat="1">
-      <c r="B34" s="61" t="s">
+      <c r="C33" s="48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="39" customFormat="1">
+      <c r="B34" s="57" t="s">
         <v>375</v>
       </c>
-      <c r="C34" s="52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" s="43" customFormat="1">
-      <c r="B35" s="56" t="s">
+      <c r="C34" s="48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="39" customFormat="1">
+      <c r="B35" s="52" t="s">
         <v>376</v>
       </c>
-      <c r="C35" s="57" t="s">
+      <c r="C35" s="53" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="43" customFormat="1">
-      <c r="B36" s="61" t="s">
+    <row r="36" spans="1:3" s="39" customFormat="1">
+      <c r="B36" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="C36" s="52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" s="43" customFormat="1">
-      <c r="B37" s="61" t="s">
+      <c r="C36" s="48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="39" customFormat="1">
+      <c r="B37" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="43" customFormat="1">
-      <c r="B38" s="61" t="s">
+      <c r="C37" s="48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="39" customFormat="1">
+      <c r="B38" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="43" customFormat="1">
-      <c r="B39" s="61" t="s">
+      <c r="C38" s="48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="39" customFormat="1">
+      <c r="B39" s="57" t="s">
         <v>377</v>
       </c>
-      <c r="C39" s="52" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" s="43" customFormat="1">
-      <c r="B40" s="61" t="s">
+      <c r="C39" s="48" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" s="39" customFormat="1">
+      <c r="B40" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="52" t="s">
+      <c r="C40" s="48" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5631,39 +6122,39 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="4"/>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="3" t="s">
@@ -5951,10 +6442,10 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="48" t="s">
         <v>36</v>
       </c>
     </row>
@@ -6084,55 +6575,55 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="4"/>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="68" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="4"/>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="4"/>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="68" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="3" t="s">
@@ -6157,7 +6648,7 @@
         <v>36</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="69" t="s">
         <v>144</v>
       </c>
     </row>
@@ -6171,7 +6662,7 @@
       <c r="D11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="69"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="5" t="s">
@@ -6183,7 +6674,7 @@
       <c r="D12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="38"/>
+      <c r="E12" s="69"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="12" t="s">
@@ -6193,7 +6684,7 @@
         <v>35</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="38"/>
+      <c r="E13" s="69"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="5" t="s">
@@ -6203,7 +6694,7 @@
         <v>37</v>
       </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="38"/>
+      <c r="E14" s="69"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="12" t="s">
@@ -6215,7 +6706,7 @@
       <c r="D15" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="E15" s="38"/>
+      <c r="E15" s="69"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="7" t="s">
@@ -6225,7 +6716,7 @@
         <v>36</v>
       </c>
       <c r="D16" s="5"/>
-      <c r="E16" s="38"/>
+      <c r="E16" s="69"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="8" t="s">
@@ -6237,7 +6728,7 @@
       <c r="D17" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="69"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="8" t="s">
@@ -6247,7 +6738,7 @@
         <v>37</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="38"/>
+      <c r="E18" s="69"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="8" t="s">
@@ -6259,7 +6750,7 @@
       <c r="D19" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="38"/>
+      <c r="E19" s="69"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="8" t="s">
@@ -6271,7 +6762,7 @@
       <c r="D20" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E20" s="38"/>
+      <c r="E20" s="69"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="8" t="s">
@@ -6281,7 +6772,7 @@
         <v>37</v>
       </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="38"/>
+      <c r="E21" s="69"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="7" t="s">
@@ -6291,7 +6782,7 @@
         <v>37</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="38"/>
+      <c r="E22" s="69"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="5" t="s">
@@ -6301,7 +6792,7 @@
         <v>37</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="38"/>
+      <c r="E23" s="69"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="21" t="s">
@@ -6311,7 +6802,7 @@
         <v>37</v>
       </c>
       <c r="D24" s="5"/>
-      <c r="E24" s="38"/>
+      <c r="E24" s="69"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="21" t="s">
@@ -6321,7 +6812,7 @@
         <v>37</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="38"/>
+      <c r="E25" s="69"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="5" t="s">
@@ -6331,7 +6822,7 @@
         <v>37</v>
       </c>
       <c r="D26" s="2"/>
-      <c r="E26" s="38"/>
+      <c r="E26" s="69"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="13" t="s">
@@ -6340,7 +6831,7 @@
       <c r="C27" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="38"/>
+      <c r="E27" s="69"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="15" t="s">
@@ -6349,7 +6840,7 @@
       <c r="C28" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E28" s="38"/>
+      <c r="E28" s="69"/>
     </row>
     <row r="29" spans="2:5">
       <c r="B29" s="15" t="s">
@@ -6358,7 +6849,7 @@
       <c r="C29" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="38"/>
+      <c r="E29" s="69"/>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" s="14" t="s">
@@ -6368,7 +6859,7 @@
         <v>35</v>
       </c>
       <c r="D30" s="2"/>
-      <c r="E30" s="38"/>
+      <c r="E30" s="69"/>
     </row>
     <row r="31" spans="2:5">
       <c r="B31" s="12" t="s">
@@ -6380,7 +6871,7 @@
       <c r="D31" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="38"/>
+      <c r="E31" s="69"/>
     </row>
     <row r="32" spans="2:5">
       <c r="B32" s="22" t="s">
@@ -6390,7 +6881,7 @@
         <v>35</v>
       </c>
       <c r="D32" s="5"/>
-      <c r="E32" s="38"/>
+      <c r="E32" s="69"/>
     </row>
     <row r="33" spans="1:5">
       <c r="B33" s="8" t="s">
@@ -6402,7 +6893,7 @@
       <c r="D33" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="38"/>
+      <c r="E33" s="69"/>
     </row>
     <row r="34" spans="1:5">
       <c r="B34" s="23" t="s">
@@ -6414,7 +6905,7 @@
       <c r="D34" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="38"/>
+      <c r="E34" s="69"/>
     </row>
     <row r="35" spans="1:5">
       <c r="B35" s="23" t="s">
@@ -6424,7 +6915,7 @@
         <v>37</v>
       </c>
       <c r="D35" s="2"/>
-      <c r="E35" s="38"/>
+      <c r="E35" s="69"/>
     </row>
     <row r="36" spans="1:5">
       <c r="B36" s="23" t="s">
@@ -6436,7 +6927,7 @@
       <c r="D36" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="38"/>
+      <c r="E36" s="69"/>
     </row>
     <row r="37" spans="1:5">
       <c r="B37" s="23" t="s">
@@ -6448,7 +6939,7 @@
       <c r="D37" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E37" s="38"/>
+      <c r="E37" s="69"/>
     </row>
     <row r="38" spans="1:5">
       <c r="B38" s="23" t="s">
@@ -6458,7 +6949,7 @@
         <v>37</v>
       </c>
       <c r="D38" s="2"/>
-      <c r="E38" s="38"/>
+      <c r="E38" s="69"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="10" t="s">
@@ -6473,7 +6964,7 @@
       <c r="D39" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="38"/>
+      <c r="E39" s="69"/>
     </row>
     <row r="40" spans="1:5">
       <c r="B40" s="8" t="s">
@@ -6485,7 +6976,7 @@
       <c r="D40" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="38"/>
+      <c r="E40" s="69"/>
     </row>
     <row r="41" spans="1:5">
       <c r="B41" s="7" t="s">
@@ -6495,7 +6986,7 @@
         <v>37</v>
       </c>
       <c r="D41" s="5"/>
-      <c r="E41" s="38"/>
+      <c r="E41" s="69"/>
     </row>
     <row r="42" spans="1:5">
       <c r="B42" s="7" t="s">
@@ -6505,7 +6996,7 @@
         <v>37</v>
       </c>
       <c r="D42" s="5"/>
-      <c r="E42" s="38"/>
+      <c r="E42" s="69"/>
     </row>
     <row r="43" spans="1:5">
       <c r="B43" s="7" t="s">
@@ -6514,7 +7005,7 @@
       <c r="C43" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E43" s="38"/>
+      <c r="E43" s="69"/>
     </row>
     <row r="44" spans="1:5">
       <c r="B44" s="24" t="s">
@@ -6523,7 +7014,7 @@
       <c r="C44" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E44" s="38"/>
+      <c r="E44" s="69"/>
     </row>
     <row r="45" spans="1:5">
       <c r="B45" s="24" t="s">
@@ -6532,7 +7023,7 @@
       <c r="C45" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E45" s="38"/>
+      <c r="E45" s="69"/>
     </row>
     <row r="46" spans="1:5">
       <c r="B46" s="25" t="s">
@@ -6544,7 +7035,7 @@
       <c r="D46" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E46" s="38"/>
+      <c r="E46" s="69"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="10" t="s">
@@ -6559,7 +7050,7 @@
       <c r="D47" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E47" s="38"/>
+      <c r="E47" s="69"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="10" t="s">
@@ -6571,7 +7062,7 @@
       <c r="C48" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E48" s="38"/>
+      <c r="E48" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -6610,31 +7101,31 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>132</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
@@ -6659,7 +7150,7 @@
         <v>35</v>
       </c>
       <c r="D7" s="26"/>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="70" t="s">
         <v>144</v>
       </c>
       <c r="F7" s="26"/>
@@ -6672,7 +7163,7 @@
         <v>36</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="39"/>
+      <c r="E8" s="70"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="27" t="s">
@@ -6684,7 +7175,7 @@
       <c r="D9" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="70"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="28" t="s">
@@ -6696,7 +7187,7 @@
       <c r="D10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="70"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="28" t="s">
@@ -6708,7 +7199,7 @@
       <c r="D11" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="70"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="28" t="s">
@@ -6720,7 +7211,7 @@
       <c r="D12" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="70"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="28" t="s">
@@ -6732,7 +7223,7 @@
       <c r="D13" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E13" s="39"/>
+      <c r="E13" s="70"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="11" t="s">
@@ -6744,7 +7235,7 @@
       <c r="D14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="39"/>
+      <c r="E14" s="70"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="11" t="s">
@@ -6756,7 +7247,7 @@
       <c r="D15" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E15" s="39"/>
+      <c r="E15" s="70"/>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="11" t="s">
@@ -6768,7 +7259,7 @@
       <c r="D16" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E16" s="39"/>
+      <c r="E16" s="70"/>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" t="s">
@@ -6778,7 +7269,7 @@
         <v>37</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="39"/>
+      <c r="E17" s="70"/>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
@@ -6790,7 +7281,7 @@
       <c r="D18" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="39"/>
+      <c r="E18" s="70"/>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" t="s">
@@ -6802,7 +7293,7 @@
       <c r="D19" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="39"/>
+      <c r="E19" s="70"/>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" s="7" t="s">
@@ -6814,7 +7305,7 @@
       <c r="D20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="39"/>
+      <c r="E20" s="70"/>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="8" t="s">
@@ -6826,7 +7317,7 @@
       <c r="D21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="39"/>
+      <c r="E21" s="70"/>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" s="8" t="s">
@@ -6836,7 +7327,7 @@
         <v>37</v>
       </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="39"/>
+      <c r="E22" s="70"/>
     </row>
     <row r="23" spans="1:5">
       <c r="B23" s="8" t="s">
@@ -6848,7 +7339,7 @@
       <c r="D23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="39"/>
+      <c r="E23" s="70"/>
     </row>
     <row r="24" spans="1:5">
       <c r="B24" s="8" t="s">
@@ -6860,7 +7351,7 @@
       <c r="D24" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="39"/>
+      <c r="E24" s="70"/>
     </row>
     <row r="25" spans="1:5">
       <c r="B25" s="8" t="s">
@@ -6870,7 +7361,7 @@
         <v>37</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="39"/>
+      <c r="E25" s="70"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="10" t="s">
@@ -6885,7 +7376,7 @@
       <c r="D26" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="39"/>
+      <c r="E26" s="70"/>
     </row>
     <row r="27" spans="1:5">
       <c r="B27" s="7" t="s">
@@ -6897,7 +7388,7 @@
       <c r="D27" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="39"/>
+      <c r="E27" s="70"/>
     </row>
     <row r="28" spans="1:5">
       <c r="B28" s="13" t="s">
@@ -6909,7 +7400,7 @@
       <c r="D28" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E28" s="39"/>
+      <c r="E28" s="70"/>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" s="13" t="s">
@@ -6918,7 +7409,7 @@
       <c r="C29" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="39"/>
+      <c r="E29" s="70"/>
     </row>
     <row r="30" spans="1:5">
       <c r="B30" s="13" t="s">
@@ -6930,7 +7421,7 @@
       <c r="D30" t="s">
         <v>153</v>
       </c>
-      <c r="E30" s="39"/>
+      <c r="E30" s="70"/>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="13" t="s">
@@ -6942,7 +7433,7 @@
       <c r="D31" t="s">
         <v>152</v>
       </c>
-      <c r="E31" s="39"/>
+      <c r="E31" s="70"/>
     </row>
     <row r="33" spans="4:4">
       <c r="D33" s="20" t="s">
@@ -7008,31 +7499,31 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>309</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="1:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>310</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="3" t="s">
@@ -7057,7 +7548,7 @@
         <v>36</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="70" t="s">
         <v>144</v>
       </c>
     </row>
@@ -7071,7 +7562,7 @@
       <c r="D8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="70"/>
     </row>
     <row r="9" spans="1:6">
       <c r="B9" s="11" t="s">
@@ -7083,7 +7574,7 @@
       <c r="D9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="70"/>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" s="7" t="s">
@@ -7095,7 +7586,7 @@
       <c r="D10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="70"/>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" s="8" t="s">
@@ -7107,7 +7598,7 @@
       <c r="D11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="70"/>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" s="8" t="s">
@@ -7117,7 +7608,7 @@
         <v>37</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="39"/>
+      <c r="E12" s="70"/>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" s="8" t="s">
@@ -7129,7 +7620,7 @@
       <c r="D13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="39"/>
+      <c r="E13" s="70"/>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" s="8" t="s">
@@ -7141,7 +7632,7 @@
       <c r="D14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="39"/>
+      <c r="E14" s="70"/>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="8" t="s">
@@ -7151,7 +7642,7 @@
         <v>37</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="39"/>
+      <c r="E15" s="70"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="10" t="s">
@@ -7166,7 +7657,7 @@
       <c r="D16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="39"/>
+      <c r="E16" s="70"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="7" t="s">
@@ -7178,7 +7669,7 @@
       <c r="D17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="39"/>
+      <c r="E17" s="70"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="13" t="s">
@@ -7187,7 +7678,7 @@
       <c r="C18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="39"/>
+      <c r="E18" s="70"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="13" t="s">
@@ -7196,7 +7687,7 @@
       <c r="C19" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="39"/>
+      <c r="E19" s="70"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="13" t="s">
@@ -7208,7 +7699,7 @@
       <c r="D20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="39"/>
+      <c r="E20" s="70"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="13" t="s">
@@ -7217,7 +7708,7 @@
       <c r="C21" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="39"/>
+      <c r="E21" s="70"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="13" t="s">
@@ -7226,7 +7717,7 @@
       <c r="C22" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="39"/>
+      <c r="E22" s="70"/>
     </row>
     <row r="23" spans="2:5">
       <c r="B23" s="13" t="s">
@@ -7235,7 +7726,7 @@
       <c r="C23" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="39"/>
+      <c r="E23" s="70"/>
     </row>
     <row r="24" spans="2:5">
       <c r="B24" s="13" t="s">
@@ -7247,7 +7738,7 @@
       <c r="D24" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="39"/>
+      <c r="E24" s="70"/>
     </row>
     <row r="25" spans="2:5">
       <c r="B25" s="13" t="s">
@@ -7256,7 +7747,7 @@
       <c r="C25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="39"/>
+      <c r="E25" s="70"/>
     </row>
     <row r="26" spans="2:5">
       <c r="B26" s="13" t="s">
@@ -7265,7 +7756,7 @@
       <c r="C26" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="39"/>
+      <c r="E26" s="70"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="13" t="s">
@@ -7274,7 +7765,7 @@
       <c r="C27" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="39"/>
+      <c r="E27" s="70"/>
     </row>
     <row r="28" spans="2:5">
       <c r="B28" s="13" t="s">
@@ -7283,7 +7774,7 @@
       <c r="C28" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="39"/>
+      <c r="E28" s="70"/>
     </row>
     <row r="29" spans="2:5">
       <c r="E29" s="33"/>
@@ -7311,7 +7802,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection sqref="A1:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -7328,31 +7819,31 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>184</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
@@ -7728,29 +8219,29 @@
       <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="67" t="s">
         <v>277</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
     </row>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="67" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
@@ -7774,7 +8265,7 @@
       <c r="C7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="70" t="s">
         <v>144</v>
       </c>
       <c r="E7" t="s">
@@ -7788,7 +8279,7 @@
       <c r="C8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="39"/>
+      <c r="D8" s="70"/>
       <c r="E8" t="s">
         <v>282</v>
       </c>
@@ -7800,7 +8291,7 @@
       <c r="C9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="39"/>
+      <c r="D9" s="70"/>
       <c r="E9" t="s">
         <v>39</v>
       </c>
@@ -7812,7 +8303,7 @@
       <c r="C10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="70"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="1" t="s">
@@ -7821,7 +8312,7 @@
       <c r="C11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="70"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="1" t="s">
@@ -7830,7 +8321,7 @@
       <c r="C12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" s="70"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="2:6">
@@ -7840,7 +8331,7 @@
       <c r="C13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="39"/>
+      <c r="D13" s="70"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="1" t="s">
@@ -7849,7 +8340,7 @@
       <c r="C14" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="39"/>
+      <c r="D14" s="70"/>
       <c r="E14" t="s">
         <v>44</v>
       </c>
@@ -7861,7 +8352,7 @@
       <c r="C15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="39"/>
+      <c r="D15" s="70"/>
       <c r="E15" t="s">
         <v>283</v>
       </c>
@@ -7873,7 +8364,7 @@
       <c r="C16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="39"/>
+      <c r="D16" s="70"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="14" t="s">
@@ -7882,7 +8373,7 @@
       <c r="C17" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="39"/>
+      <c r="D17" s="70"/>
     </row>
     <row r="18" spans="2:5">
       <c r="B18" s="22" t="s">
@@ -7891,7 +8382,7 @@
       <c r="C18" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="39"/>
+      <c r="D18" s="70"/>
     </row>
     <row r="19" spans="2:5">
       <c r="B19" s="35" t="s">
@@ -7900,7 +8391,7 @@
       <c r="C19" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="39"/>
+      <c r="D19" s="70"/>
     </row>
     <row r="20" spans="2:5">
       <c r="B20" s="34" t="s">
@@ -7909,7 +8400,7 @@
       <c r="C20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="39"/>
+      <c r="D20" s="70"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="21" t="s">
@@ -7918,7 +8409,7 @@
       <c r="C21" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="39"/>
+      <c r="D21" s="70"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="14" t="s">
@@ -7927,7 +8418,7 @@
       <c r="C22" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="39"/>
+      <c r="D22" s="70"/>
       <c r="E22" t="s">
         <v>284</v>
       </c>
@@ -7939,7 +8430,7 @@
       <c r="C23" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="39"/>
+      <c r="D23" s="70"/>
       <c r="E23" t="s">
         <v>200</v>
       </c>
@@ -7951,7 +8442,7 @@
       <c r="C24" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="39"/>
+      <c r="D24" s="70"/>
       <c r="E24" t="s">
         <v>108</v>
       </c>
@@ -7963,7 +8454,7 @@
       <c r="C25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="39"/>
+      <c r="D25" s="70"/>
       <c r="E25" t="s">
         <v>44</v>
       </c>
@@ -7975,7 +8466,7 @@
       <c r="C26" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="39"/>
+      <c r="D26" s="70"/>
     </row>
     <row r="27" spans="2:5">
       <c r="B27" s="1" t="s">
@@ -7984,7 +8475,7 @@
       <c r="C27" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="39"/>
+      <c r="D27" s="70"/>
       <c r="E27" t="s">
         <v>86</v>
       </c>

</xml_diff>